<commit_message>
#undef interface xll bond
</commit_message>
<xml_diff>
--- a/bondxll.xlsx
+++ b/bondxll.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\source\repos\tmcrossx\bondxll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1482E94-3E26-4A23-B06D-801B14C64E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65A8AF9-518F-4E88-A37F-430AA27540E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3240" yWindow="1320" windowWidth="32415" windowHeight="17685" activeTab="1" xr2:uid="{B41655E8-20ED-4B49-A343-A4ADF5D922ED}"/>
   </bookViews>
   <sheets>
     <sheet name="ENUM" sheetId="1" r:id="rId1"/>
-    <sheet name="PWFLAT" sheetId="2" r:id="rId2"/>
+    <sheet name="INSTRUMENT" sheetId="3" r:id="rId2"/>
+    <sheet name="PWFLAT" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="date">ENUM!$E$3</definedName>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>TMX_DAY_COUNT_ENUM</t>
   </si>
@@ -117,6 +118,9 @@
   <si>
     <t>years</t>
   </si>
+  <si>
+    <t>instrument</t>
+  </si>
 </sst>
 </file>
 
@@ -125,9 +129,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;0x&quot;#"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -275,37 +286,42 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -720,307 +736,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.33643114122081186</c:v>
+                  <c:v>3.2461778028678001E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.33643114122081186</c:v>
+                  <c:v>3.2461778028678001E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.33643114122081186</c:v>
+                  <c:v>3.2461778028678001E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.33643114122081186</c:v>
+                  <c:v>3.2461778028678001E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.33643114122081186</c:v>
+                  <c:v>3.2461778028678001E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.33643114122081186</c:v>
+                  <c:v>3.2461778028678001E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.33643114122081186</c:v>
+                  <c:v>3.2461778028678001E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.33643114122081186</c:v>
+                  <c:v>3.2461778028678001E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.33643114122081186</c:v>
+                  <c:v>3.2461778028678001E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.33643114122081186</c:v>
+                  <c:v>3.2461778028678001E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.66519395089168798</c:v>
+                  <c:v>0.9013900471794476</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.66519395089168798</c:v>
+                  <c:v>0.9013900471794476</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.66519395089168798</c:v>
+                  <c:v>0.9013900471794476</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.66519395089168798</c:v>
+                  <c:v>0.9013900471794476</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.66519395089168798</c:v>
+                  <c:v>0.9013900471794476</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.66519395089168798</c:v>
+                  <c:v>0.9013900471794476</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.66519395089168798</c:v>
+                  <c:v>0.9013900471794476</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.66519395089168798</c:v>
+                  <c:v>0.9013900471794476</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.66519395089168798</c:v>
+                  <c:v>0.9013900471794476</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.66519395089168798</c:v>
+                  <c:v>0.9013900471794476</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.19062816323881138</c:v>
+                  <c:v>0.27300148238849498</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.19062816323881138</c:v>
+                  <c:v>0.27300148238849498</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.19062816323881138</c:v>
+                  <c:v>0.27300148238849498</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.19062816323881138</c:v>
+                  <c:v>0.27300148238849498</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.19062816323881138</c:v>
+                  <c:v>0.27300148238849498</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.19062816323881138</c:v>
+                  <c:v>0.27300148238849498</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.19062816323881138</c:v>
+                  <c:v>0.27300148238849498</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.19062816323881138</c:v>
+                  <c:v>0.27300148238849498</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.19062816323881138</c:v>
+                  <c:v>0.27300148238849498</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.19062816323881138</c:v>
+                  <c:v>0.27300148238849498</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.43828870656484975</c:v>
+                  <c:v>0.85065876641893867</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.43828870656484975</c:v>
+                  <c:v>0.85065876641893867</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.43828870656484975</c:v>
+                  <c:v>0.85065876641893867</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.43828870656484975</c:v>
+                  <c:v>0.85065876641893867</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.43828870656484975</c:v>
+                  <c:v>0.85065876641893867</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.43828870656484975</c:v>
+                  <c:v>0.85065876641893867</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.43828870656484975</c:v>
+                  <c:v>0.85065876641893867</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.43828870656484975</c:v>
+                  <c:v>0.85065876641893867</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.43828870656484975</c:v>
+                  <c:v>0.85065876641893867</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.43828870656484975</c:v>
+                  <c:v>0.85065876641893867</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.34888225615158475</c:v>
+                  <c:v>0.50941830878664573</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.34888225615158475</c:v>
+                  <c:v>0.50941830878664573</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.34888225615158475</c:v>
+                  <c:v>0.50941830878664573</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.34888225615158475</c:v>
+                  <c:v>0.50941830878664573</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.34888225615158475</c:v>
+                  <c:v>0.50941830878664573</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.34888225615158475</c:v>
+                  <c:v>0.50941830878664573</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.34888225615158475</c:v>
+                  <c:v>0.50941830878664573</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.34888225615158475</c:v>
+                  <c:v>0.50941830878664573</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.34888225615158475</c:v>
+                  <c:v>0.50941830878664573</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.34888225615158475</c:v>
+                  <c:v>0.50941830878664573</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.32313040685963279</c:v>
+                  <c:v>0.61829312960625149</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.32313040685963279</c:v>
+                  <c:v>0.61829312960625149</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.32313040685963279</c:v>
+                  <c:v>0.61829312960625149</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.32313040685963279</c:v>
+                  <c:v>0.61829312960625149</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.32313040685963279</c:v>
+                  <c:v>0.61829312960625149</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.32313040685963279</c:v>
+                  <c:v>0.61829312960625149</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.32313040685963279</c:v>
+                  <c:v>0.61829312960625149</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.32313040685963279</c:v>
+                  <c:v>0.61829312960625149</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.32313040685963279</c:v>
+                  <c:v>0.61829312960625149</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.32313040685963279</c:v>
+                  <c:v>0.61829312960625149</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.50982090706683314</c:v>
+                  <c:v>0.55649330279809406</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.50982090706683314</c:v>
+                  <c:v>0.55649330279809406</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.50982090706683314</c:v>
+                  <c:v>0.55649330279809406</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.50982090706683314</c:v>
+                  <c:v>0.55649330279809406</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.50982090706683314</c:v>
+                  <c:v>0.55649330279809406</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.50982090706683314</c:v>
+                  <c:v>0.55649330279809406</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.50982090706683314</c:v>
+                  <c:v>0.55649330279809406</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.50982090706683314</c:v>
+                  <c:v>0.55649330279809406</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.50982090706683314</c:v>
+                  <c:v>0.55649330279809406</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.50982090706683314</c:v>
+                  <c:v>0.55649330279809406</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.39874822970447998</c:v>
+                  <c:v>0.35531318939366341</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.39874822970447998</c:v>
+                  <c:v>0.35531318939366341</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.39874822970447998</c:v>
+                  <c:v>0.35531318939366341</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.39874822970447998</c:v>
+                  <c:v>0.35531318939366341</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.39874822970447998</c:v>
+                  <c:v>0.35531318939366341</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.39874822970447998</c:v>
+                  <c:v>0.35531318939366341</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.39874822970447998</c:v>
+                  <c:v>0.35531318939366341</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.39874822970447998</c:v>
+                  <c:v>0.35531318939366341</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.39874822970447998</c:v>
+                  <c:v>0.35531318939366341</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.39874822970447998</c:v>
+                  <c:v>0.35531318939366341</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.88005095914214659</c:v>
+                  <c:v>0.33946532617874281</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.88005095914214659</c:v>
+                  <c:v>0.33946532617874281</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.88005095914214659</c:v>
+                  <c:v>0.33946532617874281</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.88005095914214659</c:v>
+                  <c:v>0.33946532617874281</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.88005095914214659</c:v>
+                  <c:v>0.33946532617874281</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.88005095914214659</c:v>
+                  <c:v>0.33946532617874281</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.88005095914214659</c:v>
+                  <c:v>0.33946532617874281</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.88005095914214659</c:v>
+                  <c:v>0.33946532617874281</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.88005095914214659</c:v>
+                  <c:v>0.33946532617874281</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.88005095914214659</c:v>
+                  <c:v>0.33946532617874281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1377,307 +1393,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557745</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557745</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.75925229970493102</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.75925229970493113</c:v>
+                  <c:v>0.85258063760557756</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.72081401257001121</c:v>
+                  <c:v>0.7780243776440412</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.68878210662424455</c:v>
+                  <c:v>0.71589416100942749</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.66167818620859598</c:v>
+                  <c:v>0.66332243924167766</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.63844625442375424</c:v>
+                  <c:v>0.61826096344074899</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.61831191354355808</c:v>
+                  <c:v>0.57920768441327775</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.60069436527338638</c:v>
+                  <c:v>0.5450360652642402</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.585149469740882</c:v>
+                  <c:v>0.51488463660332473</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.57133178482310032</c:v>
+                  <c:v>0.48808336668251107</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.55896859305455882</c:v>
+                  <c:v>0.46410328306915138</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.5478417204628715</c:v>
+                  <c:v>0.44252120781712778</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.5534299219118628</c:v>
+                  <c:v>0.46437210492961922</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.55851010504730936</c:v>
+                  <c:v>0.48423655685006595</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.5631485331274998</c:v>
+                  <c:v>0.5023736651252565</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.567400425534341</c:v>
+                  <c:v>0.51899934771084777</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.57131216654863481</c:v>
+                  <c:v>0.53429497568959172</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.57492300440798305</c:v>
+                  <c:v>0.5484140169007401</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.57826637279626836</c:v>
+                  <c:v>0.5614872032073589</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.58137092915681909</c:v>
+                  <c:v>0.57362659049207643</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.58426137818215929</c:v>
+                  <c:v>0.58492877865370985</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.58695913060581029</c:v>
+                  <c:v>0.59547748760456776</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.57417426069074584</c:v>
+                  <c:v>0.58507503582340403</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.56218844514537292</c:v>
+                  <c:v>0.5753227372785632</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.55092904266335585</c:v>
+                  <c:v>0.56616148713037928</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.54033195797439859</c:v>
+                  <c:v>0.55753913404973565</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.53034042098195333</c:v>
+                  <c:v>0.54940948685941449</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.52090396937797712</c:v>
+                  <c:v>0.5417314867352222</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.51197759623908079</c:v>
+                  <c:v>0.5344685136447701</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.5035210322127579</c:v>
+                  <c:v>0.52758780229592073</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.49549813813650284</c:v>
+                  <c:v>0.52105994793932009</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.48787638876406059</c:v>
+                  <c:v>0.51485848630054953</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.48666693310066517</c:v>
+                  <c:v>0.52304873703514443</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.48551507056409821</c:v>
+                  <c:v>0.53084897582999668</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.48441678302923191</c:v>
+                  <c:v>0.5382864128204371</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.4833684176550414</c:v>
+                  <c:v>0.54538578449313035</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.48236664629748166</c:v>
+                  <c:v>0.5521696285359261</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.48140843021633745</c:v>
+                  <c:v>0.55865852283773076</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.48049098928758238</c:v>
+                  <c:v>0.56487129397775648</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.47961177506419206</c:v>
+                  <c:v>0.57082519965361445</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.47876844713563416</c:v>
+                  <c:v>0.57653608877127416</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.47795885232421842</c:v>
+                  <c:v>0.58201854232422734</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.47542793867377459</c:v>
+                  <c:v>0.58059500833329436</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.47299436785604021</c:v>
+                  <c:v>0.57922622564970505</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.47065262989935236</c:v>
+                  <c:v>0.57790909514285482</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.46839762297809739</c:v>
+                  <c:v>0.57664074724736947</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.46622461630852446</c:v>
+                  <c:v>0.57541852109353819</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.46412921702000765</c:v>
+                  <c:v>0.57423994587377214</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.46210734051354407</c:v>
+                  <c:v>0.57310272417048924</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.46015518388661369</c:v>
+                  <c:v>0.57200471700869882</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.45826920206059635</c:v>
+                  <c:v>0.57094393042866409</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.4564460862954462</c:v>
+                  <c:v>0.56991850340129713</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.45426058335387542</c:v>
+                  <c:v>0.57071153006039466</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.45214558050719411</c:v>
+                  <c:v>0.57147897521436009</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.45009772060802644</c:v>
+                  <c:v>0.57222205703010443</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.44811385633070783</c:v>
+                  <c:v>0.57294191753910673</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.44619103403115284</c:v>
+                  <c:v>0.57363962849398586</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.44432647907400857</c:v>
+                  <c:v>0.57431619669265654</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.44251758247379402</c:v>
+                  <c:v>0.57497256882569536</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.44076188871476224</c:v>
+                  <c:v>0.57560963589599767</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.43905708462990528</c:v>
+                  <c:v>0.5762282372541172</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.43740098923318715</c:v>
+                  <c:v>0.57682916428771924</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.43842098807591462</c:v>
+                  <c:v>0.57654274370335823</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.43941265361745507</c:v>
+                  <c:v>0.57626427924634072</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.44037715024004931</c:v>
+                  <c:v>0.57599344395252916</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.44131557938635724</c:v>
+                  <c:v>0.57572992853152327</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.44222898375543024</c:v>
+                  <c:v>0.57547344018841085</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.44311835116742238</c:v>
+                  <c:v>0.57522370153853819</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.44398461812715501</c:v>
+                  <c:v>0.57498044960684425</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.44482867311356111</c:v>
+                  <c:v>0.5747434349041679</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.44565135961929875</c:v>
+                  <c:v>0.57451242057371132</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.4464534789623929</c:v>
+                  <c:v>0.57428718160151604</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.44586452526785081</c:v>
+                  <c:v>0.571583798981666</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.44528993629756575</c:v>
+                  <c:v>0.56894635252327574</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.44472919284463702</c:v>
+                  <c:v>0.56637245899159372</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.44418180042630184</c:v>
+                  <c:v>0.56385984863923733</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.44364728782957447</c:v>
+                  <c:v>0.56140635853046594</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.44312520575835246</c:v>
+                  <c:v>0.55900992633120083</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.44261512557382515</c:v>
+                  <c:v>0.55666858452732093</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.44211663812076446</c:v>
+                  <c:v>0.55438045503716571</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.44162935263294106</c:v>
+                  <c:v>0.55214374418723877</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.44115289571151373</c:v>
+                  <c:v>0.54995673802286571</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.44597595135360857</c:v>
+                  <c:v>0.54764364558501821</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.45069415796000578</c:v>
+                  <c:v>0.54538083776538482</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.4553108977576632</c:v>
+                  <c:v>0.543166692479507</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.45982940904898745</c:v>
+                  <c:v>0.54099965666779659</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.46425279378681017</c:v>
+                  <c:v>0.53887824266264872</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.4685840246759283</c:v>
+                  <c:v>0.53680102478260805</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.47282595183537385</c:v>
+                  <c:v>0.53476663613720743</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.47698130905278985</c:v>
+                  <c:v>0.53277376562742707</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.4810527196597531</c:v>
+                  <c:v>0.53082115512794548</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.485042702054577</c:v>
+                  <c:v>0.52890759683845334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2880,7 +2896,7 @@
       </c>
       <c r="E3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45402</v>
+        <v>45404</v>
       </c>
       <c r="G3" s="1" t="str" cm="1">
         <f t="array" ref="G3:G6">TRANSPOSE(_xll.ENUM(G2))</f>
@@ -2943,14 +2959,221 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99BC35DD-ADD1-43A6-94D0-1926D9A51F0B}">
+  <dimension ref="B2:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" style="13" customWidth="1"/>
+    <col min="2" max="3" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="15">
+        <v>10</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="11" cm="1">
+        <f t="array" aca="1" ref="E2" ca="1">_xll.\TMX.INSTRUMENT(_xlfn.ANCHORARRAY(B3),_xlfn.ANCHORARRAY(C3))</f>
+        <v>3002384175648</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="13" cm="1">
+        <f t="array" ref="B3:B12">_xlfn.SEQUENCE(B2,1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" cm="1">
+        <f t="array" aca="1" ref="C3:C12" ca="1">_xlfn.RANDARRAY(B2,1)</f>
+        <v>0.68926256462505098</v>
+      </c>
+      <c r="E3" s="13" cm="1">
+        <f t="array" aca="1" ref="E3:F12" ca="1">_xll.TMX.INSTRUMENT(E2)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="13">
+        <f ca="1"/>
+        <v>0.68926256462505098</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="13">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13">
+        <f ca="1"/>
+        <v>0.16684703237718068</v>
+      </c>
+      <c r="E4" s="13">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="F4" s="13">
+        <f ca="1"/>
+        <v>0.16684703237718068</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="13">
+        <v>3</v>
+      </c>
+      <c r="C5" s="13">
+        <f ca="1"/>
+        <v>0.66012003099798866</v>
+      </c>
+      <c r="E5" s="13">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="F5" s="13">
+        <f ca="1"/>
+        <v>0.66012003099798866</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="13">
+        <v>4</v>
+      </c>
+      <c r="C6" s="13">
+        <f ca="1"/>
+        <v>0.97092395139611676</v>
+      </c>
+      <c r="E6" s="13">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="F6" s="13">
+        <f ca="1"/>
+        <v>0.97092395139611676</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="13">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13">
+        <f ca="1"/>
+        <v>0.73248511673096472</v>
+      </c>
+      <c r="E7" s="13">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="F7" s="13">
+        <f ca="1"/>
+        <v>0.73248511673096472</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="13">
+        <v>6</v>
+      </c>
+      <c r="C8" s="13">
+        <f ca="1"/>
+        <v>7.4108078373929853E-2</v>
+      </c>
+      <c r="E8" s="13">
+        <f ca="1"/>
+        <v>6</v>
+      </c>
+      <c r="F8" s="13">
+        <f ca="1"/>
+        <v>7.4108078373929853E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="13">
+        <v>7</v>
+      </c>
+      <c r="C9" s="13">
+        <f ca="1"/>
+        <v>0.59915272648638473</v>
+      </c>
+      <c r="E9" s="13">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="F9" s="13">
+        <f ca="1"/>
+        <v>0.59915272648638473</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="13">
+        <v>8</v>
+      </c>
+      <c r="C10" s="13">
+        <f ca="1"/>
+        <v>0.48966660505380966</v>
+      </c>
+      <c r="E10" s="13">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+      <c r="F10" s="13">
+        <f ca="1"/>
+        <v>0.48966660505380966</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="13">
+        <v>9</v>
+      </c>
+      <c r="C11" s="13">
+        <f ca="1"/>
+        <v>0.3556269310625384</v>
+      </c>
+      <c r="E11" s="13">
+        <f ca="1"/>
+        <v>9</v>
+      </c>
+      <c r="F11" s="13">
+        <f ca="1"/>
+        <v>0.3556269310625384</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="13">
+        <v>10</v>
+      </c>
+      <c r="C12" s="13">
+        <f ca="1"/>
+        <v>0.63915890609686077</v>
+      </c>
+      <c r="E12" s="13">
+        <f ca="1"/>
+        <v>10</v>
+      </c>
+      <c r="F12" s="13">
+        <f ca="1"/>
+        <v>0.63915890609686077</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5540266-91BE-4B2E-A8BC-1082BDC425C0}">
   <dimension ref="B2:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="8"/>
+    <col min="1" max="1" width="3.7109375" style="8" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="8"/>
     <col min="6" max="6" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="8"/>
   </cols>
@@ -2967,7 +3190,7 @@
       </c>
       <c r="F2" s="11" cm="1">
         <f t="array" aca="1" ref="F2" ca="1">_xll.\TMX.CURVE.PWFLAT(time,rate)</f>
-        <v>2119430488624</v>
+        <v>3002389605104</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>15</v>
@@ -2989,7 +3212,7 @@
       </c>
       <c r="C3" s="8" cm="1">
         <f t="array" aca="1" ref="C3:C12" ca="1">_xlfn.RANDARRAY(ROWS(_xlfn.ANCHORARRAY(B3)))</f>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="F3" s="8" cm="1">
         <f t="array" aca="1" ref="F3:G13" ca="1">TRANSPOSE(_xll.TMX.CURVE.PWFLAT(F2))</f>
@@ -2997,7 +3220,7 @@
       </c>
       <c r="G3" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="I3" s="8" cm="1">
         <f t="array" ref="I3:I103">_xll.ARRAY.SEQUENCE(0,10,0.1)</f>
@@ -3005,11 +3228,11 @@
       </c>
       <c r="J3" s="8" cm="1">
         <f t="array" aca="1" ref="J3:J103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY($I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.PWFLAT.FORWARD(pwflat,_xlpm.t)))</f>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="K3" s="8" cm="1">
         <f t="array" aca="1" ref="K3:K103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY($I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.PWFLAT.SPOT(pwflat,_xlpm.t)))</f>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="L3" s="8" cm="1">
         <f t="array" aca="1" ref="L3:L103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY($I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.PWFLAT.DISCOUNT(pwflat,_xlpm.t)))</f>
@@ -3022,7 +3245,7 @@
       </c>
       <c r="C4" s="8">
         <f ca="1"/>
-        <v>0.33643114122081186</v>
+        <v>3.2461778028678001E-2</v>
       </c>
       <c r="F4" s="8">
         <f ca="1"/>
@@ -3030,22 +3253,22 @@
       </c>
       <c r="G4" s="8">
         <f ca="1"/>
-        <v>0.33643114122081186</v>
+        <v>3.2461778028678001E-2</v>
       </c>
       <c r="I4" s="8">
         <v>0.1</v>
       </c>
       <c r="J4" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="K4" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="L4" s="8">
         <f ca="1"/>
-        <v>0.92688550722812701</v>
+        <v>0.91827528025606131</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
@@ -3054,7 +3277,7 @@
       </c>
       <c r="C5" s="8">
         <f ca="1"/>
-        <v>0.66519395089168798</v>
+        <v>0.9013900471794476</v>
       </c>
       <c r="F5" s="8">
         <f ca="1"/>
@@ -3062,22 +3285,22 @@
       </c>
       <c r="G5" s="8">
         <f ca="1"/>
-        <v>0.66519395089168798</v>
+        <v>0.9013900471794476</v>
       </c>
       <c r="I5" s="8">
         <v>0.2</v>
       </c>
       <c r="J5" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="K5" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="L5" s="8">
         <f ca="1"/>
-        <v>0.85911674349734801</v>
+        <v>0.84322949030014638</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
@@ -3086,7 +3309,7 @@
       </c>
       <c r="C6" s="8">
         <f ca="1"/>
-        <v>0.19062816323881138</v>
+        <v>0.27300148238849498</v>
       </c>
       <c r="F6" s="8">
         <f ca="1"/>
@@ -3094,22 +3317,22 @@
       </c>
       <c r="G6" s="8">
         <f ca="1"/>
-        <v>0.19062816323881138</v>
+        <v>0.27300148238849498</v>
       </c>
       <c r="I6" s="8">
         <v>0.30000000000000004</v>
       </c>
       <c r="J6" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="K6" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557745</v>
       </c>
       <c r="L6" s="8">
         <f ca="1"/>
-        <v>0.7963028583934012</v>
+        <v>0.77431679609439374</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
@@ -3118,7 +3341,7 @@
       </c>
       <c r="C7" s="8">
         <f ca="1"/>
-        <v>0.43828870656484975</v>
+        <v>0.85065876641893867</v>
       </c>
       <c r="F7" s="8">
         <f ca="1"/>
@@ -3126,22 +3349,22 @@
       </c>
       <c r="G7" s="8">
         <f ca="1"/>
-        <v>0.43828870656484975</v>
+        <v>0.85065876641893867</v>
       </c>
       <c r="I7" s="8">
         <v>0.4</v>
       </c>
       <c r="J7" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="K7" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="L7" s="8">
         <f ca="1"/>
-        <v>0.73808157902811433</v>
+        <v>0.71103597350744163</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -3150,7 +3373,7 @@
       </c>
       <c r="C8" s="8">
         <f ca="1"/>
-        <v>0.34888225615158475</v>
+        <v>0.50941830878664573</v>
       </c>
       <c r="F8" s="8">
         <f ca="1"/>
@@ -3158,22 +3381,22 @@
       </c>
       <c r="G8" s="8">
         <f ca="1"/>
-        <v>0.34888225615158475</v>
+        <v>0.50941830878664573</v>
       </c>
       <c r="I8" s="8">
         <v>0.5</v>
       </c>
       <c r="J8" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="K8" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="L8" s="8">
         <f ca="1"/>
-        <v>0.6841171191313361</v>
+        <v>0.65292675763487495</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
@@ -3182,7 +3405,7 @@
       </c>
       <c r="C9" s="8">
         <f ca="1"/>
-        <v>0.32313040685963279</v>
+        <v>0.61829312960625149</v>
       </c>
       <c r="F9" s="8">
         <f ca="1"/>
@@ -3190,22 +3413,22 @@
       </c>
       <c r="G9" s="8">
         <f ca="1"/>
-        <v>0.32313040685963279</v>
+        <v>0.61829312960625149</v>
       </c>
       <c r="I9" s="8">
         <v>0.60000000000000009</v>
       </c>
       <c r="J9" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="K9" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557745</v>
       </c>
       <c r="L9" s="8">
         <f ca="1"/>
-        <v>0.63409824246276214</v>
+        <v>0.59956650107485587</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -3214,7 +3437,7 @@
       </c>
       <c r="C10" s="8">
         <f ca="1"/>
-        <v>0.50982090706683314</v>
+        <v>0.55649330279809406</v>
       </c>
       <c r="F10" s="8">
         <f ca="1"/>
@@ -3222,22 +3445,22 @@
       </c>
       <c r="G10" s="8">
         <f ca="1"/>
-        <v>0.50982090706683314</v>
+        <v>0.55649330279809406</v>
       </c>
       <c r="I10" s="8">
         <v>0.70000000000000007</v>
       </c>
       <c r="J10" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="K10" s="8">
         <f ca="1"/>
-        <v>0.75925229970493102</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="L10" s="8">
         <f ca="1"/>
-        <v>0.58773647071752899</v>
+        <v>0.55056709718109975</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
@@ -3246,7 +3469,7 @@
       </c>
       <c r="C11" s="8">
         <f ca="1"/>
-        <v>0.39874822970447998</v>
+        <v>0.35531318939366341</v>
       </c>
       <c r="F11" s="8">
         <f ca="1"/>
@@ -3254,22 +3477,22 @@
       </c>
       <c r="G11" s="8">
         <f ca="1"/>
-        <v>0.39874822970447998</v>
+        <v>0.35531318939366341</v>
       </c>
       <c r="I11" s="8">
         <v>0.8</v>
       </c>
       <c r="J11" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="K11" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="L11" s="8">
         <f ca="1"/>
-        <v>0.54476441731284919</v>
+        <v>0.50557215573746372</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
@@ -3278,7 +3501,7 @@
       </c>
       <c r="C12" s="8">
         <f ca="1"/>
-        <v>0.88005095914214659</v>
+        <v>0.33946532617874281</v>
       </c>
       <c r="F12" s="8">
         <f ca="1"/>
@@ -3286,22 +3509,22 @@
       </c>
       <c r="G12" s="8">
         <f ca="1"/>
-        <v>0.88005095914214659</v>
+        <v>0.33946532617874281</v>
       </c>
       <c r="I12" s="8">
         <v>0.9</v>
       </c>
       <c r="J12" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="K12" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="L12" s="8">
         <f ca="1"/>
-        <v>0.5049342435269778</v>
+        <v>0.46425441259068356</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
@@ -3318,15 +3541,15 @@
       </c>
       <c r="J13" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="K13" s="8">
         <f ca="1"/>
-        <v>0.75925229970493113</v>
+        <v>0.85258063760557756</v>
       </c>
       <c r="L13" s="8">
         <f ca="1"/>
-        <v>0.46801623202139542</v>
+        <v>0.42631335061531511</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
@@ -3335,15 +3558,15 @@
       </c>
       <c r="J14" s="8">
         <f ca="1"/>
-        <v>0.33643114122081186</v>
+        <v>3.2461778028678001E-2</v>
       </c>
       <c r="K14" s="8">
         <f ca="1"/>
-        <v>0.72081401257001121</v>
+        <v>0.7780243776440412</v>
       </c>
       <c r="L14" s="8">
         <f ca="1"/>
-        <v>0.45253262721662568</v>
+        <v>0.4249317054113852</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
@@ -3352,15 +3575,15 @@
       </c>
       <c r="J15" s="8">
         <f ca="1"/>
-        <v>0.33643114122081186</v>
+        <v>3.2461778028678001E-2</v>
       </c>
       <c r="K15" s="8">
         <f ca="1"/>
-        <v>0.68878210662424455</v>
+        <v>0.71589416100942749</v>
       </c>
       <c r="L15" s="8">
         <f ca="1"/>
-        <v>0.43756127388145027</v>
+        <v>0.42355453800104653</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
@@ -3369,15 +3592,15 @@
       </c>
       <c r="J16" s="8">
         <f ca="1"/>
-        <v>0.33643114122081186</v>
+        <v>3.2461778028678001E-2</v>
       </c>
       <c r="K16" s="8">
         <f ca="1"/>
-        <v>0.66167818620859598</v>
+        <v>0.66332243924167766</v>
       </c>
       <c r="L16" s="8">
         <f ca="1"/>
-        <v>0.42308522493990602</v>
+        <v>0.42218183387212821</v>
       </c>
     </row>
     <row r="17" spans="9:12" x14ac:dyDescent="0.3">
@@ -3386,15 +3609,15 @@
       </c>
       <c r="J17" s="8">
         <f ca="1"/>
-        <v>0.33643114122081186</v>
+        <v>3.2461778028678001E-2</v>
       </c>
       <c r="K17" s="8">
         <f ca="1"/>
-        <v>0.63844625442375424</v>
+        <v>0.61826096344074899</v>
       </c>
       <c r="L17" s="8">
         <f ca="1"/>
-        <v>0.4090880939773292</v>
+        <v>0.42081357855949186</v>
       </c>
     </row>
     <row r="18" spans="9:12" x14ac:dyDescent="0.3">
@@ -3403,15 +3626,15 @@
       </c>
       <c r="J18" s="8">
         <f ca="1"/>
-        <v>0.33643114122081186</v>
+        <v>3.2461778028678001E-2</v>
       </c>
       <c r="K18" s="8">
         <f ca="1"/>
-        <v>0.61831191354355808</v>
+        <v>0.57920768441327775</v>
       </c>
       <c r="L18" s="8">
         <f ca="1"/>
-        <v>0.39555403668913763</v>
+        <v>0.41944975764487846</v>
       </c>
     </row>
     <row r="19" spans="9:12" x14ac:dyDescent="0.3">
@@ -3420,15 +3643,15 @@
       </c>
       <c r="J19" s="8">
         <f ca="1"/>
-        <v>0.33643114122081186</v>
+        <v>3.2461778028678001E-2</v>
       </c>
       <c r="K19" s="8">
         <f ca="1"/>
-        <v>0.60069436527338638</v>
+        <v>0.5450360652642402</v>
       </c>
       <c r="L19" s="8">
         <f ca="1"/>
-        <v>0.38246773423956143</v>
+        <v>0.41809035675675582</v>
       </c>
     </row>
     <row r="20" spans="9:12" x14ac:dyDescent="0.3">
@@ -3437,15 +3660,15 @@
       </c>
       <c r="J20" s="8">
         <f ca="1"/>
-        <v>0.33643114122081186</v>
+        <v>3.2461778028678001E-2</v>
       </c>
       <c r="K20" s="8">
         <f ca="1"/>
-        <v>0.585149469740882</v>
+        <v>0.51488463660332473</v>
       </c>
       <c r="L20" s="8">
         <f ca="1"/>
-        <v>0.36981437139069079</v>
+        <v>0.41673536157016872</v>
       </c>
     </row>
     <row r="21" spans="9:12" x14ac:dyDescent="0.3">
@@ -3454,15 +3677,15 @@
       </c>
       <c r="J21" s="8">
         <f ca="1"/>
-        <v>0.33643114122081186</v>
+        <v>3.2461778028678001E-2</v>
       </c>
       <c r="K21" s="8">
         <f ca="1"/>
-        <v>0.57133178482310032</v>
+        <v>0.48808336668251107</v>
       </c>
       <c r="L21" s="8">
         <f ca="1"/>
-        <v>0.35757962582089259</v>
+        <v>0.41538475780658657</v>
       </c>
     </row>
     <row r="22" spans="9:12" x14ac:dyDescent="0.3">
@@ -3471,15 +3694,15 @@
       </c>
       <c r="J22" s="8">
         <f ca="1"/>
-        <v>0.33643114122081186</v>
+        <v>3.2461778028678001E-2</v>
       </c>
       <c r="K22" s="8">
         <f ca="1"/>
-        <v>0.55896859305455882</v>
+        <v>0.46410328306915138</v>
       </c>
       <c r="L22" s="8">
         <f ca="1"/>
-        <v>0.34574964822632431</v>
+        <v>0.414038531233753</v>
       </c>
     </row>
     <row r="23" spans="9:12" x14ac:dyDescent="0.3">
@@ -3488,15 +3711,15 @@
       </c>
       <c r="J23" s="8">
         <f ca="1"/>
-        <v>0.33643114122081186</v>
+        <v>3.2461778028678001E-2</v>
       </c>
       <c r="K23" s="8">
         <f ca="1"/>
-        <v>0.5478417204628715</v>
+        <v>0.44252120781712778</v>
       </c>
       <c r="L23" s="8">
         <f ca="1"/>
-        <v>0.33431104749081081</v>
+        <v>0.41269666766553664</v>
       </c>
     </row>
     <row r="24" spans="9:12" x14ac:dyDescent="0.3">
@@ -3505,15 +3728,15 @@
       </c>
       <c r="J24" s="8">
         <f ca="1"/>
-        <v>0.66519395089168798</v>
+        <v>0.9013900471794476</v>
       </c>
       <c r="K24" s="8">
         <f ca="1"/>
-        <v>0.5534299219118628</v>
+        <v>0.46437210492961922</v>
       </c>
       <c r="L24" s="8">
         <f ca="1"/>
-        <v>0.31279638331484094</v>
+        <v>0.37712392950874002</v>
       </c>
     </row>
     <row r="25" spans="9:12" x14ac:dyDescent="0.3">
@@ -3522,15 +3745,15 @@
       </c>
       <c r="J25" s="8">
         <f ca="1"/>
-        <v>0.66519395089168798</v>
+        <v>0.9013900471794476</v>
       </c>
       <c r="K25" s="8">
         <f ca="1"/>
-        <v>0.55851010504730936</v>
+        <v>0.48423655685006595</v>
       </c>
       <c r="L25" s="8">
         <f ca="1"/>
-        <v>0.29266629856937243</v>
+        <v>0.34461741335487162</v>
       </c>
     </row>
     <row r="26" spans="9:12" x14ac:dyDescent="0.3">
@@ -3539,15 +3762,15 @@
       </c>
       <c r="J26" s="8">
         <f ca="1"/>
-        <v>0.66519395089168798</v>
+        <v>0.9013900471794476</v>
       </c>
       <c r="K26" s="8">
         <f ca="1"/>
-        <v>0.5631485331274998</v>
+        <v>0.5023736651252565</v>
       </c>
       <c r="L26" s="8">
         <f ca="1"/>
-        <v>0.27383169103324012</v>
+        <v>0.31491282430173329</v>
       </c>
     </row>
     <row r="27" spans="9:12" x14ac:dyDescent="0.3">
@@ -3556,15 +3779,15 @@
       </c>
       <c r="J27" s="8">
         <f ca="1"/>
-        <v>0.66519395089168798</v>
+        <v>0.9013900471794476</v>
       </c>
       <c r="K27" s="8">
         <f ca="1"/>
-        <v>0.567400425534341</v>
+        <v>0.51899934771084777</v>
       </c>
       <c r="L27" s="8">
         <f ca="1"/>
-        <v>0.2562091888145116</v>
+        <v>0.2877686456754891</v>
       </c>
     </row>
     <row r="28" spans="9:12" x14ac:dyDescent="0.3">
@@ -3573,15 +3796,15 @@
       </c>
       <c r="J28" s="8">
         <f ca="1"/>
-        <v>0.66519395089168798</v>
+        <v>0.9013900471794476</v>
       </c>
       <c r="K28" s="8">
         <f ca="1"/>
-        <v>0.57131216654863481</v>
+        <v>0.53429497568959172</v>
       </c>
       <c r="L28" s="8">
         <f ca="1"/>
-        <v>0.23972078811322978</v>
+        <v>0.26296418322666909</v>
       </c>
     </row>
     <row r="29" spans="9:12" x14ac:dyDescent="0.3">
@@ -3590,15 +3813,15 @@
       </c>
       <c r="J29" s="8">
         <f ca="1"/>
-        <v>0.66519395089168798</v>
+        <v>0.9013900471794476</v>
       </c>
       <c r="K29" s="8">
         <f ca="1"/>
-        <v>0.57492300440798305</v>
+        <v>0.5484140169007401</v>
       </c>
       <c r="L29" s="8">
         <f ca="1"/>
-        <v>0.22429350151545649</v>
+        <v>0.24029776351327548</v>
       </c>
     </row>
     <row r="30" spans="9:12" x14ac:dyDescent="0.3">
@@ -3607,15 +3830,15 @@
       </c>
       <c r="J30" s="8">
         <f ca="1"/>
-        <v>0.66519395089168798</v>
+        <v>0.9013900471794476</v>
       </c>
       <c r="K30" s="8">
         <f ca="1"/>
-        <v>0.57826637279626836</v>
+        <v>0.5614872032073589</v>
       </c>
       <c r="L30" s="8">
         <f ca="1"/>
-        <v>0.20985904164560895</v>
+        <v>0.21958509456729031</v>
       </c>
     </row>
     <row r="31" spans="9:12" x14ac:dyDescent="0.3">
@@ -3624,15 +3847,15 @@
       </c>
       <c r="J31" s="8">
         <f ca="1"/>
-        <v>0.66519395089168798</v>
+        <v>0.9013900471794476</v>
       </c>
       <c r="K31" s="8">
         <f ca="1"/>
-        <v>0.58137092915681909</v>
+        <v>0.57362659049207643</v>
       </c>
       <c r="L31" s="8">
         <f ca="1"/>
-        <v>0.19635351500970671</v>
+        <v>0.20065777195083925</v>
       </c>
     </row>
     <row r="32" spans="9:12" x14ac:dyDescent="0.3">
@@ -3641,15 +3864,15 @@
       </c>
       <c r="J32" s="8">
         <f ca="1"/>
-        <v>0.66519395089168798</v>
+        <v>0.9013900471794476</v>
       </c>
       <c r="K32" s="8">
         <f ca="1"/>
-        <v>0.58426137818215929</v>
+        <v>0.58492877865370985</v>
       </c>
       <c r="L32" s="8">
         <f ca="1"/>
-        <v>0.18371713797797554</v>
+        <v>0.18336190443210154</v>
       </c>
     </row>
     <row r="33" spans="9:12" x14ac:dyDescent="0.3">
@@ -3658,15 +3881,15 @@
       </c>
       <c r="J33" s="8">
         <f ca="1"/>
-        <v>0.66519395089168798</v>
+        <v>0.9013900471794476</v>
       </c>
       <c r="K33" s="8">
         <f ca="1"/>
-        <v>0.58695913060581029</v>
+        <v>0.59547748760456776</v>
       </c>
       <c r="L33" s="8">
         <f ca="1"/>
-        <v>0.17189397889956717</v>
+        <v>0.16755686955834523</v>
       </c>
     </row>
     <row r="34" spans="9:12" x14ac:dyDescent="0.3">
@@ -3675,15 +3898,15 @@
       </c>
       <c r="J34" s="8">
         <f ca="1"/>
-        <v>0.19062816323881138</v>
+        <v>0.27300148238849498</v>
       </c>
       <c r="K34" s="8">
         <f ca="1"/>
-        <v>0.57417426069074584</v>
+        <v>0.58507503582340403</v>
       </c>
       <c r="L34" s="8">
         <f ca="1"/>
-        <v>0.16864823031938309</v>
+        <v>0.16304441760002616</v>
       </c>
     </row>
     <row r="35" spans="9:12" x14ac:dyDescent="0.3">
@@ -3692,15 +3915,15 @@
       </c>
       <c r="J35" s="8">
         <f ca="1"/>
-        <v>0.19062816323881138</v>
+        <v>0.27300148238849498</v>
       </c>
       <c r="K35" s="8">
         <f ca="1"/>
-        <v>0.56218844514537292</v>
+        <v>0.5753227372785632</v>
       </c>
       <c r="L35" s="8">
         <f ca="1"/>
-        <v>0.16546376882666955</v>
+        <v>0.15865348985128819</v>
       </c>
     </row>
     <row r="36" spans="9:12" x14ac:dyDescent="0.3">
@@ -3709,15 +3932,15 @@
       </c>
       <c r="J36" s="8">
         <f ca="1"/>
-        <v>0.19062816323881138</v>
+        <v>0.27300148238849498</v>
       </c>
       <c r="K36" s="8">
         <f ca="1"/>
-        <v>0.55092904266335585</v>
+        <v>0.56616148713037928</v>
       </c>
       <c r="L36" s="8">
         <f ca="1"/>
-        <v>0.16233943717996824</v>
+        <v>0.15438081355156302</v>
       </c>
     </row>
     <row r="37" spans="9:12" x14ac:dyDescent="0.3">
@@ -3726,15 +3949,15 @@
       </c>
       <c r="J37" s="8">
         <f ca="1"/>
-        <v>0.19062816323881138</v>
+        <v>0.27300148238849498</v>
       </c>
       <c r="K37" s="8">
         <f ca="1"/>
-        <v>0.54033195797439859</v>
+        <v>0.55753913404973565</v>
       </c>
       <c r="L37" s="8">
         <f ca="1"/>
-        <v>0.1592740999888515</v>
+        <v>0.15022320407681938</v>
       </c>
     </row>
     <row r="38" spans="9:12" x14ac:dyDescent="0.3">
@@ -3743,15 +3966,15 @@
       </c>
       <c r="J38" s="8">
         <f ca="1"/>
-        <v>0.19062816323881138</v>
+        <v>0.27300148238849498</v>
       </c>
       <c r="K38" s="8">
         <f ca="1"/>
-        <v>0.53034042098195333</v>
+        <v>0.54940948685941449</v>
       </c>
       <c r="L38" s="8">
         <f ca="1"/>
-        <v>0.15626664330128379</v>
+        <v>0.14617756256563347</v>
       </c>
     </row>
     <row r="39" spans="9:12" x14ac:dyDescent="0.3">
@@ -3760,15 +3983,15 @@
       </c>
       <c r="J39" s="8">
         <f ca="1"/>
-        <v>0.19062816323881138</v>
+        <v>0.27300148238849498</v>
       </c>
       <c r="K39" s="8">
         <f ca="1"/>
-        <v>0.52090396937797712</v>
+        <v>0.5417314867352222</v>
       </c>
       <c r="L39" s="8">
         <f ca="1"/>
-        <v>0.15331597419876711</v>
+        <v>0.14224087570211402</v>
       </c>
     </row>
     <row r="40" spans="9:12" x14ac:dyDescent="0.3">
@@ -3777,15 +4000,15 @@
       </c>
       <c r="J40" s="8">
         <f ca="1"/>
-        <v>0.19062816323881138</v>
+        <v>0.27300148238849498</v>
       </c>
       <c r="K40" s="8">
         <f ca="1"/>
-        <v>0.51197759623908079</v>
+        <v>0.5344685136447701</v>
       </c>
       <c r="L40" s="8">
         <f ca="1"/>
-        <v>0.15042102039912819</v>
+        <v>0.13841020561741718</v>
       </c>
     </row>
     <row r="41" spans="9:12" x14ac:dyDescent="0.3">
@@ -3794,15 +4017,15 @@
       </c>
       <c r="J41" s="8">
         <f ca="1"/>
-        <v>0.19062816323881138</v>
+        <v>0.27300148238849498</v>
       </c>
       <c r="K41" s="8">
         <f ca="1"/>
-        <v>0.5035210322127579</v>
+        <v>0.52758780229592073</v>
       </c>
       <c r="L41" s="8">
         <f ca="1"/>
-        <v>0.14758072986679688</v>
+        <v>0.13468269881604389</v>
       </c>
     </row>
     <row r="42" spans="9:12" x14ac:dyDescent="0.3">
@@ -3811,15 +4034,15 @@
       </c>
       <c r="J42" s="8">
         <f ca="1"/>
-        <v>0.19062816323881138</v>
+        <v>0.27300148238849498</v>
       </c>
       <c r="K42" s="8">
         <f ca="1"/>
-        <v>0.49549813813650284</v>
+        <v>0.52105994793932009</v>
       </c>
       <c r="L42" s="8">
         <f ca="1"/>
-        <v>0.14479407223797325</v>
+        <v>0.13105557702486409</v>
       </c>
     </row>
     <row r="43" spans="9:12" x14ac:dyDescent="0.3">
@@ -3828,15 +4051,15 @@
       </c>
       <c r="J43" s="8">
         <f ca="1"/>
-        <v>0.19062816323881138</v>
+        <v>0.27300148238849498</v>
       </c>
       <c r="K43" s="8">
         <f ca="1"/>
-        <v>0.48787638876406059</v>
+        <v>0.51485848630054953</v>
       </c>
       <c r="L43" s="8">
         <f ca="1"/>
-        <v>0.14206003152273289</v>
+        <v>0.12752613679279967</v>
       </c>
     </row>
     <row r="44" spans="9:12" x14ac:dyDescent="0.3">
@@ -3845,15 +4068,15 @@
       </c>
       <c r="J44" s="8">
         <f ca="1"/>
-        <v>0.43828870656484975</v>
+        <v>0.85065876641893867</v>
       </c>
       <c r="K44" s="8">
         <f ca="1"/>
-        <v>0.48666693310066517</v>
+        <v>0.52304873703514443</v>
       </c>
       <c r="L44" s="8">
         <f ca="1"/>
-        <v>0.1359681756273346</v>
+        <v>0.11712660764265916</v>
       </c>
     </row>
     <row r="45" spans="9:12" x14ac:dyDescent="0.3">
@@ -3862,15 +4085,15 @@
       </c>
       <c r="J45" s="8">
         <f ca="1"/>
-        <v>0.43828870656484975</v>
+        <v>0.85065876641893867</v>
       </c>
       <c r="K45" s="8">
         <f ca="1"/>
-        <v>0.48551507056409821</v>
+        <v>0.53084897582999668</v>
       </c>
       <c r="L45" s="8">
         <f ca="1"/>
-        <v>0.13013755236042376</v>
+        <v>0.10757513977922312</v>
       </c>
     </row>
     <row r="46" spans="9:12" x14ac:dyDescent="0.3">
@@ -3879,15 +4102,15 @@
       </c>
       <c r="J46" s="8">
         <f ca="1"/>
-        <v>0.43828870656484975</v>
+        <v>0.85065876641893867</v>
       </c>
       <c r="K46" s="8">
         <f ca="1"/>
-        <v>0.48441678302923191</v>
+        <v>0.5382864128204371</v>
       </c>
       <c r="L46" s="8">
         <f ca="1"/>
-        <v>0.12455695949270629</v>
+        <v>9.8802578118776546E-2</v>
       </c>
     </row>
     <row r="47" spans="9:12" x14ac:dyDescent="0.3">
@@ -3896,15 +4119,15 @@
       </c>
       <c r="J47" s="8">
         <f ca="1"/>
-        <v>0.43828870656484975</v>
+        <v>0.85065876641893867</v>
       </c>
       <c r="K47" s="8">
         <f ca="1"/>
-        <v>0.4833684176550414</v>
+        <v>0.54538578449313035</v>
       </c>
       <c r="L47" s="8">
         <f ca="1"/>
-        <v>0.11921567517805101</v>
+        <v>9.0745403032967159E-2</v>
       </c>
     </row>
     <row r="48" spans="9:12" x14ac:dyDescent="0.3">
@@ -3913,15 +4136,15 @@
       </c>
       <c r="J48" s="8">
         <f ca="1"/>
-        <v>0.43828870656484975</v>
+        <v>0.85065876641893867</v>
       </c>
       <c r="K48" s="8">
         <f ca="1"/>
-        <v>0.48236664629748166</v>
+        <v>0.5521696285359261</v>
       </c>
       <c r="L48" s="8">
         <f ca="1"/>
-        <v>0.11410343735554</v>
+        <v>8.3345275837926447E-2</v>
       </c>
     </row>
     <row r="49" spans="9:12" x14ac:dyDescent="0.3">
@@ -3930,15 +4153,15 @@
       </c>
       <c r="J49" s="8">
         <f ca="1"/>
-        <v>0.43828870656484975</v>
+        <v>0.85065876641893867</v>
       </c>
       <c r="K49" s="8">
         <f ca="1"/>
-        <v>0.48140843021633745</v>
+        <v>0.55865852283773076</v>
       </c>
       <c r="L49" s="8">
         <f ca="1"/>
-        <v>0.10921042195304825</v>
+        <v>7.6548618871669416E-2</v>
       </c>
     </row>
     <row r="50" spans="9:12" x14ac:dyDescent="0.3">
@@ -3947,15 +4170,15 @@
       </c>
       <c r="J50" s="8">
         <f ca="1"/>
-        <v>0.43828870656484975</v>
+        <v>0.85065876641893867</v>
       </c>
       <c r="K50" s="8">
         <f ca="1"/>
-        <v>0.48049098928758238</v>
+        <v>0.56487129397775648</v>
       </c>
       <c r="L50" s="8">
         <f ca="1"/>
-        <v>0.1045272315251778</v>
+        <v>7.0306215513893405E-2</v>
       </c>
     </row>
     <row r="51" spans="9:12" x14ac:dyDescent="0.3">
@@ -3964,15 +4187,15 @@
       </c>
       <c r="J51" s="8">
         <f ca="1"/>
-        <v>0.43828870656484975</v>
+        <v>0.85065876641893867</v>
       </c>
       <c r="K51" s="8">
         <f ca="1"/>
-        <v>0.47961177506419206</v>
+        <v>0.57082519965361445</v>
       </c>
       <c r="L51" s="8">
         <f ca="1"/>
-        <v>0.10004486687167619</v>
+        <v>6.4572869375704112E-2</v>
       </c>
     </row>
     <row r="52" spans="9:12" x14ac:dyDescent="0.3">
@@ -3981,15 +4204,15 @@
       </c>
       <c r="J52" s="8">
         <f ca="1"/>
-        <v>0.43828870656484975</v>
+        <v>0.85065876641893867</v>
       </c>
       <c r="K52" s="8">
         <f ca="1"/>
-        <v>0.47876844713563416</v>
+        <v>0.57653608877127416</v>
       </c>
       <c r="L52" s="8">
         <f ca="1"/>
-        <v>9.5754716113430852E-2</v>
+        <v>5.9307064924702342E-2</v>
       </c>
     </row>
     <row r="53" spans="9:12" x14ac:dyDescent="0.3">
@@ -3998,15 +4221,15 @@
       </c>
       <c r="J53" s="8">
         <f ca="1"/>
-        <v>0.43828870656484975</v>
+        <v>0.85065876641893867</v>
       </c>
       <c r="K53" s="8">
         <f ca="1"/>
-        <v>0.47795885232421842</v>
+        <v>0.58201854232422734</v>
       </c>
       <c r="L53" s="8">
         <f ca="1"/>
-        <v>9.1648536663293839E-2</v>
+        <v>5.4470678885610135E-2</v>
       </c>
     </row>
     <row r="54" spans="9:12" x14ac:dyDescent="0.3">
@@ -4015,15 +4238,15 @@
       </c>
       <c r="J54" s="8">
         <f ca="1"/>
-        <v>0.34888225615158475</v>
+        <v>0.50941830878664573</v>
       </c>
       <c r="K54" s="8">
         <f ca="1"/>
-        <v>0.47542793867377459</v>
+        <v>0.58059500833329436</v>
       </c>
       <c r="L54" s="8">
         <f ca="1"/>
-        <v>8.8506215273145908E-2</v>
+        <v>5.1765335054997662E-2</v>
       </c>
     </row>
     <row r="55" spans="9:12" x14ac:dyDescent="0.3">
@@ -4032,15 +4255,15 @@
       </c>
       <c r="J55" s="8">
         <f ca="1"/>
-        <v>0.34888225615158475</v>
+        <v>0.50941830878664573</v>
       </c>
       <c r="K55" s="8">
         <f ca="1"/>
-        <v>0.47299436785604021</v>
+        <v>0.57922622564970505</v>
       </c>
       <c r="L55" s="8">
         <f ca="1"/>
-        <v>8.5471633467659264E-2</v>
+        <v>4.9194354846936274E-2</v>
       </c>
     </row>
     <row r="56" spans="9:12" x14ac:dyDescent="0.3">
@@ -4049,15 +4272,15 @@
       </c>
       <c r="J56" s="8">
         <f ca="1"/>
-        <v>0.34888225615158475</v>
+        <v>0.50941830878664573</v>
       </c>
       <c r="K56" s="8">
         <f ca="1"/>
-        <v>0.47065262989935236</v>
+        <v>0.57790909514285482</v>
       </c>
       <c r="L56" s="8">
         <f ca="1"/>
-        <v>8.2541099380506092E-2</v>
+        <v>4.6751064907068401E-2</v>
       </c>
     </row>
     <row r="57" spans="9:12" x14ac:dyDescent="0.3">
@@ -4066,15 +4289,15 @@
       </c>
       <c r="J57" s="8">
         <f ca="1"/>
-        <v>0.34888225615158475</v>
+        <v>0.50941830878664573</v>
       </c>
       <c r="K57" s="8">
         <f ca="1"/>
-        <v>0.46839762297809739</v>
+        <v>0.57664074724736947</v>
       </c>
       <c r="L57" s="8">
         <f ca="1"/>
-        <v>7.9711041865570584E-2</v>
+        <v>4.4429126324576899E-2</v>
       </c>
     </row>
     <row r="58" spans="9:12" x14ac:dyDescent="0.3">
@@ -4083,15 +4306,15 @@
       </c>
       <c r="J58" s="8">
         <f ca="1"/>
-        <v>0.34888225615158475</v>
+        <v>0.50941830878664573</v>
       </c>
       <c r="K58" s="8">
         <f ca="1"/>
-        <v>0.46622461630852446</v>
+        <v>0.57541852109353819</v>
       </c>
       <c r="L58" s="8">
         <f ca="1"/>
-        <v>7.6978017559777928E-2</v>
+        <v>4.2222507248794033E-2</v>
       </c>
     </row>
     <row r="59" spans="9:12" x14ac:dyDescent="0.3">
@@ -4100,15 +4323,15 @@
       </c>
       <c r="J59" s="8">
         <f ca="1"/>
-        <v>0.34888225615158475</v>
+        <v>0.50941830878664573</v>
       </c>
       <c r="K59" s="8">
         <f ca="1"/>
-        <v>0.46412921702000765</v>
+        <v>0.57423994587377214</v>
       </c>
       <c r="L59" s="8">
         <f ca="1"/>
-        <v>7.4338699525952678E-2</v>
+        <v>4.0125482295890406E-2</v>
       </c>
     </row>
     <row r="60" spans="9:12" x14ac:dyDescent="0.3">
@@ -4117,15 +4340,15 @@
       </c>
       <c r="J60" s="8">
         <f ca="1"/>
-        <v>0.34888225615158475</v>
+        <v>0.50941830878664573</v>
       </c>
       <c r="K60" s="8">
         <f ca="1"/>
-        <v>0.46210734051354407</v>
+        <v>0.57310272417048924</v>
       </c>
       <c r="L60" s="8">
         <f ca="1"/>
-        <v>7.1789874897971104E-2</v>
+        <v>3.8132608382424084E-2</v>
       </c>
     </row>
     <row r="61" spans="9:12" x14ac:dyDescent="0.3">
@@ -4134,15 +4357,15 @@
       </c>
       <c r="J61" s="8">
         <f ca="1"/>
-        <v>0.34888225615158475</v>
+        <v>0.50941830878664573</v>
       </c>
       <c r="K61" s="8">
         <f ca="1"/>
-        <v>0.46015518388661369</v>
+        <v>0.57200471700869882</v>
       </c>
       <c r="L61" s="8">
         <f ca="1"/>
-        <v>6.9328440969987984E-2</v>
+        <v>3.6238712769270841E-2</v>
       </c>
     </row>
     <row r="62" spans="9:12" x14ac:dyDescent="0.3">
@@ -4151,15 +4374,15 @@
       </c>
       <c r="J62" s="8">
         <f ca="1"/>
-        <v>0.34888225615158475</v>
+        <v>0.50941830878664573</v>
       </c>
       <c r="K62" s="8">
         <f ca="1"/>
-        <v>0.45826920206059635</v>
+        <v>0.57094393042866409</v>
       </c>
       <c r="L62" s="8">
         <f ca="1"/>
-        <v>6.6951401419826459E-2</v>
+        <v>3.4438879637098699E-2</v>
       </c>
     </row>
     <row r="63" spans="9:12" x14ac:dyDescent="0.3">
@@ -4168,15 +4391,15 @@
       </c>
       <c r="J63" s="8">
         <f ca="1"/>
-        <v>0.34888225615158475</v>
+        <v>0.50941830878664573</v>
       </c>
       <c r="K63" s="8">
         <f ca="1"/>
-        <v>0.4564460862954462</v>
+        <v>0.56991850340129713</v>
       </c>
       <c r="L63" s="8">
         <f ca="1"/>
-        <v>6.4655862661935487E-2</v>
+        <v>3.2728434131092915E-2</v>
       </c>
     </row>
     <row r="64" spans="9:12" x14ac:dyDescent="0.3">
@@ -4185,15 +4408,15 @@
       </c>
       <c r="J64" s="8">
         <f ca="1"/>
-        <v>0.32313040685963279</v>
+        <v>0.61829312960625149</v>
       </c>
       <c r="K64" s="8">
         <f ca="1"/>
-        <v>0.45426058335387542</v>
+        <v>0.57071153006039466</v>
       </c>
       <c r="L64" s="8">
         <f ca="1"/>
-        <v>6.2600029550166386E-2</v>
+        <v>3.0766145852128359E-2</v>
       </c>
     </row>
     <row r="65" spans="9:12" x14ac:dyDescent="0.3">
@@ -4202,15 +4425,15 @@
       </c>
       <c r="J65" s="8">
         <f ca="1"/>
-        <v>0.32313040685963279</v>
+        <v>0.61829312960625149</v>
       </c>
       <c r="K65" s="8">
         <f ca="1"/>
-        <v>0.45214558050719411</v>
+        <v>0.57147897521436009</v>
       </c>
       <c r="L65" s="8">
         <f ca="1"/>
-        <v>6.0609562306681686E-2</v>
+        <v>2.8921509745761961E-2</v>
       </c>
     </row>
     <row r="66" spans="9:12" x14ac:dyDescent="0.3">
@@ -4219,15 +4442,15 @@
       </c>
       <c r="J66" s="8">
         <f ca="1"/>
-        <v>0.32313040685963279</v>
+        <v>0.61829312960625149</v>
       </c>
       <c r="K66" s="8">
         <f ca="1"/>
-        <v>0.45009772060802644</v>
+        <v>0.57222205703010443</v>
       </c>
       <c r="L66" s="8">
         <f ca="1"/>
-        <v>5.868238708699957E-2</v>
+        <v>2.7187471734633942E-2</v>
       </c>
     </row>
     <row r="67" spans="9:12" x14ac:dyDescent="0.3">
@@ -4236,15 +4459,15 @@
       </c>
       <c r="J67" s="8">
         <f ca="1"/>
-        <v>0.32313040685963279</v>
+        <v>0.61829312960625149</v>
       </c>
       <c r="K67" s="8">
         <f ca="1"/>
-        <v>0.44811385633070783</v>
+        <v>0.57294191753910673</v>
       </c>
       <c r="L67" s="8">
         <f ca="1"/>
-        <v>5.6816489372611023E-2</v>
+        <v>2.5557400662959123E-2</v>
       </c>
     </row>
     <row r="68" spans="9:12" x14ac:dyDescent="0.3">
@@ -4253,15 +4476,15 @@
       </c>
       <c r="J68" s="8">
         <f ca="1"/>
-        <v>0.32313040685963279</v>
+        <v>0.61829312960625149</v>
       </c>
       <c r="K68" s="8">
         <f ca="1"/>
-        <v>0.44619103403115284</v>
+        <v>0.57363962849398586</v>
       </c>
       <c r="L68" s="8">
         <f ca="1"/>
-        <v>5.5009920744988366E-2</v>
+        <v>2.402506627044388E-2</v>
       </c>
     </row>
     <row r="69" spans="9:12" x14ac:dyDescent="0.3">
@@ -4270,15 +4493,15 @@
       </c>
       <c r="J69" s="8">
         <f ca="1"/>
-        <v>0.32313040685963279</v>
+        <v>0.61829312960625149</v>
       </c>
       <c r="K69" s="8">
         <f ca="1"/>
-        <v>0.44432647907400857</v>
+        <v>0.57431619669265654</v>
       </c>
       <c r="L69" s="8">
         <f ca="1"/>
-        <v>5.3260794737512759E-2</v>
+        <v>2.2584603453345065E-2</v>
       </c>
     </row>
     <row r="70" spans="9:12" x14ac:dyDescent="0.3">
@@ -4287,15 +4510,15 @@
       </c>
       <c r="J70" s="8">
         <f ca="1"/>
-        <v>0.32313040685963279</v>
+        <v>0.61829312960625149</v>
       </c>
       <c r="K70" s="8">
         <f ca="1"/>
-        <v>0.44251758247379402</v>
+        <v>0.57497256882569536</v>
       </c>
       <c r="L70" s="8">
         <f ca="1"/>
-        <v>5.1567284865411872E-2</v>
+        <v>2.1230506099585125E-2</v>
       </c>
     </row>
     <row r="71" spans="9:12" x14ac:dyDescent="0.3">
@@ -4304,15 +4527,15 @@
       </c>
       <c r="J71" s="8">
         <f ca="1"/>
-        <v>0.32313040685963279</v>
+        <v>0.61829312960625149</v>
       </c>
       <c r="K71" s="8">
         <f ca="1"/>
-        <v>0.44076188871476224</v>
+        <v>0.57560963589599767</v>
       </c>
       <c r="L71" s="8">
         <f ca="1"/>
-        <v>4.9927622718288038E-2</v>
+        <v>1.9957596065397831E-2</v>
       </c>
     </row>
     <row r="72" spans="9:12" x14ac:dyDescent="0.3">
@@ -4321,15 +4544,15 @@
       </c>
       <c r="J72" s="8">
         <f ca="1"/>
-        <v>0.32313040685963279</v>
+        <v>0.61829312960625149</v>
       </c>
       <c r="K72" s="8">
         <f ca="1"/>
-        <v>0.43905708462990528</v>
+        <v>0.5762282372541172</v>
       </c>
       <c r="L72" s="8">
         <f ca="1"/>
-        <v>4.8340096113260816E-2</v>
+        <v>1.8761005687217357E-2</v>
       </c>
     </row>
     <row r="73" spans="9:12" x14ac:dyDescent="0.3">
@@ -4338,15 +4561,15 @@
       </c>
       <c r="J73" s="8">
         <f ca="1"/>
-        <v>0.32313040685963279</v>
+        <v>0.61829312960625149</v>
       </c>
       <c r="K73" s="8">
         <f ca="1"/>
-        <v>0.43740098923318715</v>
+        <v>0.57682916428771924</v>
       </c>
       <c r="L73" s="8">
         <f ca="1"/>
-        <v>4.680304730677614E-2</v>
+        <v>1.7636155792487687E-2</v>
       </c>
     </row>
     <row r="74" spans="9:12" x14ac:dyDescent="0.3">
@@ -4355,15 +4578,15 @@
       </c>
       <c r="J74" s="8">
         <f ca="1"/>
-        <v>0.50982090706683314</v>
+        <v>0.55649330279809406</v>
       </c>
       <c r="K74" s="8">
         <f ca="1"/>
-        <v>0.43842098807591462</v>
+        <v>0.57654274370335823</v>
       </c>
       <c r="L74" s="8">
         <f ca="1"/>
-        <v>4.44767362862575E-2</v>
+        <v>1.6681523972949881E-2</v>
       </c>
     </row>
     <row r="75" spans="9:12" x14ac:dyDescent="0.3">
@@ -4372,15 +4595,15 @@
       </c>
       <c r="J75" s="8">
         <f ca="1"/>
-        <v>0.50982090706683314</v>
+        <v>0.55649330279809406</v>
       </c>
       <c r="K75" s="8">
         <f ca="1"/>
-        <v>0.43941265361745507</v>
+        <v>0.57626427924634072</v>
       </c>
       <c r="L75" s="8">
         <f ca="1"/>
-        <v>4.2266050952454406E-2</v>
+        <v>1.5778565563548806E-2</v>
       </c>
     </row>
     <row r="76" spans="9:12" x14ac:dyDescent="0.3">
@@ -4389,15 +4612,15 @@
       </c>
       <c r="J76" s="8">
         <f ca="1"/>
-        <v>0.50982090706683314</v>
+        <v>0.55649330279809406</v>
       </c>
       <c r="K76" s="8">
         <f ca="1"/>
-        <v>0.44037715024004931</v>
+        <v>0.57599344395252916</v>
       </c>
       <c r="L76" s="8">
         <f ca="1"/>
-        <v>4.0165246275939905E-2</v>
+        <v>1.4924483494859761E-2</v>
       </c>
     </row>
     <row r="77" spans="9:12" x14ac:dyDescent="0.3">
@@ -4406,15 +4629,15 @@
       </c>
       <c r="J77" s="8">
         <f ca="1"/>
-        <v>0.50982090706683314</v>
+        <v>0.55649330279809406</v>
       </c>
       <c r="K77" s="8">
         <f ca="1"/>
-        <v>0.44131557938635724</v>
+        <v>0.57572992853152327</v>
       </c>
       <c r="L77" s="8">
         <f ca="1"/>
-        <v>3.8168860738178455E-2</v>
+        <v>1.4116632091803711E-2</v>
       </c>
     </row>
     <row r="78" spans="9:12" x14ac:dyDescent="0.3">
@@ -4423,15 +4646,15 @@
       </c>
       <c r="J78" s="8">
         <f ca="1"/>
-        <v>0.50982090706683314</v>
+        <v>0.55649330279809406</v>
       </c>
       <c r="K78" s="8">
         <f ca="1"/>
-        <v>0.44222898375543024</v>
+        <v>0.57547344018841085</v>
       </c>
       <c r="L78" s="8">
         <f ca="1"/>
-        <v>3.6271704289492272E-2</v>
+        <v>1.335251169039541E-2</v>
       </c>
     </row>
     <row r="79" spans="9:12" x14ac:dyDescent="0.3">
@@ -4440,15 +4663,15 @@
       </c>
       <c r="J79" s="8">
         <f ca="1"/>
-        <v>0.50982090706683314</v>
+        <v>0.55649330279809406</v>
       </c>
       <c r="K79" s="8">
         <f ca="1"/>
-        <v>0.44311835116742238</v>
+        <v>0.57522370153853819</v>
       </c>
       <c r="L79" s="8">
         <f ca="1"/>
-        <v>3.4468844858290083E-2</v>
+        <v>1.2629750638982456E-2</v>
       </c>
     </row>
     <row r="80" spans="9:12" x14ac:dyDescent="0.3">
@@ -4457,15 +4680,15 @@
       </c>
       <c r="J80" s="8">
         <f ca="1"/>
-        <v>0.50982090706683314</v>
+        <v>0.55649330279809406</v>
       </c>
       <c r="K80" s="8">
         <f ca="1"/>
-        <v>0.44398461812715501</v>
+        <v>0.57498044960684425</v>
       </c>
       <c r="L80" s="8">
         <f ca="1"/>
-        <v>3.2755592349617238E-2</v>
+        <v>1.1946112153477129E-2</v>
       </c>
     </row>
     <row r="81" spans="9:12" x14ac:dyDescent="0.3">
@@ -4474,15 +4697,15 @@
       </c>
       <c r="J81" s="8">
         <f ca="1"/>
-        <v>0.50982090706683314</v>
+        <v>0.55649330279809406</v>
       </c>
       <c r="K81" s="8">
         <f ca="1"/>
-        <v>0.44482867311356111</v>
+        <v>0.5747434349041679</v>
       </c>
       <c r="L81" s="8">
         <f ca="1"/>
-        <v>3.112749803119012E-2</v>
+        <v>1.1299478580885595E-2</v>
       </c>
     </row>
     <row r="82" spans="9:12" x14ac:dyDescent="0.3">
@@ -4491,15 +4714,15 @@
       </c>
       <c r="J82" s="8">
         <f ca="1"/>
-        <v>0.50982090706683314</v>
+        <v>0.55649330279809406</v>
       </c>
       <c r="K82" s="8">
         <f ca="1"/>
-        <v>0.44565135961929875</v>
+        <v>0.57451242057371132</v>
       </c>
       <c r="L82" s="8">
         <f ca="1"/>
-        <v>2.9580326951149597E-2</v>
+        <v>1.0687846901998289E-2</v>
       </c>
     </row>
     <row r="83" spans="9:12" x14ac:dyDescent="0.3">
@@ -4508,15 +4731,15 @@
       </c>
       <c r="J83" s="8">
         <f ca="1"/>
-        <v>0.50982090706683314</v>
+        <v>0.55649330279809406</v>
       </c>
       <c r="K83" s="8">
         <f ca="1"/>
-        <v>0.4464534789623929</v>
+        <v>0.57428718160151604</v>
       </c>
       <c r="L83" s="8">
         <f ca="1"/>
-        <v>2.8110056853004491E-2</v>
+        <v>1.0109322528408444E-2</v>
       </c>
     </row>
     <row r="84" spans="9:12" x14ac:dyDescent="0.3">
@@ -4525,15 +4748,15 @@
       </c>
       <c r="J84" s="8">
         <f ca="1"/>
-        <v>0.39874822970447998</v>
+        <v>0.35531318939366341</v>
       </c>
       <c r="K84" s="8">
         <f ca="1"/>
-        <v>0.44586452526785081</v>
+        <v>0.571583798981666</v>
       </c>
       <c r="L84" s="8">
         <f ca="1"/>
-        <v>2.7011226380325128E-2</v>
+        <v>9.7564291090904299E-3</v>
       </c>
     </row>
     <row r="85" spans="9:12" x14ac:dyDescent="0.3">
@@ -4542,15 +4765,15 @@
       </c>
       <c r="J85" s="8">
         <f ca="1"/>
-        <v>0.39874822970447998</v>
+        <v>0.35531318939366341</v>
       </c>
       <c r="K85" s="8">
         <f ca="1"/>
-        <v>0.44528993629756575</v>
+        <v>0.56894635252327574</v>
       </c>
       <c r="L85" s="8">
         <f ca="1"/>
-        <v>2.5955349411791562E-2</v>
+        <v>9.4158565307181433E-3</v>
       </c>
     </row>
     <row r="86" spans="9:12" x14ac:dyDescent="0.3">
@@ -4559,15 +4782,15 @@
       </c>
       <c r="J86" s="8">
         <f ca="1"/>
-        <v>0.39874822970447998</v>
+        <v>0.35531318939366341</v>
       </c>
       <c r="K86" s="8">
         <f ca="1"/>
-        <v>0.44472919284463702</v>
+        <v>0.56637245899159372</v>
       </c>
       <c r="L86" s="8">
         <f ca="1"/>
-        <v>2.4940749533541081E-2</v>
+        <v>9.087172464200861E-3</v>
       </c>
     </row>
     <row r="87" spans="9:12" x14ac:dyDescent="0.3">
@@ -4576,15 +4799,15 @@
       </c>
       <c r="J87" s="8">
         <f ca="1"/>
-        <v>0.39874822970447998</v>
+        <v>0.35531318939366341</v>
       </c>
       <c r="K87" s="8">
         <f ca="1"/>
-        <v>0.44418180042630184</v>
+        <v>0.56385984863923733</v>
       </c>
       <c r="L87" s="8">
         <f ca="1"/>
-        <v>2.3965808655341352E-2</v>
+        <v>8.7699619068797863E-3</v>
       </c>
     </row>
     <row r="88" spans="9:12" x14ac:dyDescent="0.3">
@@ -4593,15 +4816,15 @@
       </c>
       <c r="J88" s="8">
         <f ca="1"/>
-        <v>0.39874822970447998</v>
+        <v>0.35531318939366341</v>
       </c>
       <c r="K88" s="8">
         <f ca="1"/>
-        <v>0.44364728782957447</v>
+        <v>0.56140635853046594</v>
       </c>
       <c r="L88" s="8">
         <f ca="1"/>
-        <v>2.3028978524761514E-2</v>
+        <v>8.4638243419457478E-3</v>
       </c>
     </row>
     <row r="89" spans="9:12" x14ac:dyDescent="0.3">
@@ -4610,15 +4833,15 @@
       </c>
       <c r="J89" s="8">
         <f ca="1"/>
-        <v>0.39874822970447998</v>
+        <v>0.35531318939366341</v>
       </c>
       <c r="K89" s="8">
         <f ca="1"/>
-        <v>0.44312520575835246</v>
+        <v>0.55900992633120083</v>
       </c>
       <c r="L89" s="8">
         <f ca="1"/>
-        <v>2.2128769389649815E-2</v>
+        <v>8.1683732326001905E-3</v>
       </c>
     </row>
     <row r="90" spans="9:12" x14ac:dyDescent="0.3">
@@ -4627,15 +4850,15 @@
       </c>
       <c r="J90" s="8">
         <f ca="1"/>
-        <v>0.39874822970447998</v>
+        <v>0.35531318939366341</v>
       </c>
       <c r="K90" s="8">
         <f ca="1"/>
-        <v>0.44261512557382515</v>
+        <v>0.55666858452732093</v>
       </c>
       <c r="L90" s="8">
         <f ca="1"/>
-        <v>2.1263749734530272E-2</v>
+        <v>7.8832355338890152E-3</v>
       </c>
     </row>
     <row r="91" spans="9:12" x14ac:dyDescent="0.3">
@@ -4644,15 +4867,15 @@
       </c>
       <c r="J91" s="8">
         <f ca="1"/>
-        <v>0.39874822970447998</v>
+        <v>0.35531318939366341</v>
       </c>
       <c r="K91" s="8">
         <f ca="1"/>
-        <v>0.44211663812076446</v>
+        <v>0.55438045503716571</v>
       </c>
       <c r="L91" s="8">
         <f ca="1"/>
-        <v>2.0432544004520912E-2</v>
+        <v>7.608051221513124E-3</v>
       </c>
     </row>
     <row r="92" spans="9:12" x14ac:dyDescent="0.3">
@@ -4661,15 +4884,15 @@
       </c>
       <c r="J92" s="8">
         <f ca="1"/>
-        <v>0.39874822970447998</v>
+        <v>0.35531318939366341</v>
       </c>
       <c r="K92" s="8">
         <f ca="1"/>
-        <v>0.44162935263294106</v>
+        <v>0.55214374418723877</v>
       </c>
       <c r="L92" s="8">
         <f ca="1"/>
-        <v>1.9633830418309038E-2</v>
+        <v>7.3424728370593906E-3</v>
       </c>
     </row>
     <row r="93" spans="9:12" x14ac:dyDescent="0.3">
@@ -4678,15 +4901,15 @@
       </c>
       <c r="J93" s="8">
         <f ca="1"/>
-        <v>0.39874822970447998</v>
+        <v>0.35531318939366341</v>
       </c>
       <c r="K93" s="8">
         <f ca="1"/>
-        <v>0.44115289571151373</v>
+        <v>0.54995673802286571</v>
       </c>
       <c r="L93" s="8">
         <f ca="1"/>
-        <v>1.8866338866720699E-2</v>
+        <v>7.0861678884948463E-3</v>
       </c>
     </row>
     <row r="94" spans="9:12" x14ac:dyDescent="0.3">
@@ -4695,15 +4918,15 @@
       </c>
       <c r="J94" s="8">
         <f ca="1"/>
-        <v>0.88005095914214659</v>
+        <v>0.33946532617874281</v>
       </c>
       <c r="K94" s="8">
         <f ca="1"/>
-        <v>0.44597595135360857</v>
+        <v>0.54764364558501821</v>
       </c>
       <c r="L94" s="8">
         <f ca="1"/>
-        <v>1.7276964625548504E-2</v>
+        <v>6.8496542851597111E-3</v>
       </c>
     </row>
     <row r="95" spans="9:12" x14ac:dyDescent="0.3">
@@ -4712,15 +4935,15 @@
       </c>
       <c r="J95" s="8">
         <f ca="1"/>
-        <v>0.88005095914214659</v>
+        <v>0.33946532617874281</v>
       </c>
       <c r="K95" s="8">
         <f ca="1"/>
-        <v>0.45069415796000578</v>
+        <v>0.54538083776538482</v>
       </c>
       <c r="L95" s="8">
         <f ca="1"/>
-        <v>1.5821487231890467E-2</v>
+        <v>6.6210347724593053E-3</v>
       </c>
     </row>
     <row r="96" spans="9:12" x14ac:dyDescent="0.3">
@@ -4729,15 +4952,15 @@
       </c>
       <c r="J96" s="8">
         <f ca="1"/>
-        <v>0.88005095914214659</v>
+        <v>0.33946532617874281</v>
       </c>
       <c r="K96" s="8">
         <f ca="1"/>
-        <v>0.4553108977576632</v>
+        <v>0.543166692479507</v>
       </c>
       <c r="L96" s="8">
         <f ca="1"/>
-        <v>1.4488624508776545E-2</v>
+        <v>6.4000458745178948E-3</v>
       </c>
     </row>
     <row r="97" spans="9:12" x14ac:dyDescent="0.3">
@@ -4746,15 +4969,15 @@
       </c>
       <c r="J97" s="8">
         <f ca="1"/>
-        <v>0.88005095914214659</v>
+        <v>0.33946532617874281</v>
       </c>
       <c r="K97" s="8">
         <f ca="1"/>
-        <v>0.45982940904898745</v>
+        <v>0.54099965666779659</v>
       </c>
       <c r="L97" s="8">
         <f ca="1"/>
-        <v>1.3268049693872143E-2</v>
+        <v>6.186432910099079E-3</v>
       </c>
     </row>
     <row r="98" spans="9:12" x14ac:dyDescent="0.3">
@@ -4763,15 +4986,15 @@
       </c>
       <c r="J98" s="8">
         <f ca="1"/>
-        <v>0.88005095914214659</v>
+        <v>0.33946532617874281</v>
       </c>
       <c r="K98" s="8">
         <f ca="1"/>
-        <v>0.46425279378681017</v>
+        <v>0.53887824266264872</v>
       </c>
       <c r="L98" s="8">
         <f ca="1"/>
-        <v>1.2150299220262418E-2</v>
+        <v>5.979949699183743E-3</v>
       </c>
     </row>
     <row r="99" spans="9:12" x14ac:dyDescent="0.3">
@@ -4780,15 +5003,15 @@
       </c>
       <c r="J99" s="8">
         <f ca="1"/>
-        <v>0.88005095914214659</v>
+        <v>0.33946532617874281</v>
       </c>
       <c r="K99" s="8">
         <f ca="1"/>
-        <v>0.4685840246759283</v>
+        <v>0.53680102478260805</v>
       </c>
       <c r="L99" s="8">
         <f ca="1"/>
-        <v>1.1126712477372807E-2</v>
+        <v>5.7803582793450863E-3</v>
       </c>
     </row>
     <row r="100" spans="9:12" x14ac:dyDescent="0.3">
@@ -4797,15 +5020,15 @@
       </c>
       <c r="J100" s="8">
         <f ca="1"/>
-        <v>0.88005095914214659</v>
+        <v>0.33946532617874281</v>
       </c>
       <c r="K100" s="8">
         <f ca="1"/>
-        <v>0.47282595183537385</v>
+        <v>0.53476663613720743</v>
       </c>
       <c r="L100" s="8">
         <f ca="1"/>
-        <v>1.0189356867418529E-2</v>
+        <v>5.587428631620513E-3</v>
       </c>
     </row>
     <row r="101" spans="9:12" x14ac:dyDescent="0.3">
@@ -4814,15 +5037,15 @@
       </c>
       <c r="J101" s="8">
         <f ca="1"/>
-        <v>0.88005095914214659</v>
+        <v>0.33946532617874281</v>
       </c>
       <c r="K101" s="8">
         <f ca="1"/>
-        <v>0.47698130905278985</v>
+        <v>0.53277376562742707</v>
       </c>
       <c r="L101" s="8">
         <f ca="1"/>
-        <v>9.3309645557251228E-3</v>
+        <v>5.4009384155712971E-3</v>
       </c>
     </row>
     <row r="102" spans="9:12" x14ac:dyDescent="0.3">
@@ -4831,15 +5054,15 @@
       </c>
       <c r="J102" s="8">
         <f ca="1"/>
-        <v>0.88005095914214659</v>
+        <v>0.33946532617874281</v>
       </c>
       <c r="K102" s="8">
         <f ca="1"/>
-        <v>0.4810527196597531</v>
+        <v>0.53082115512794548</v>
       </c>
       <c r="L102" s="8">
         <f ca="1"/>
-        <v>8.5448883534588894E-3</v>
+        <v>5.2206727131716311E-3</v>
       </c>
     </row>
     <row r="103" spans="9:12" x14ac:dyDescent="0.3">
@@ -4848,15 +5071,15 @@
       </c>
       <c r="J103" s="8">
         <f ca="1"/>
-        <v>0.88005095914214659</v>
+        <v>0.33946532617874281</v>
       </c>
       <c r="K103" s="8">
         <f ca="1"/>
-        <v>0.485042702054577</v>
+        <v>0.52890759683845334</v>
       </c>
       <c r="L103" s="8">
         <f ca="1"/>
-        <v>7.8250339639814193E-3</v>
+        <v>5.046420660467895E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bond::fix -> bond::instrument pwflat::constant
</commit_message>
<xml_diff>
--- a/bondxll.xlsx
+++ b/bondxll.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\source\repos\tmcrossx\bondxll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keith\source\repos\tmcrossx\bondxll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BEC00D-B485-4F8D-BD31-B9EA3821BF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1102A441-0447-4F0F-A0E1-78EDB03CCACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="1665" windowWidth="32415" windowHeight="17685" activeTab="3" xr2:uid="{B41655E8-20ED-4B49-A343-A4ADF5D922ED}"/>
+    <workbookView xWindow="2088" yWindow="1068" windowWidth="19716" windowHeight="11892" activeTab="4" xr2:uid="{B41655E8-20ED-4B49-A343-A4ADF5D922ED}"/>
   </bookViews>
   <sheets>
     <sheet name="ENUM" sheetId="1" r:id="rId1"/>
     <sheet name="INSTRUMENT" sheetId="3" r:id="rId2"/>
     <sheet name="PWFLAT" sheetId="2" r:id="rId3"/>
     <sheet name="BOND" sheetId="4" r:id="rId4"/>
+    <sheet name="VALUATION" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="bond">VALUATION!$C$3</definedName>
     <definedName name="bond_basic">BOND!$C$8</definedName>
     <definedName name="coupon">BOND!$C$4</definedName>
     <definedName name="date">ENUM!$E$3</definedName>
@@ -30,6 +32,7 @@
     <definedName name="face">BOND!$C$7</definedName>
     <definedName name="frequency">BOND!$C$5</definedName>
     <definedName name="maturity">BOND!$C$3</definedName>
+    <definedName name="pvdate" localSheetId="4">VALUATION!$C$2</definedName>
     <definedName name="pvdate">BOND!$C$9</definedName>
     <definedName name="pwflat">PWFLAT!$F$2</definedName>
     <definedName name="rate">PWFLAT!$C$3:$C$12</definedName>
@@ -78,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>TMX_DAY_COUNT_ENUM</t>
   </si>
@@ -102,9 +105,6 @@
   </si>
   <si>
     <t>FREQUENCY</t>
-  </si>
-  <si>
-    <t>TMX_FREQUENCY_QUARTERLY</t>
   </si>
   <si>
     <t>time</t>
@@ -171,6 +171,18 @@
   </si>
   <si>
     <t>FREQ_ANNUAL</t>
+  </si>
+  <si>
+    <t>TMX_FREQUENCY_SEMIANNUALLY</t>
+  </si>
+  <si>
+    <t>bond</t>
+  </si>
+  <si>
+    <t>curve</t>
+  </si>
+  <si>
+    <t>=\TMX.CURVE.CONSTANT(H2)</t>
   </si>
 </sst>
 </file>
@@ -354,7 +366,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -395,6 +407,10 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -810,307 +826,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.97521185509924591</c:v>
+                  <c:v>8.9383682239568829E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.97521185509924591</c:v>
+                  <c:v>8.9383682239568829E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.97521185509924591</c:v>
+                  <c:v>8.9383682239568829E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.97521185509924591</c:v>
+                  <c:v>8.9383682239568829E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.97521185509924591</c:v>
+                  <c:v>8.9383682239568829E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.97521185509924591</c:v>
+                  <c:v>8.9383682239568829E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.97521185509924591</c:v>
+                  <c:v>8.9383682239568829E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.97521185509924591</c:v>
+                  <c:v>8.9383682239568829E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.97521185509924591</c:v>
+                  <c:v>8.9383682239568829E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.97521185509924591</c:v>
+                  <c:v>8.9383682239568829E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.99691947434149752</c:v>
+                  <c:v>0.9098121920374147</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.99691947434149752</c:v>
+                  <c:v>0.9098121920374147</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.99691947434149752</c:v>
+                  <c:v>0.9098121920374147</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.99691947434149752</c:v>
+                  <c:v>0.9098121920374147</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.99691947434149752</c:v>
+                  <c:v>0.9098121920374147</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.99691947434149752</c:v>
+                  <c:v>0.9098121920374147</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.99691947434149752</c:v>
+                  <c:v>0.9098121920374147</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.99691947434149752</c:v>
+                  <c:v>0.9098121920374147</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.99691947434149752</c:v>
+                  <c:v>0.9098121920374147</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.99691947434149752</c:v>
+                  <c:v>0.9098121920374147</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.54672864773213004</c:v>
+                  <c:v>0.10261778272441902</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.54672864773213004</c:v>
+                  <c:v>0.10261778272441902</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.54672864773213004</c:v>
+                  <c:v>0.10261778272441902</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.54672864773213004</c:v>
+                  <c:v>0.10261778272441902</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.54672864773213004</c:v>
+                  <c:v>0.10261778272441902</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.54672864773213004</c:v>
+                  <c:v>0.10261778272441902</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.54672864773213004</c:v>
+                  <c:v>0.10261778272441902</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.54672864773213004</c:v>
+                  <c:v>0.10261778272441902</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.54672864773213004</c:v>
+                  <c:v>0.10261778272441902</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.54672864773213004</c:v>
+                  <c:v>0.10261778272441902</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.83770297712941599</c:v>
+                  <c:v>0.21567196970698377</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.83770297712941599</c:v>
+                  <c:v>0.21567196970698377</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.83770297712941599</c:v>
+                  <c:v>0.21567196970698377</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.83770297712941599</c:v>
+                  <c:v>0.21567196970698377</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.83770297712941599</c:v>
+                  <c:v>0.21567196970698377</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.83770297712941599</c:v>
+                  <c:v>0.21567196970698377</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.83770297712941599</c:v>
+                  <c:v>0.21567196970698377</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.83770297712941599</c:v>
+                  <c:v>0.21567196970698377</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.83770297712941599</c:v>
+                  <c:v>0.21567196970698377</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.83770297712941599</c:v>
+                  <c:v>0.21567196970698377</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.69707891184125215</c:v>
+                  <c:v>0.70240536737706383</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.69707891184125215</c:v>
+                  <c:v>0.70240536737706383</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.69707891184125215</c:v>
+                  <c:v>0.70240536737706383</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.69707891184125215</c:v>
+                  <c:v>0.70240536737706383</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.69707891184125215</c:v>
+                  <c:v>0.70240536737706383</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.69707891184125215</c:v>
+                  <c:v>0.70240536737706383</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.69707891184125215</c:v>
+                  <c:v>0.70240536737706383</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.69707891184125215</c:v>
+                  <c:v>0.70240536737706383</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.69707891184125215</c:v>
+                  <c:v>0.70240536737706383</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.69707891184125215</c:v>
+                  <c:v>0.70240536737706383</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>7.8071604142182061E-2</c:v>
+                  <c:v>5.409639036802627E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>7.8071604142182061E-2</c:v>
+                  <c:v>5.409639036802627E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>7.8071604142182061E-2</c:v>
+                  <c:v>5.409639036802627E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>7.8071604142182061E-2</c:v>
+                  <c:v>5.409639036802627E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>7.8071604142182061E-2</c:v>
+                  <c:v>5.409639036802627E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>7.8071604142182061E-2</c:v>
+                  <c:v>5.409639036802627E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>7.8071604142182061E-2</c:v>
+                  <c:v>5.409639036802627E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>7.8071604142182061E-2</c:v>
+                  <c:v>5.409639036802627E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>7.8071604142182061E-2</c:v>
+                  <c:v>5.409639036802627E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>7.8071604142182061E-2</c:v>
+                  <c:v>5.409639036802627E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.80925543441441206</c:v>
+                  <c:v>0.73487589397700526</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.80925543441441206</c:v>
+                  <c:v>0.73487589397700526</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.80925543441441206</c:v>
+                  <c:v>0.73487589397700526</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.80925543441441206</c:v>
+                  <c:v>0.73487589397700526</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.80925543441441206</c:v>
+                  <c:v>0.73487589397700526</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.80925543441441206</c:v>
+                  <c:v>0.73487589397700526</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.80925543441441206</c:v>
+                  <c:v>0.73487589397700526</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.80925543441441206</c:v>
+                  <c:v>0.73487589397700526</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.80925543441441206</c:v>
+                  <c:v>0.73487589397700526</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.80925543441441206</c:v>
+                  <c:v>0.73487589397700526</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.20186189379151176</c:v>
+                  <c:v>0.1314634821513172</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.20186189379151176</c:v>
+                  <c:v>0.1314634821513172</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.20186189379151176</c:v>
+                  <c:v>0.1314634821513172</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.20186189379151176</c:v>
+                  <c:v>0.1314634821513172</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.20186189379151176</c:v>
+                  <c:v>0.1314634821513172</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.20186189379151176</c:v>
+                  <c:v>0.1314634821513172</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.20186189379151176</c:v>
+                  <c:v>0.1314634821513172</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.20186189379151176</c:v>
+                  <c:v>0.1314634821513172</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.20186189379151176</c:v>
+                  <c:v>0.1314634821513172</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.20186189379151176</c:v>
+                  <c:v>0.1314634821513172</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.44387199209227735</c:v>
+                  <c:v>0.40066932382155351</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.44387199209227735</c:v>
+                  <c:v>0.40066932382155351</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.44387199209227735</c:v>
+                  <c:v>0.40066932382155351</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.44387199209227735</c:v>
+                  <c:v>0.40066932382155351</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.44387199209227735</c:v>
+                  <c:v>0.40066932382155351</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.44387199209227735</c:v>
+                  <c:v>0.40066932382155351</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.44387199209227735</c:v>
+                  <c:v>0.40066932382155351</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.44387199209227735</c:v>
+                  <c:v>0.40066932382155351</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.44387199209227735</c:v>
+                  <c:v>0.40066932382155351</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.44387199209227735</c:v>
+                  <c:v>0.40066932382155351</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1467,307 +1483,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677778</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677778</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677778</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677756</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677778</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.60389744283288471</c:v>
+                  <c:v>0.94726356375677767</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.63765329849346308</c:v>
+                  <c:v>0.86927448361884951</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.66578317821061161</c:v>
+                  <c:v>0.80428358350390938</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.68958538412512194</c:v>
+                  <c:v>0.74929128340665252</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.70998727490898794</c:v>
+                  <c:v>0.70215502618043224</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.72766891358833841</c:v>
+                  <c:v>0.66130360325104143</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.74314034743277024</c:v>
+                  <c:v>0.62555860818782427</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.7567916125896218</c:v>
+                  <c:v>0.5940189066614564</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.76892607050682293</c:v>
+                  <c:v>0.56598361641579598</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.77978321706431897</c:v>
+                  <c:v>0.54089940935388925</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.78955464896606531</c:v>
+                  <c:v>0.51832362299817325</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.79942916446013346</c:v>
+                  <c:v>0.53696593580956575</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.80840599672746827</c:v>
+                  <c:v>0.55391349291083158</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.81660223488459993</c:v>
+                  <c:v>0.56938734939459601</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.82411545319530399</c:v>
+                  <c:v>0.58357171783804684</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.83102761404115166</c:v>
+                  <c:v>0.59662133680602147</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.83740807020654962</c:v>
+                  <c:v>0.60866713893030588</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.84331589998932543</c:v>
+                  <c:v>0.61982065941575437</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.84880174193047453</c:v>
+                  <c:v>0.63017749986652793</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.85390924994464779</c:v>
+                  <c:v>0.63982007545862751</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.85867625742454268</c:v>
+                  <c:v>0.64881981267792044</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.84861343130543265</c:v>
+                  <c:v>0.63120039235683967</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.83917953181876692</c:v>
+                  <c:v>0.61468218580582656</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.83031738381614162</c:v>
+                  <c:v>0.59916508268214752</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.8219765386372001</c:v>
+                  <c:v>0.58456075033044963</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.81411231318276944</c:v>
+                  <c:v>0.57079095125599166</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.80668498914247388</c:v>
+                  <c:v>0.55778614101900348</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.79965914207732947</c:v>
+                  <c:v>0.54548429349752825</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.79300307643666634</c:v>
+                  <c:v>0.53382991163507798</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.78668834749552441</c:v>
+                  <c:v>0.52277319038095849</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.78068935500143954</c:v>
+                  <c:v>0.51226930518954505</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.78207993115090246</c:v>
+                  <c:v>0.50503522383631183</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.78340428938848605</c:v>
+                  <c:v>0.49814562254751826</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.78466704956850775</c:v>
+                  <c:v>0.49157646783029663</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.78587241155852827</c:v>
+                  <c:v>0.48530591105476678</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.78702420190454803</c:v>
+                  <c:v>0.47931404569148267</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.78812591440943647</c:v>
+                  <c:v>0.47358269621355875</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.78918074553113815</c:v>
+                  <c:v>0.4680952339474615</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.79019162535610221</c:v>
+                  <c:v>0.46283641594245151</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.79116124478004746</c:v>
+                  <c:v>0.45779224357029907</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.79209207942703475</c:v>
+                  <c:v>0.45294983809303274</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.7902290761410391</c:v>
+                  <c:v>0.45784112298095497</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.78843772682758162</c:v>
+                  <c:v>0.46254428152703392</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.78671397560142453</c:v>
+                  <c:v>0.46706996239212883</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.78505406701327318</c:v>
+                  <c:v>0.47142802544740547</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.78345451873741823</c:v>
+                  <c:v>0.47562761348249011</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.78191209718570087</c:v>
+                  <c:v>0.47967721623060749</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.78042379568843001</c:v>
+                  <c:v>0.48358472765422961</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.77898681493244404</c:v>
+                  <c:v>0.4873574973046233</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.77759854538852546</c:v>
+                  <c:v>0.49100237645839345</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.77625655149607109</c:v>
+                  <c:v>0.49452575964037121</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.7648108966214171</c:v>
+                  <c:v>0.48730560604574263</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.75373445642013914</c:v>
+                  <c:v>0.48031836063158589</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.74300964924112389</c:v>
+                  <c:v>0.47355293253216429</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.73261999228645303</c:v>
+                  <c:v>0.46699892406084964</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.72255001708423339</c:v>
+                  <c:v>0.46064657738865239</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.71278519264571749</c:v>
+                  <c:v>0.45448672607015805</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.70331185550387376</c:v>
+                  <c:v>0.44851075091042469</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.69411714592502527</c:v>
+                  <c:v>0.44271053972597768</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.68518894966730293</c:v>
+                  <c:v>0.4370784506048479</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.67651584473122983</c:v>
+                  <c:v>0.43160727831575052</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.67838541641690842</c:v>
+                  <c:v>0.43587866726872598</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.68020305555576266</c:v>
+                  <c:v>0.44003140652856315</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.68197089636204555</c:v>
+                  <c:v>0.44407037211004868</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.68369095768707755</c:v>
+                  <c:v>0.44800017645960216</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.68536515071010862</c:v>
+                  <c:v>0.45182518602650085</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.68699528602200743</c:v>
+                  <c:v>0.45554953744690224</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.68858308015697367</c:v>
+                  <c:v>0.45917715246677371</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.69013016162181262</c:v>
+                  <c:v>0.46271175171690487</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.69163807646728859</c:v>
+                  <c:v>0.46615686744171625</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.69310829344162761</c:v>
+                  <c:v>0.46951585527340733</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.68704352307557681</c:v>
+                  <c:v>0.46534236918548033</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.68112667393796622</c:v>
+                  <c:v>0.46127067544116118</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.67535239947837045</c:v>
+                  <c:v>0.4572970947991149</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.66971560774400307</c:v>
+                  <c:v>0.45341812321997443</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.66421144640338547</c:v>
+                  <c:v>0.44963042156034322</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.6588352888148753</c:v>
+                  <c:v>0.44593080598581969</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.65358272105598603</c:v>
+                  <c:v>0.44231623904519313</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.6484495298370716</c:v>
+                  <c:v>0.43878382135321731</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.64343169122981814</c:v>
+                  <c:v>0.43533078383409485</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.63852536014717032</c:v>
+                  <c:v>0.43195448048206397</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.63638631214656705</c:v>
+                  <c:v>0.43161068755172871</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.63429376518945524</c:v>
+                  <c:v>0.43127436838074856</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.63224621924217372</c:v>
+                  <c:v>0.43094528188011205</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.63024223810228119</c:v>
+                  <c:v>0.4306231972199146</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.628280446039018</c:v>
+                  <c:v>0.43030789328940555</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.62635952464373945</c:v>
+                  <c:v>0.42999915819078205</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.62447820987516767</c:v>
+                  <c:v>0.42969678876429512</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.62263528928554635</c:v>
+                  <c:v>0.42940059014243048</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.62082959941490734</c:v>
+                  <c:v>0.42911037533110846</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.61906002334168098</c:v>
+                  <c:v>0.42882596481601293</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2915,28 +2931,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1158A502-D294-49DE-A9D7-C71F5820CCB0}">
-  <dimension ref="B2:K5"/>
+  <dimension ref="B2:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2953,17 +2969,17 @@
         <v>7</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1" cm="1">
         <f t="array" ref="K2">_xll.ENUM(J2)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" cm="1">
-        <f t="array" ref="B3">TRANSPOSE(_xll.ENUM(B2))</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="str" cm="1">
+        <f t="array" ref="B3:B7">TRANSPOSE(_xll.ENUM(B2))</f>
+        <v>TMX_DAY_COUNT_30_360</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
@@ -2972,26 +2988,51 @@
         <f ca="1">TODAY()</f>
         <v>45410</v>
       </c>
-      <c r="G3" s="1" cm="1">
-        <f t="array" ref="G3">TRANSPOSE(_xll.ENUM(G2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="str" cm="1">
+        <f t="array" ref="G3:G6">TRANSPOSE(_xll.ENUM(G2))</f>
+        <v>TMX_FREQUENCY_ANNUALLY</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="str">
+        <v>TMX_DAY_COUNT_30E_360</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3">
         <v>180</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G4" s="1" t="str">
+        <v>TMX_FREQUENCY_SEMIANNUALLY</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="str">
+        <v>TMX_DAY_COUNT_ACTUAL_ACTUAL</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="5" cm="1">
         <f t="array" aca="1" ref="E5" ca="1">_xll.TMX.DATE.DAY_COUNT(date,date+days,_xll.ENUM(DAY_COUNT))</f>
         <v>0.5</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <v>TMX_FREQUENCY_QUARTERLY</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="str">
+        <v>TMX_DAY_COUNT_ACTUAL_360</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <v>TMX_FREQUENCY_MONTHLY</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="str">
+        <v>TMX_DAY_COUNT_ACTUAL_365</v>
       </c>
     </row>
   </sheetData>
@@ -3012,39 +3053,39 @@
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="13" customWidth="1"/>
-    <col min="2" max="3" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="13"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="15">
         <v>10</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="11" cm="1">
         <f t="array" aca="1" ref="E2" ca="1">_xll.\TMX.INSTRUMENT(_xlfn.ANCHORARRAY(B3),_xlfn.ANCHORARRAY(C3))</f>
-        <v>2509955565728</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+        <v>2273345525488</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="13" cm="1">
         <f t="array" ref="B3:B12">_xlfn.SEQUENCE(B2,1,1)</f>
         <v>1</v>
       </c>
       <c r="C3" s="13" cm="1">
         <f t="array" aca="1" ref="C3:C12" ca="1">_xlfn.RANDARRAY(B2,1)</f>
-        <v>0.58547007613793456</v>
+        <v>0.41509716066858493</v>
       </c>
       <c r="E3" s="13" cm="1">
         <f t="array" aca="1" ref="E3:F12" ca="1">_xll.TMX.INSTRUMENT(E2)</f>
@@ -3052,16 +3093,16 @@
       </c>
       <c r="F3" s="13">
         <f ca="1"/>
-        <v>0.58547007613793456</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+        <v>0.41509716066858493</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="13">
         <v>2</v>
       </c>
       <c r="C4" s="13">
         <f ca="1"/>
-        <v>0.93914919904214789</v>
+        <v>0.16637080590089415</v>
       </c>
       <c r="E4" s="13">
         <f ca="1"/>
@@ -3069,16 +3110,16 @@
       </c>
       <c r="F4" s="13">
         <f ca="1"/>
-        <v>0.93914919904214789</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+        <v>0.16637080590089415</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="13">
         <v>3</v>
       </c>
       <c r="C5" s="13">
         <f ca="1"/>
-        <v>0.19723773050585791</v>
+        <v>0.18781207533545774</v>
       </c>
       <c r="E5" s="13">
         <f ca="1"/>
@@ -3086,16 +3127,16 @@
       </c>
       <c r="F5" s="13">
         <f ca="1"/>
-        <v>0.19723773050585791</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+        <v>0.18781207533545774</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="13">
         <v>4</v>
       </c>
       <c r="C6" s="13">
         <f ca="1"/>
-        <v>0.74612601940522638</v>
+        <v>0.67965834898291422</v>
       </c>
       <c r="E6" s="13">
         <f ca="1"/>
@@ -3103,16 +3144,16 @@
       </c>
       <c r="F6" s="13">
         <f ca="1"/>
-        <v>0.74612601940522638</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+        <v>0.67965834898291422</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="13">
         <v>5</v>
       </c>
       <c r="C7" s="13">
         <f ca="1"/>
-        <v>0.78639760043122831</v>
+        <v>0.92388142338020862</v>
       </c>
       <c r="E7" s="13">
         <f ca="1"/>
@@ -3120,16 +3161,16 @@
       </c>
       <c r="F7" s="13">
         <f ca="1"/>
-        <v>0.78639760043122831</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+        <v>0.92388142338020862</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="13">
         <v>6</v>
       </c>
       <c r="C8" s="13">
         <f ca="1"/>
-        <v>0.2908851172650484</v>
+        <v>0.30230157701445215</v>
       </c>
       <c r="E8" s="13">
         <f ca="1"/>
@@ -3137,16 +3178,16 @@
       </c>
       <c r="F8" s="13">
         <f ca="1"/>
-        <v>0.2908851172650484</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+        <v>0.30230157701445215</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="13">
         <v>7</v>
       </c>
       <c r="C9" s="13">
         <f ca="1"/>
-        <v>0.21952616443531325</v>
+        <v>0.74482628734007505</v>
       </c>
       <c r="E9" s="13">
         <f ca="1"/>
@@ -3154,16 +3195,16 @@
       </c>
       <c r="F9" s="13">
         <f ca="1"/>
-        <v>0.21952616443531325</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+        <v>0.74482628734007505</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="13">
         <v>8</v>
       </c>
       <c r="C10" s="13">
         <f ca="1"/>
-        <v>0.99522796275776315</v>
+        <v>0.56900910389977644</v>
       </c>
       <c r="E10" s="13">
         <f ca="1"/>
@@ -3171,16 +3212,16 @@
       </c>
       <c r="F10" s="13">
         <f ca="1"/>
-        <v>0.99522796275776315</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+        <v>0.56900910389977644</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="13">
         <v>9</v>
       </c>
       <c r="C11" s="13">
         <f ca="1"/>
-        <v>0.86728207976307248</v>
+        <v>0.9194361794480066</v>
       </c>
       <c r="E11" s="13">
         <f ca="1"/>
@@ -3188,16 +3229,16 @@
       </c>
       <c r="F11" s="13">
         <f ca="1"/>
-        <v>0.86728207976307248</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+        <v>0.9194361794480066</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="13">
         <v>10</v>
       </c>
       <c r="C12" s="13">
         <f ca="1"/>
-        <v>0.17119175519146013</v>
+        <v>0.40181899548169975</v>
       </c>
       <c r="E12" s="13">
         <f ca="1"/>
@@ -3205,7 +3246,7 @@
       </c>
       <c r="F12" s="13">
         <f ca="1"/>
-        <v>0.17119175519146013</v>
+        <v>0.40181899548169975</v>
       </c>
     </row>
   </sheetData>
@@ -3217,53 +3258,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5540266-91BE-4B2E-A8BC-1082BDC425C0}">
   <dimension ref="B2:L103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="8" customWidth="1"/>
-    <col min="2" max="5" width="9.140625" style="8"/>
-    <col min="6" max="6" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="3.6640625" style="8" customWidth="1"/>
+    <col min="2" max="5" width="9.109375" style="8"/>
+    <col min="6" max="6" width="13.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="11" cm="1">
         <f t="array" aca="1" ref="F2" ca="1">_xll.\TMX.CURVE.PWFLAT(time,rate)</f>
-        <v>2508277291536</v>
+        <v>2273350483504</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="8" cm="1">
         <f t="array" ref="B3:B12">_xll.ARRAY.SEQUENCE(1,10)</f>
         <v>1</v>
       </c>
       <c r="C3" s="8" cm="1">
         <f t="array" aca="1" ref="C3:C12" ca="1">_xlfn.RANDARRAY(ROWS(_xlfn.ANCHORARRAY(B3)))</f>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="F3" s="8" cm="1">
         <f t="array" aca="1" ref="F3:G13" ca="1">TRANSPOSE(_xll.TMX.CURVE.PWFLAT(F2))</f>
@@ -3271,7 +3310,7 @@
       </c>
       <c r="G3" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="I3" s="8" cm="1">
         <f t="array" ref="I3:I103">_xll.ARRAY.SEQUENCE(0,10,0.1)</f>
@@ -3279,24 +3318,24 @@
       </c>
       <c r="J3" s="8" cm="1">
         <f t="array" aca="1" ref="J3:J103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY($I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.PWFLAT.FORWARD(pwflat,_xlpm.t)))</f>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="K3" s="8" cm="1">
         <f t="array" aca="1" ref="K3:K103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY($I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.PWFLAT.SPOT(pwflat,_xlpm.t)))</f>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="L3" s="8" cm="1">
         <f t="array" aca="1" ref="L3:L103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY($I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.PWFLAT.DISCOUNT(pwflat,_xlpm.t)))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="8">
         <f ca="1"/>
-        <v>0.97521185509924591</v>
+        <v>8.9383682239568829E-2</v>
       </c>
       <c r="F4" s="8">
         <f ca="1"/>
@@ -3304,31 +3343,31 @@
       </c>
       <c r="G4" s="8">
         <f ca="1"/>
-        <v>0.97521185509924591</v>
+        <v>8.9383682239568829E-2</v>
       </c>
       <c r="I4" s="8">
         <v>0.1</v>
       </c>
       <c r="J4" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="K4" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677778</v>
       </c>
       <c r="L4" s="8">
         <f ca="1"/>
-        <v>0.94139755769230049</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.90962181263770703</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="8">
         <f ca="1"/>
-        <v>0.99691947434149752</v>
+        <v>0.9098121920374147</v>
       </c>
       <c r="F5" s="8">
         <f ca="1"/>
@@ -3336,31 +3375,31 @@
       </c>
       <c r="G5" s="8">
         <f ca="1"/>
-        <v>0.99691947434149752</v>
+        <v>0.9098121920374147</v>
       </c>
       <c r="I5" s="8">
         <v>0.2</v>
       </c>
       <c r="J5" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="K5" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677778</v>
       </c>
       <c r="L5" s="8">
         <f ca="1"/>
-        <v>0.88622936182806356</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.82741184196158302</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="8">
         <f ca="1"/>
-        <v>0.54672864773213004</v>
+        <v>0.10261778272441902</v>
       </c>
       <c r="F6" s="8">
         <f ca="1"/>
@@ -3368,31 +3407,31 @@
       </c>
       <c r="G6" s="8">
         <f ca="1"/>
-        <v>0.54672864773213004</v>
+        <v>0.10261778272441902</v>
       </c>
       <c r="I6" s="8">
         <v>0.30000000000000004</v>
       </c>
       <c r="J6" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="K6" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="L6" s="8">
         <f ca="1"/>
-        <v>0.83429415674213292</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.75263185954094924</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="8">
         <v>5</v>
       </c>
       <c r="C7" s="8">
         <f ca="1"/>
-        <v>0.83770297712941599</v>
+        <v>0.21567196970698377</v>
       </c>
       <c r="F7" s="8">
         <f ca="1"/>
@@ -3400,31 +3439,31 @@
       </c>
       <c r="G7" s="8">
         <f ca="1"/>
-        <v>0.83770297712941599</v>
+        <v>0.21567196970698377</v>
       </c>
       <c r="I7" s="8">
         <v>0.4</v>
       </c>
       <c r="J7" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="K7" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677778</v>
       </c>
       <c r="L7" s="8">
         <f ca="1"/>
-        <v>0.78540248135630242</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.68461035671234227</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="8">
         <v>6</v>
       </c>
       <c r="C8" s="8">
         <f ca="1"/>
-        <v>0.69707891184125215</v>
+        <v>0.70240536737706383</v>
       </c>
       <c r="F8" s="8">
         <f ca="1"/>
@@ -3432,31 +3471,31 @@
       </c>
       <c r="G8" s="8">
         <f ca="1"/>
-        <v>0.69707891184125215</v>
+        <v>0.70240536737706383</v>
       </c>
       <c r="I8" s="8">
         <v>0.5</v>
       </c>
       <c r="J8" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="K8" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="L8" s="8">
         <f ca="1"/>
-        <v>0.73937597812613465</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.62273651307522726</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="8">
         <v>7</v>
       </c>
       <c r="C9" s="8">
         <f ca="1"/>
-        <v>7.8071604142182061E-2</v>
+        <v>5.409639036802627E-2</v>
       </c>
       <c r="F9" s="8">
         <f ca="1"/>
@@ -3464,31 +3503,31 @@
       </c>
       <c r="G9" s="8">
         <f ca="1"/>
-        <v>7.8071604142182061E-2</v>
+        <v>5.409639036802627E-2</v>
       </c>
       <c r="I9" s="8">
         <v>0.60000000000000009</v>
       </c>
       <c r="J9" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="K9" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="L9" s="8">
         <f ca="1"/>
-        <v>0.69604674030740588</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.56645471599512753</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="8">
         <v>8</v>
       </c>
       <c r="C10" s="8">
         <f ca="1"/>
-        <v>0.80925543441441206</v>
+        <v>0.73487589397700526</v>
       </c>
       <c r="F10" s="8">
         <f ca="1"/>
@@ -3496,31 +3535,31 @@
       </c>
       <c r="G10" s="8">
         <f ca="1"/>
-        <v>0.80925543441441206</v>
+        <v>0.73487589397700526</v>
       </c>
       <c r="I10" s="8">
         <v>0.70000000000000007</v>
       </c>
       <c r="J10" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="K10" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677756</v>
       </c>
       <c r="L10" s="8">
         <f ca="1"/>
-        <v>0.65525670109373091</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.51525956574818732</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="8">
         <v>9</v>
       </c>
       <c r="C11" s="8">
         <f ca="1"/>
-        <v>0.20186189379151176</v>
+        <v>0.1314634821513172</v>
       </c>
       <c r="F11" s="8">
         <f ca="1"/>
@@ -3528,31 +3567,31 @@
       </c>
       <c r="G11" s="8">
         <f ca="1"/>
-        <v>0.20186189379151176</v>
+        <v>0.1314634821513172</v>
       </c>
       <c r="I11" s="8">
         <v>0.8</v>
       </c>
       <c r="J11" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="K11" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677778</v>
       </c>
       <c r="L11" s="8">
         <f ca="1"/>
-        <v>0.61685705797761059</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.46869133986188494</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="8">
         <v>10</v>
       </c>
       <c r="C12" s="8">
         <f ca="1"/>
-        <v>0.44387199209227735</v>
+        <v>0.40066932382155351</v>
       </c>
       <c r="F12" s="8">
         <f ca="1"/>
@@ -3560,25 +3599,25 @@
       </c>
       <c r="G12" s="8">
         <f ca="1"/>
-        <v>0.44387199209227735</v>
+        <v>0.40066932382155351</v>
       </c>
       <c r="I12" s="8">
         <v>0.9</v>
       </c>
       <c r="J12" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="K12" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="L12" s="8">
         <f ca="1"/>
-        <v>0.58070772744812715</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.42633186590207683</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F13" s="8">
         <f ca="1"/>
         <v>10</v>
@@ -3592,1545 +3631,1545 @@
       </c>
       <c r="J13" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="K13" s="8">
         <f ca="1"/>
-        <v>0.60389744283288471</v>
+        <v>0.94726356375677767</v>
       </c>
       <c r="L13" s="8">
         <f ca="1"/>
-        <v>0.54667683704035974</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.38780076388862872</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="I14" s="8">
         <v>1.1000000000000001</v>
       </c>
       <c r="J14" s="8">
         <f ca="1"/>
-        <v>0.97521185509924591</v>
+        <v>8.9383682239568829E-2</v>
       </c>
       <c r="K14" s="8">
         <f ca="1"/>
-        <v>0.63765329849346308</v>
+        <v>0.86927448361884951</v>
       </c>
       <c r="L14" s="8">
         <f ca="1"/>
-        <v>0.49588133373759707</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.38434990446009432</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="I15" s="8">
         <v>1.2000000000000002</v>
       </c>
       <c r="J15" s="8">
         <f ca="1"/>
-        <v>0.97521185509924591</v>
+        <v>8.9383682239568829E-2</v>
       </c>
       <c r="K15" s="8">
         <f ca="1"/>
-        <v>0.66578317821061161</v>
+        <v>0.80428358350390938</v>
       </c>
       <c r="L15" s="8">
         <f ca="1"/>
-        <v>0.44980558893849587</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.38092975156261277</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="I16" s="8">
         <v>1.3</v>
       </c>
       <c r="J16" s="8">
         <f ca="1"/>
-        <v>0.97521185509924591</v>
+        <v>8.9383682239568829E-2</v>
       </c>
       <c r="K16" s="8">
         <f ca="1"/>
-        <v>0.68958538412512194</v>
+        <v>0.74929128340665252</v>
       </c>
       <c r="L16" s="8">
         <f ca="1"/>
-        <v>0.40801105855177394</v>
-      </c>
-    </row>
-    <row r="17" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.37754003303304567</v>
+      </c>
+    </row>
+    <row r="17" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I17" s="8">
         <v>1.4000000000000001</v>
       </c>
       <c r="J17" s="8">
         <f ca="1"/>
-        <v>0.97521185509924591</v>
+        <v>8.9383682239568829E-2</v>
       </c>
       <c r="K17" s="8">
         <f ca="1"/>
-        <v>0.70998727490898794</v>
+        <v>0.70215502618043224</v>
       </c>
       <c r="L17" s="8">
         <f ca="1"/>
-        <v>0.37009994636951693</v>
-      </c>
-    </row>
-    <row r="18" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.37418047805010396</v>
+      </c>
+    </row>
+    <row r="18" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I18" s="8">
         <v>1.5</v>
       </c>
       <c r="J18" s="8">
         <f ca="1"/>
-        <v>0.97521185509924591</v>
+        <v>8.9383682239568829E-2</v>
       </c>
       <c r="K18" s="8">
         <f ca="1"/>
-        <v>0.72766891358833841</v>
+        <v>0.66130360325104143</v>
       </c>
       <c r="L18" s="8">
         <f ca="1"/>
-        <v>0.33571141600771087</v>
-      </c>
-    </row>
-    <row r="19" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.37085081820242644</v>
+      </c>
+    </row>
+    <row r="19" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I19" s="8">
         <v>1.6</v>
       </c>
       <c r="J19" s="8">
         <f ca="1"/>
-        <v>0.97521185509924591</v>
+        <v>8.9383682239568829E-2</v>
       </c>
       <c r="K19" s="8">
         <f ca="1"/>
-        <v>0.74314034743277024</v>
+        <v>0.62555860818782427</v>
       </c>
       <c r="L19" s="8">
         <f ca="1"/>
-        <v>0.30451815956518846</v>
-      </c>
-    </row>
-    <row r="20" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.36755078746713593</v>
+      </c>
+    </row>
+    <row r="20" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I20" s="8">
         <v>1.7000000000000002</v>
       </c>
       <c r="J20" s="8">
         <f ca="1"/>
-        <v>0.97521185509924591</v>
+        <v>8.9383682239568829E-2</v>
       </c>
       <c r="K20" s="8">
         <f ca="1"/>
-        <v>0.7567916125896218</v>
+        <v>0.5940189066614564</v>
       </c>
       <c r="L20" s="8">
         <f ca="1"/>
-        <v>0.27622328334409524</v>
-      </c>
-    </row>
-    <row r="21" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.36428012218858702</v>
+      </c>
+    </row>
+    <row r="21" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I21" s="8">
         <v>1.8</v>
       </c>
       <c r="J21" s="8">
         <f ca="1"/>
-        <v>0.97521185509924591</v>
+        <v>8.9383682239568829E-2</v>
       </c>
       <c r="K21" s="8">
         <f ca="1"/>
-        <v>0.76892607050682293</v>
+        <v>0.56598361641579598</v>
       </c>
       <c r="L21" s="8">
         <f ca="1"/>
-        <v>0.25055747820180713</v>
-      </c>
-    </row>
-    <row r="22" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.36103856105730198</v>
+      </c>
+    </row>
+    <row r="22" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I22" s="8">
         <v>1.9000000000000001</v>
       </c>
       <c r="J22" s="8">
         <f ca="1"/>
-        <v>0.97521185509924591</v>
+        <v>8.9383682239568829E-2</v>
       </c>
       <c r="K22" s="8">
         <f ca="1"/>
-        <v>0.77978321706431897</v>
+        <v>0.54089940935388925</v>
       </c>
       <c r="L22" s="8">
         <f ca="1"/>
-        <v>0.22727646130839924</v>
-      </c>
-    </row>
-    <row r="23" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.35782584508909487</v>
+      </c>
+    </row>
+    <row r="23" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I23" s="8">
         <v>2</v>
       </c>
       <c r="J23" s="8">
         <f ca="1"/>
-        <v>0.97521185509924591</v>
+        <v>8.9383682239568829E-2</v>
       </c>
       <c r="K23" s="8">
         <f ca="1"/>
-        <v>0.78955464896606531</v>
+        <v>0.51832362299817325</v>
       </c>
       <c r="L23" s="8">
         <f ca="1"/>
-        <v>0.20615864303879922</v>
-      </c>
-    </row>
-    <row r="24" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.35464171760438201</v>
+      </c>
+    </row>
+    <row r="24" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I24" s="8">
         <v>2.1</v>
       </c>
       <c r="J24" s="8">
         <f ca="1"/>
-        <v>0.99691947434149752</v>
+        <v>0.9098121920374147</v>
       </c>
       <c r="K24" s="8">
         <f ca="1"/>
-        <v>0.79942916446013346</v>
+        <v>0.53696593580956575</v>
       </c>
       <c r="L24" s="8">
         <f ca="1"/>
-        <v>0.18659752649811001</v>
-      </c>
-    </row>
-    <row r="25" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.32380025085612985</v>
+      </c>
+    </row>
+    <row r="25" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I25" s="8">
         <v>2.2000000000000002</v>
       </c>
       <c r="J25" s="8">
         <f ca="1"/>
-        <v>0.99691947434149752</v>
+        <v>0.9098121920374147</v>
       </c>
       <c r="K25" s="8">
         <f ca="1"/>
-        <v>0.80840599672746827</v>
+        <v>0.55391349291083158</v>
       </c>
       <c r="L25" s="8">
         <f ca="1"/>
-        <v>0.16889244354967303</v>
-      </c>
-    </row>
-    <row r="26" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.29564091532956366</v>
+      </c>
+    </row>
+    <row r="26" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I26" s="8">
         <v>2.3000000000000003</v>
       </c>
       <c r="J26" s="8">
         <f ca="1"/>
-        <v>0.99691947434149752</v>
+        <v>0.9098121920374147</v>
       </c>
       <c r="K26" s="8">
         <f ca="1"/>
-        <v>0.81660223488459993</v>
+        <v>0.56938734939459601</v>
       </c>
       <c r="L26" s="8">
         <f ca="1"/>
-        <v>0.15286728581531722</v>
-      </c>
-    </row>
-    <row r="27" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.26993046091774636</v>
+      </c>
+    </row>
+    <row r="27" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I27" s="8">
         <v>2.4000000000000004</v>
       </c>
       <c r="J27" s="8">
         <f ca="1"/>
-        <v>0.99691947434149752</v>
+        <v>0.9098121920374147</v>
       </c>
       <c r="K27" s="8">
         <f ca="1"/>
-        <v>0.82411545319530399</v>
+        <v>0.58357171783804684</v>
       </c>
       <c r="L27" s="8">
         <f ca="1"/>
-        <v>0.13836265781453455</v>
-      </c>
-    </row>
-    <row r="28" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.24645591937233263</v>
+      </c>
+    </row>
+    <row r="28" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I28" s="8">
         <v>2.5</v>
       </c>
       <c r="J28" s="8">
         <f ca="1"/>
-        <v>0.99691947434149752</v>
+        <v>0.9098121920374147</v>
       </c>
       <c r="K28" s="8">
         <f ca="1"/>
-        <v>0.83102761404115166</v>
+        <v>0.59662133680602147</v>
       </c>
       <c r="L28" s="8">
         <f ca="1"/>
-        <v>0.12523428323202221</v>
-      </c>
-    </row>
-    <row r="29" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.22502284676274525</v>
+      </c>
+    </row>
+    <row r="29" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I29" s="8">
         <v>2.6</v>
       </c>
       <c r="J29" s="8">
         <f ca="1"/>
-        <v>0.99691947434149752</v>
+        <v>0.9098121920374147</v>
       </c>
       <c r="K29" s="8">
         <f ca="1"/>
-        <v>0.83740807020654962</v>
+        <v>0.60866713893030588</v>
       </c>
       <c r="L29" s="8">
         <f ca="1"/>
-        <v>0.11335157917705942</v>
-      </c>
-    </row>
-    <row r="30" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.20545370342259878</v>
+      </c>
+    </row>
+    <row r="30" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I30" s="8">
         <v>2.7</v>
       </c>
       <c r="J30" s="8">
         <f ca="1"/>
-        <v>0.99691947434149752</v>
+        <v>0.9098121920374147</v>
       </c>
       <c r="K30" s="8">
         <f ca="1"/>
-        <v>0.84331589998932543</v>
+        <v>0.61982065941575437</v>
       </c>
       <c r="L30" s="8">
         <f ca="1"/>
-        <v>0.1025963487974534</v>
-      </c>
-    </row>
-    <row r="31" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.18758639219777179</v>
+      </c>
+    </row>
+    <row r="31" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I31" s="8">
         <v>2.8000000000000003</v>
       </c>
       <c r="J31" s="8">
         <f ca="1"/>
-        <v>0.99691947434149752</v>
+        <v>0.9098121920374147</v>
       </c>
       <c r="K31" s="8">
         <f ca="1"/>
-        <v>0.84880174193047453</v>
+        <v>0.63017749986652793</v>
       </c>
       <c r="L31" s="8">
         <f ca="1"/>
-        <v>9.2861616729037172E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.17127291477995266</v>
+      </c>
+    </row>
+    <row r="32" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I32" s="8">
         <v>2.9000000000000004</v>
       </c>
       <c r="J32" s="8">
         <f ca="1"/>
-        <v>0.99691947434149752</v>
+        <v>0.9098121920374147</v>
       </c>
       <c r="K32" s="8">
         <f ca="1"/>
-        <v>0.85390924994464779</v>
+        <v>0.63982007545862751</v>
       </c>
       <c r="L32" s="8">
         <f ca="1"/>
-        <v>8.4050552558442113E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.15637814096871455</v>
+      </c>
+    </row>
+    <row r="33" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I33" s="8">
         <v>3</v>
       </c>
       <c r="J33" s="8">
         <f ca="1"/>
-        <v>0.99691947434149752</v>
+        <v>0.9098121920374147</v>
       </c>
       <c r="K33" s="8">
         <f ca="1"/>
-        <v>0.85867625742454268</v>
+        <v>0.64881981267792044</v>
       </c>
       <c r="L33" s="8">
         <f ca="1"/>
-        <v>7.6075518610737733E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.14277869475999616</v>
+      </c>
+    </row>
+    <row r="34" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I34" s="8">
         <v>3.1</v>
       </c>
       <c r="J34" s="8">
         <f ca="1"/>
-        <v>0.54672864773213004</v>
+        <v>0.10261778272441902</v>
       </c>
       <c r="K34" s="8">
         <f ca="1"/>
-        <v>0.84861343130543265</v>
+        <v>0.63120039235683967</v>
       </c>
       <c r="L34" s="8">
         <f ca="1"/>
-        <v>7.2027907752673051E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.14132102341567182</v>
+      </c>
+    </row>
+    <row r="35" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I35" s="8">
         <v>3.2</v>
       </c>
       <c r="J35" s="8">
         <f ca="1"/>
-        <v>0.54672864773213004</v>
+        <v>0.10261778272441902</v>
       </c>
       <c r="K35" s="8">
         <f ca="1"/>
-        <v>0.83917953181876692</v>
+        <v>0.61468218580582656</v>
       </c>
       <c r="L35" s="8">
         <f ca="1"/>
-        <v>6.8195650844088074E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.1398782338858455</v>
+      </c>
+    </row>
+    <row r="36" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I36" s="8">
         <v>3.3000000000000003</v>
       </c>
       <c r="J36" s="8">
         <f ca="1"/>
-        <v>0.54672864773213004</v>
+        <v>0.10261778272441902</v>
       </c>
       <c r="K36" s="8">
         <f ca="1"/>
-        <v>0.83031738381614162</v>
+        <v>0.59916508268214752</v>
       </c>
       <c r="L36" s="8">
         <f ca="1"/>
-        <v>6.4567289988760448E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.13845017423767522</v>
+      </c>
+    </row>
+    <row r="37" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I37" s="8">
         <v>3.4000000000000004</v>
       </c>
       <c r="J37" s="8">
         <f ca="1"/>
-        <v>0.54672864773213004</v>
+        <v>0.10261778272441902</v>
       </c>
       <c r="K37" s="8">
         <f ca="1"/>
-        <v>0.8219765386372001</v>
+        <v>0.58456075033044963</v>
       </c>
       <c r="L37" s="8">
         <f ca="1"/>
-        <v>6.1131974443167522E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.13703669408946051</v>
+      </c>
+    </row>
+    <row r="38" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I38" s="8">
         <v>3.5</v>
       </c>
       <c r="J38" s="8">
         <f ca="1"/>
-        <v>0.54672864773213004</v>
+        <v>0.10261778272441902</v>
       </c>
       <c r="K38" s="8">
         <f ca="1"/>
-        <v>0.81411231318276944</v>
+        <v>0.57079095125599166</v>
       </c>
       <c r="L38" s="8">
         <f ca="1"/>
-        <v>5.7879437021424854E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.13563764459480529</v>
+      </c>
+    </row>
+    <row r="39" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I39" s="8">
         <v>3.6</v>
       </c>
       <c r="J39" s="8">
         <f ca="1"/>
-        <v>0.54672864773213004</v>
+        <v>0.10261778272441902</v>
       </c>
       <c r="K39" s="8">
         <f ca="1"/>
-        <v>0.80668498914247388</v>
+        <v>0.55778614101900348</v>
       </c>
       <c r="L39" s="8">
         <f ca="1"/>
-        <v>5.4799951344704015E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.13425287842694539</v>
+      </c>
+    </row>
+    <row r="40" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I40" s="8">
         <v>3.7</v>
       </c>
       <c r="J40" s="8">
         <f ca="1"/>
-        <v>0.54672864773213004</v>
+        <v>0.10261778272441902</v>
       </c>
       <c r="K40" s="8">
         <f ca="1"/>
-        <v>0.79965914207732947</v>
+        <v>0.54548429349752825</v>
       </c>
       <c r="L40" s="8">
         <f ca="1"/>
-        <v>5.1884310136328986E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.13288224976323554</v>
+      </c>
+    </row>
+    <row r="41" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I41" s="8">
         <v>3.8000000000000003</v>
       </c>
       <c r="J41" s="8">
         <f ca="1"/>
-        <v>0.54672864773213004</v>
+        <v>0.10261778272441902</v>
       </c>
       <c r="K41" s="8">
         <f ca="1"/>
-        <v>0.79300307643666634</v>
+        <v>0.53382991163507798</v>
       </c>
       <c r="L41" s="8">
         <f ca="1"/>
-        <v>4.9123795983566837E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.13152561426979276</v>
+      </c>
+    </row>
+    <row r="42" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I42" s="8">
         <v>3.9000000000000004</v>
       </c>
       <c r="J42" s="8">
         <f ca="1"/>
-        <v>0.54672864773213004</v>
+        <v>0.10261778272441902</v>
       </c>
       <c r="K42" s="8">
         <f ca="1"/>
-        <v>0.78668834749552441</v>
+        <v>0.52277319038095849</v>
       </c>
       <c r="L42" s="8">
         <f ca="1"/>
-        <v>4.6510155270586565E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.13018282908630013</v>
+      </c>
+    </row>
+    <row r="43" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I43" s="8">
         <v>4</v>
       </c>
       <c r="J43" s="8">
         <f ca="1"/>
-        <v>0.54672864773213004</v>
+        <v>0.10261778272441902</v>
       </c>
       <c r="K43" s="8">
         <f ca="1"/>
-        <v>0.78068935500143954</v>
+        <v>0.51226930518954505</v>
       </c>
       <c r="L43" s="8">
         <f ca="1"/>
-        <v>4.403557669336701E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.1288537528109624</v>
+      </c>
+    </row>
+    <row r="44" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I44" s="8">
         <v>4.1000000000000005</v>
       </c>
       <c r="J44" s="8">
         <f ca="1"/>
-        <v>0.83770297712941599</v>
+        <v>0.21567196970698377</v>
       </c>
       <c r="K44" s="8">
         <f ca="1"/>
-        <v>0.78207993115090246</v>
+        <v>0.50503522383631183</v>
       </c>
       <c r="L44" s="8">
         <f ca="1"/>
-        <v>4.0496987114491824E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.12610449214131936</v>
+      </c>
+    </row>
+    <row r="45" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I45" s="8">
         <v>4.2</v>
       </c>
       <c r="J45" s="8">
         <f ca="1"/>
-        <v>0.83770297712941599</v>
+        <v>0.21567196970698377</v>
       </c>
       <c r="K45" s="8">
         <f ca="1"/>
-        <v>0.78340428938848605</v>
+        <v>0.49814562254751826</v>
       </c>
       <c r="L45" s="8">
         <f ca="1"/>
-        <v>3.7242750066410757E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.1234138905084997</v>
+      </c>
+    </row>
+    <row r="46" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I46" s="8">
         <v>4.3</v>
       </c>
       <c r="J46" s="8">
         <f ca="1"/>
-        <v>0.83770297712941599</v>
+        <v>0.21567196970698377</v>
       </c>
       <c r="K46" s="8">
         <f ca="1"/>
-        <v>0.78466704956850775</v>
+        <v>0.49157646783029663</v>
       </c>
       <c r="L46" s="8">
         <f ca="1"/>
-        <v>3.4250013415930793E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.12078069634967034</v>
+      </c>
+    </row>
+    <row r="47" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I47" s="8">
         <v>4.4000000000000004</v>
       </c>
       <c r="J47" s="8">
         <f ca="1"/>
-        <v>0.83770297712941599</v>
+        <v>0.21567196970698377</v>
       </c>
       <c r="K47" s="8">
         <f ca="1"/>
-        <v>0.78587241155852827</v>
+        <v>0.48530591105476678</v>
       </c>
       <c r="L47" s="8">
         <f ca="1"/>
-        <v>3.1497766879532901E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.11820368480621211</v>
+      </c>
+    </row>
+    <row r="48" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I48" s="8">
         <v>4.5</v>
       </c>
       <c r="J48" s="8">
         <f ca="1"/>
-        <v>0.83770297712941599</v>
+        <v>0.21567196970698377</v>
       </c>
       <c r="K48" s="8">
         <f ca="1"/>
-        <v>0.78702420190454803</v>
+        <v>0.47931404569148267</v>
       </c>
       <c r="L48" s="8">
         <f ca="1"/>
-        <v>2.8966683891861265E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.11568165715402111</v>
+      </c>
+    </row>
+    <row r="49" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I49" s="8">
         <v>4.6000000000000005</v>
       </c>
       <c r="J49" s="8">
         <f ca="1"/>
-        <v>0.83770297712941599</v>
+        <v>0.21567196970698377</v>
       </c>
       <c r="K49" s="8">
         <f ca="1"/>
-        <v>0.78812591440943647</v>
+        <v>0.47358269621355875</v>
       </c>
       <c r="L49" s="8">
         <f ca="1"/>
-        <v>2.6638992194251993E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.11321344024597768</v>
+      </c>
+    </row>
+    <row r="50" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I50" s="8">
         <v>4.7</v>
       </c>
       <c r="J50" s="8">
         <f ca="1"/>
-        <v>0.83770297712941599</v>
+        <v>0.21567196970698377</v>
       </c>
       <c r="K50" s="8">
         <f ca="1"/>
-        <v>0.78918074553113815</v>
+        <v>0.4680952339474615</v>
       </c>
       <c r="L50" s="8">
         <f ca="1"/>
-        <v>2.4498350577748948E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.11079788596632117</v>
+      </c>
+    </row>
+    <row r="51" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I51" s="8">
         <v>4.8000000000000007</v>
       </c>
       <c r="J51" s="8">
         <f ca="1"/>
-        <v>0.83770297712941599</v>
+        <v>0.21567196970698377</v>
       </c>
       <c r="K51" s="8">
         <f ca="1"/>
-        <v>0.79019162535610221</v>
+        <v>0.46283641594245151</v>
       </c>
       <c r="L51" s="8">
         <f ca="1"/>
-        <v>2.2529724088616254E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.10843386849729583</v>
+      </c>
+    </row>
+    <row r="52" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I52" s="8">
         <v>4.9000000000000004</v>
       </c>
       <c r="J52" s="8">
         <f ca="1"/>
-        <v>0.83770297712941599</v>
+        <v>0.21567196970698377</v>
       </c>
       <c r="K52" s="8">
         <f ca="1"/>
-        <v>0.79116124478004746</v>
+        <v>0.45779224357029907</v>
       </c>
       <c r="L52" s="8">
         <f ca="1"/>
-        <v>2.071929174383948E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.10612029220153078</v>
+      </c>
+    </row>
+    <row r="53" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I53" s="8">
         <v>5</v>
       </c>
       <c r="J53" s="8">
         <f ca="1"/>
-        <v>0.83770297712941599</v>
+        <v>0.21567196970698377</v>
       </c>
       <c r="K53" s="8">
         <f ca="1"/>
-        <v>0.79209207942703475</v>
+        <v>0.45294983809303274</v>
       </c>
       <c r="L53" s="8">
         <f ca="1"/>
-        <v>1.9054341566120733E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="9:12" x14ac:dyDescent="0.3">
+        <v>0.10385607902681132</v>
+      </c>
+    </row>
+    <row r="54" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I54" s="8">
         <v>5.1000000000000005</v>
       </c>
       <c r="J54" s="8">
         <f ca="1"/>
-        <v>0.69707891184125215</v>
+        <v>0.70240536737706383</v>
       </c>
       <c r="K54" s="8">
         <f ca="1"/>
-        <v>0.7902290761410391</v>
+        <v>0.45784112298095497</v>
       </c>
       <c r="L54" s="8">
         <f ca="1"/>
-        <v>1.7771338525689816E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="9:12" x14ac:dyDescent="0.3">
+        <v>9.6811476454202391E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I55" s="8">
         <v>5.2</v>
       </c>
       <c r="J55" s="8">
         <f ca="1"/>
-        <v>0.69707891184125215</v>
+        <v>0.70240536737706383</v>
       </c>
       <c r="K55" s="8">
         <f ca="1"/>
-        <v>0.78843772682758162</v>
+        <v>0.46254428152703392</v>
       </c>
       <c r="L55" s="8">
         <f ca="1"/>
-        <v>1.6574726861820578E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="9:12" x14ac:dyDescent="0.3">
+        <v>9.0244712108271341E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I56" s="8">
         <v>5.3000000000000007</v>
       </c>
       <c r="J56" s="8">
         <f ca="1"/>
-        <v>0.69707891184125215</v>
+        <v>0.70240536737706383</v>
       </c>
       <c r="K56" s="8">
         <f ca="1"/>
-        <v>0.78671397560142453</v>
+        <v>0.46706996239212883</v>
       </c>
       <c r="L56" s="8">
         <f ca="1"/>
-        <v>1.5458687456221283E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="9:12" x14ac:dyDescent="0.3">
+        <v>8.4123373907713378E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I57" s="8">
         <v>5.4</v>
       </c>
       <c r="J57" s="8">
         <f ca="1"/>
-        <v>0.69707891184125215</v>
+        <v>0.70240536737706383</v>
       </c>
       <c r="K57" s="8">
         <f ca="1"/>
-        <v>0.78505406701327318</v>
+        <v>0.47142802544740547</v>
       </c>
       <c r="L57" s="8">
         <f ca="1"/>
-        <v>1.4417795016755152E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="9:12" x14ac:dyDescent="0.3">
+        <v>7.8417251385801745E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I58" s="8">
         <v>5.5</v>
       </c>
       <c r="J58" s="8">
         <f ca="1"/>
-        <v>0.69707891184125215</v>
+        <v>0.70240536737706383</v>
       </c>
       <c r="K58" s="8">
         <f ca="1"/>
-        <v>0.78345451873741823</v>
+        <v>0.47562761348249011</v>
       </c>
       <c r="L58" s="8">
         <f ca="1"/>
-        <v>1.3446992238604665E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="9:12" x14ac:dyDescent="0.3">
+        <v>7.3098175931354481E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I59" s="8">
         <v>5.6000000000000005</v>
       </c>
       <c r="J59" s="8">
         <f ca="1"/>
-        <v>0.69707891184125215</v>
+        <v>0.70240536737706383</v>
       </c>
       <c r="K59" s="8">
         <f ca="1"/>
-        <v>0.78191209718570087</v>
+        <v>0.47967721623060749</v>
       </c>
       <c r="L59" s="8">
         <f ca="1"/>
-        <v>1.2541555646364E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="9:12" x14ac:dyDescent="0.3">
+        <v>6.8139895813772264E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I60" s="8">
         <v>5.7</v>
       </c>
       <c r="J60" s="8">
         <f ca="1"/>
-        <v>0.69707891184125215</v>
+        <v>0.70240536737706383</v>
       </c>
       <c r="K60" s="8">
         <f ca="1"/>
-        <v>0.78042379568843001</v>
+        <v>0.48358472765422961</v>
       </c>
       <c r="L60" s="8">
         <f ca="1"/>
-        <v>1.1697085625938925E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="9:12" x14ac:dyDescent="0.3">
+        <v>6.3517938228381018E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I61" s="8">
         <v>5.8000000000000007</v>
       </c>
       <c r="J61" s="8">
         <f ca="1"/>
-        <v>0.69707891184125215</v>
+        <v>0.70240536737706383</v>
       </c>
       <c r="K61" s="8">
         <f ca="1"/>
-        <v>0.77898681493244404</v>
+        <v>0.4873574973046233</v>
       </c>
       <c r="L61" s="8">
         <f ca="1"/>
-        <v>1.0909477112945765E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="9:12" x14ac:dyDescent="0.3">
+        <v>5.9209487337599988E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I62" s="8">
         <v>5.9</v>
       </c>
       <c r="J62" s="8">
         <f ca="1"/>
-        <v>0.69707891184125215</v>
+        <v>0.70240536737706383</v>
       </c>
       <c r="K62" s="8">
         <f ca="1"/>
-        <v>0.77759854538852546</v>
+        <v>0.49100237645839345</v>
       </c>
       <c r="L62" s="8">
         <f ca="1"/>
-        <v>1.0174901471145902E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="9:12" x14ac:dyDescent="0.3">
+        <v>5.5193282196937261E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I63" s="8">
         <v>6</v>
       </c>
       <c r="J63" s="8">
         <f ca="1"/>
-        <v>0.69707891184125215</v>
+        <v>0.70240536737706383</v>
       </c>
       <c r="K63" s="8">
         <f ca="1"/>
-        <v>0.77625655149607109</v>
+        <v>0.49452575964037121</v>
       </c>
       <c r="L63" s="8">
         <f ca="1"/>
-        <v>9.4897846262742731E-3</v>
-      </c>
-    </row>
-    <row r="64" spans="9:12" x14ac:dyDescent="0.3">
+        <v>5.1449497813911498E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I64" s="8">
         <v>6.1000000000000005</v>
       </c>
       <c r="J64" s="8">
         <f ca="1"/>
-        <v>7.8071604142182061E-2</v>
+        <v>5.409639036802627E-2</v>
       </c>
       <c r="K64" s="8">
         <f ca="1"/>
-        <v>0.7648108966214171</v>
+        <v>0.48730560604574263</v>
       </c>
       <c r="L64" s="8">
         <f ca="1"/>
-        <v>9.4159847878467155E-3</v>
-      </c>
-    </row>
-    <row r="65" spans="9:12" x14ac:dyDescent="0.3">
+        <v>5.1171926017968598E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I65" s="8">
         <v>6.2</v>
       </c>
       <c r="J65" s="8">
         <f ca="1"/>
-        <v>7.8071604142182061E-2</v>
+        <v>5.409639036802627E-2</v>
       </c>
       <c r="K65" s="8">
         <f ca="1"/>
-        <v>0.75373445642013914</v>
+        <v>0.48031836063158589</v>
       </c>
       <c r="L65" s="8">
         <f ca="1"/>
-        <v>9.3427588722149891E-3</v>
-      </c>
-    </row>
-    <row r="66" spans="9:12" x14ac:dyDescent="0.3">
+        <v>5.0895851729606589E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I66" s="8">
         <v>6.3000000000000007</v>
       </c>
       <c r="J66" s="8">
         <f ca="1"/>
-        <v>7.8071604142182061E-2</v>
+        <v>5.409639036802627E-2</v>
       </c>
       <c r="K66" s="8">
         <f ca="1"/>
-        <v>0.74300964924112389</v>
+        <v>0.47355293253216429</v>
       </c>
       <c r="L66" s="8">
         <f ca="1"/>
-        <v>9.2701024160769634E-3</v>
-      </c>
-    </row>
-    <row r="67" spans="9:12" x14ac:dyDescent="0.3">
+        <v>5.0621266869674615E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I67" s="8">
         <v>6.4</v>
       </c>
       <c r="J67" s="8">
         <f ca="1"/>
-        <v>7.8071604142182061E-2</v>
+        <v>5.409639036802627E-2</v>
       </c>
       <c r="K67" s="8">
         <f ca="1"/>
-        <v>0.73261999228645303</v>
+        <v>0.46699892406084964</v>
       </c>
       <c r="L67" s="8">
         <f ca="1"/>
-        <v>9.1980109908270935E-3</v>
-      </c>
-    </row>
-    <row r="68" spans="9:12" x14ac:dyDescent="0.3">
+        <v>5.0348163402604472E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I68" s="8">
         <v>6.5</v>
       </c>
       <c r="J68" s="8">
         <f ca="1"/>
-        <v>7.8071604142182061E-2</v>
+        <v>5.409639036802627E-2</v>
       </c>
       <c r="K68" s="8">
         <f ca="1"/>
-        <v>0.72255001708423339</v>
+        <v>0.46064657738865239</v>
       </c>
       <c r="L68" s="8">
         <f ca="1"/>
-        <v>9.1264802023046741E-3</v>
-      </c>
-    </row>
-    <row r="69" spans="9:12" x14ac:dyDescent="0.3">
+        <v>5.0076533336178314E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I69" s="8">
         <v>6.6000000000000005</v>
       </c>
       <c r="J69" s="8">
         <f ca="1"/>
-        <v>7.8071604142182061E-2</v>
+        <v>5.409639036802627E-2</v>
       </c>
       <c r="K69" s="8">
         <f ca="1"/>
-        <v>0.71278519264571749</v>
+        <v>0.45448672607015805</v>
       </c>
       <c r="L69" s="8">
         <f ca="1"/>
-        <v>9.0555056905291826E-3</v>
-      </c>
-    </row>
-    <row r="70" spans="9:12" x14ac:dyDescent="0.3">
+        <v>4.9806368721297532E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I70" s="8">
         <v>6.7</v>
       </c>
       <c r="J70" s="8">
         <f ca="1"/>
-        <v>7.8071604142182061E-2</v>
+        <v>5.409639036802627E-2</v>
       </c>
       <c r="K70" s="8">
         <f ca="1"/>
-        <v>0.70331185550387376</v>
+        <v>0.44851075091042469</v>
       </c>
       <c r="L70" s="8">
         <f ca="1"/>
-        <v>8.9850831294087333E-3</v>
-      </c>
-    </row>
-    <row r="71" spans="9:12" x14ac:dyDescent="0.3">
+        <v>4.9537661651745522E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I71" s="8">
         <v>6.8000000000000007</v>
       </c>
       <c r="J71" s="8">
         <f ca="1"/>
-        <v>7.8071604142182061E-2</v>
+        <v>5.409639036802627E-2</v>
       </c>
       <c r="K71" s="8">
         <f ca="1"/>
-        <v>0.69411714592502527</v>
+        <v>0.44271053972597768</v>
       </c>
       <c r="L71" s="8">
         <f ca="1"/>
-        <v>8.9152082264958715E-3</v>
-      </c>
-    </row>
-    <row r="72" spans="9:12" x14ac:dyDescent="0.3">
+        <v>4.9270404263958505E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I72" s="8">
         <v>6.9</v>
       </c>
       <c r="J72" s="8">
         <f ca="1"/>
-        <v>7.8071604142182061E-2</v>
+        <v>5.409639036802627E-2</v>
       </c>
       <c r="K72" s="8">
         <f ca="1"/>
-        <v>0.68518894966730293</v>
+        <v>0.4370784506048479</v>
       </c>
       <c r="L72" s="8">
         <f ca="1"/>
-        <v>8.8458767227284595E-3</v>
-      </c>
-    </row>
-    <row r="73" spans="9:12" x14ac:dyDescent="0.3">
+        <v>4.9004588736794204E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I73" s="8">
         <v>7</v>
       </c>
       <c r="J73" s="8">
         <f ca="1"/>
-        <v>7.8071604142182061E-2</v>
+        <v>5.409639036802627E-2</v>
       </c>
       <c r="K73" s="8">
         <f ca="1"/>
-        <v>0.67651584473122983</v>
+        <v>0.43160727831575052</v>
       </c>
       <c r="L73" s="8">
         <f ca="1"/>
-        <v>8.7770843921595489E-3</v>
-      </c>
-    </row>
-    <row r="74" spans="9:12" x14ac:dyDescent="0.3">
+        <v>4.8740207291306473E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I74" s="8">
         <v>7.1000000000000005</v>
       </c>
       <c r="J74" s="8">
         <f ca="1"/>
-        <v>0.80925543441441206</v>
+        <v>0.73487589397700526</v>
       </c>
       <c r="K74" s="8">
         <f ca="1"/>
-        <v>0.67838541641690842</v>
+        <v>0.43587866726872598</v>
       </c>
       <c r="L74" s="8">
         <f ca="1"/>
-        <v>8.0947740624918319E-3</v>
-      </c>
-    </row>
-    <row r="75" spans="9:12" x14ac:dyDescent="0.3">
+        <v>4.5286852065599521E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I75" s="8">
         <v>7.2</v>
       </c>
       <c r="J75" s="8">
         <f ca="1"/>
-        <v>0.80925543441441206</v>
+        <v>0.73487589397700526</v>
       </c>
       <c r="K75" s="8">
         <f ca="1"/>
-        <v>0.68020305555576266</v>
+        <v>0.44003140652856315</v>
       </c>
       <c r="L75" s="8">
         <f ca="1"/>
-        <v>7.4655046791022028E-3</v>
-      </c>
-    </row>
-    <row r="76" spans="9:12" x14ac:dyDescent="0.3">
+        <v>4.2078173637738532E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I76" s="8">
         <v>7.3000000000000007</v>
       </c>
       <c r="J76" s="8">
         <f ca="1"/>
-        <v>0.80925543441441206</v>
+        <v>0.73487589397700526</v>
       </c>
       <c r="K76" s="8">
         <f ca="1"/>
-        <v>0.68197089636204555</v>
+        <v>0.44407037211004868</v>
       </c>
       <c r="L76" s="8">
         <f ca="1"/>
-        <v>6.885156142290275E-3</v>
-      </c>
-    </row>
-    <row r="77" spans="9:12" x14ac:dyDescent="0.3">
+        <v>3.9096837673063455E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I77" s="8">
         <v>7.4</v>
       </c>
       <c r="J77" s="8">
         <f ca="1"/>
-        <v>0.80925543441441206</v>
+        <v>0.73487589397700526</v>
       </c>
       <c r="K77" s="8">
         <f ca="1"/>
-        <v>0.68369095768707755</v>
+        <v>0.44800017645960216</v>
       </c>
       <c r="L77" s="8">
         <f ca="1"/>
-        <v>6.349920654533288E-3</v>
-      </c>
-    </row>
-    <row r="78" spans="9:12" x14ac:dyDescent="0.3">
+        <v>3.6326736507758847E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I78" s="8">
         <v>7.5</v>
       </c>
       <c r="J78" s="8">
         <f ca="1"/>
-        <v>0.80925543441441206</v>
+        <v>0.73487589397700526</v>
       </c>
       <c r="K78" s="8">
         <f ca="1"/>
-        <v>0.68536515071010862</v>
+        <v>0.45182518602650085</v>
       </c>
       <c r="L78" s="8">
         <f ca="1"/>
-        <v>5.8562932766888422E-3</v>
-      </c>
-    </row>
-    <row r="79" spans="9:12" x14ac:dyDescent="0.3">
+        <v>3.3752901138140903E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I79" s="8">
         <v>7.6000000000000005</v>
       </c>
       <c r="J79" s="8">
         <f ca="1"/>
-        <v>0.80925543441441206</v>
+        <v>0.73487589397700526</v>
       </c>
       <c r="K79" s="8">
         <f ca="1"/>
-        <v>0.68699528602200743</v>
+        <v>0.45554953744690224</v>
       </c>
       <c r="L79" s="8">
         <f ca="1"/>
-        <v>5.4010395725461388E-3</v>
-      </c>
-    </row>
-    <row r="80" spans="9:12" x14ac:dyDescent="0.3">
+        <v>3.1361429447060371E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I80" s="8">
         <v>7.7</v>
       </c>
       <c r="J80" s="8">
         <f ca="1"/>
-        <v>0.80925543441441206</v>
+        <v>0.73487589397700526</v>
       </c>
       <c r="K80" s="8">
         <f ca="1"/>
-        <v>0.68858308015697367</v>
+        <v>0.45917715246677371</v>
       </c>
       <c r="L80" s="8">
         <f ca="1"/>
-        <v>4.9811732451142182E-3</v>
-      </c>
-    </row>
-    <row r="81" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.9139398947407417E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I81" s="8">
         <v>7.8000000000000007</v>
       </c>
       <c r="J81" s="8">
         <f ca="1"/>
-        <v>0.80925543441441206</v>
+        <v>0.73487589397700526</v>
       </c>
       <c r="K81" s="8">
         <f ca="1"/>
-        <v>0.69013016162181262</v>
+        <v>0.46271175171690487</v>
       </c>
       <c r="L81" s="8">
         <f ca="1"/>
-        <v>4.5939482581617928E-3</v>
-      </c>
-    </row>
-    <row r="82" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.7074804267709078E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I82" s="8">
         <v>7.9</v>
       </c>
       <c r="J82" s="8">
         <f ca="1"/>
-        <v>0.80925543441441206</v>
+        <v>0.73487589397700526</v>
       </c>
       <c r="K82" s="8">
         <f ca="1"/>
-        <v>0.69163807646728859</v>
+        <v>0.46615686744171625</v>
       </c>
       <c r="L82" s="8">
         <f ca="1"/>
-        <v>4.2368250680906239E-3</v>
-      </c>
-    </row>
-    <row r="83" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.515649315082838E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I83" s="8">
         <v>8</v>
       </c>
       <c r="J83" s="8">
         <f ca="1"/>
-        <v>0.80925543441441206</v>
+        <v>0.73487589397700526</v>
       </c>
       <c r="K83" s="8">
         <f ca="1"/>
-        <v>0.69310829344162761</v>
+        <v>0.46951585527340733</v>
       </c>
       <c r="L83" s="8">
         <f ca="1"/>
-        <v>3.9074635560703919E-3</v>
-      </c>
-    </row>
-    <row r="84" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.3374097398744652E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I84" s="8">
         <v>8.1</v>
       </c>
       <c r="J84" s="8">
         <f ca="1"/>
-        <v>0.20186189379151176</v>
+        <v>0.1314634821513172</v>
       </c>
       <c r="K84" s="8">
         <f ca="1"/>
-        <v>0.68704352307557681</v>
+        <v>0.46534236918548033</v>
       </c>
       <c r="L84" s="8">
         <f ca="1"/>
-        <v>3.8293773032494482E-3</v>
-      </c>
-    </row>
-    <row r="85" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.3068824437641935E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I85" s="8">
         <v>8.2000000000000011</v>
       </c>
       <c r="J85" s="8">
         <f ca="1"/>
-        <v>0.20186189379151176</v>
+        <v>0.1314634821513172</v>
       </c>
       <c r="K85" s="8">
         <f ca="1"/>
-        <v>0.68112667393796622</v>
+        <v>0.46127067544116118</v>
       </c>
       <c r="L85" s="8">
         <f ca="1"/>
-        <v>3.752851487308488E-3</v>
-      </c>
-    </row>
-    <row r="86" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.2767538441028443E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I86" s="8">
         <v>8.3000000000000007</v>
       </c>
       <c r="J86" s="8">
         <f ca="1"/>
-        <v>0.20186189379151176</v>
+        <v>0.1314634821513172</v>
       </c>
       <c r="K86" s="8">
         <f ca="1"/>
-        <v>0.67535239947837045</v>
+        <v>0.4572970947991149</v>
       </c>
       <c r="L86" s="8">
         <f ca="1"/>
-        <v>3.6778579208587743E-3</v>
-      </c>
-    </row>
-    <row r="87" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.2470187338224451E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I87" s="8">
         <v>8.4</v>
       </c>
       <c r="J87" s="8">
         <f ca="1"/>
-        <v>0.20186189379151176</v>
+        <v>0.1314634821513172</v>
       </c>
       <c r="K87" s="8">
         <f ca="1"/>
-        <v>0.66971560774400307</v>
+        <v>0.45341812321997443</v>
       </c>
       <c r="L87" s="8">
         <f ca="1"/>
-        <v>3.6043603616018501E-3</v>
-      </c>
-    </row>
-    <row r="88" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.2176719738632222E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I88" s="8">
         <v>8.5</v>
       </c>
       <c r="J88" s="8">
         <f ca="1"/>
-        <v>0.20186189379151176</v>
+        <v>0.1314634821513172</v>
       </c>
       <c r="K88" s="8">
         <f ca="1"/>
-        <v>0.66421144640338547</v>
+        <v>0.44963042156034322</v>
       </c>
       <c r="L88" s="8">
         <f ca="1"/>
-        <v>3.5323315704380801E-3</v>
-      </c>
-    </row>
-    <row r="89" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.1887084922857448E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I89" s="8">
         <v>8.6</v>
       </c>
       <c r="J89" s="8">
         <f ca="1"/>
-        <v>0.20186189379151176</v>
+        <v>0.1314634821513172</v>
       </c>
       <c r="K89" s="8">
         <f ca="1"/>
-        <v>0.6588352888148753</v>
+        <v>0.44593080598581969</v>
       </c>
       <c r="L89" s="8">
         <f ca="1"/>
-        <v>3.4617421964559855E-3</v>
-      </c>
-    </row>
-    <row r="90" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.1601232833944026E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I90" s="8">
         <v>8.7000000000000011</v>
       </c>
       <c r="J90" s="8">
         <f ca="1"/>
-        <v>0.20186189379151176</v>
+        <v>0.1314634821513172</v>
       </c>
       <c r="K90" s="8">
         <f ca="1"/>
-        <v>0.65358272105598603</v>
+        <v>0.44231623904519313</v>
       </c>
       <c r="L90" s="8">
         <f ca="1"/>
-        <v>3.3925634753573302E-3</v>
-      </c>
-    </row>
-    <row r="91" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.1319114068718691E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I91" s="8">
         <v>8.8000000000000007</v>
       </c>
       <c r="J91" s="8">
         <f ca="1"/>
-        <v>0.20186189379151176</v>
+        <v>0.1314634821513172</v>
       </c>
       <c r="K91" s="8">
         <f ca="1"/>
-        <v>0.6484495298370716</v>
+        <v>0.43878382135321731</v>
       </c>
       <c r="L91" s="8">
         <f ca="1"/>
-        <v>3.3247672177348759E-3</v>
-      </c>
-    </row>
-    <row r="92" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.1040679869265728E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I92" s="8">
         <v>8.9</v>
       </c>
       <c r="J92" s="8">
         <f ca="1"/>
-        <v>0.20186189379151176</v>
+        <v>0.1314634821513172</v>
       </c>
       <c r="K92" s="8">
         <f ca="1"/>
-        <v>0.64343169122981814</v>
+        <v>0.43533078383409485</v>
       </c>
       <c r="L92" s="8">
         <f ca="1"/>
-        <v>3.2583257975880783E-3</v>
-      </c>
-    </row>
-    <row r="93" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.0765882114489344E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I93" s="8">
         <v>9</v>
       </c>
       <c r="J93" s="8">
         <f ca="1"/>
-        <v>0.20186189379151176</v>
+        <v>0.1314634821513172</v>
       </c>
       <c r="K93" s="8">
         <f ca="1"/>
-        <v>0.63852536014717032</v>
+        <v>0.43195448048206397</v>
       </c>
       <c r="L93" s="8">
         <f ca="1"/>
-        <v>3.1932121410822144E-3</v>
-      </c>
-    </row>
-    <row r="94" spans="9:12" x14ac:dyDescent="0.3">
+        <v>2.0494673311810478E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I94" s="8">
         <v>9.1</v>
       </c>
       <c r="J94" s="8">
         <f ca="1"/>
-        <v>0.44387199209227735</v>
+        <v>0.40066932382155351</v>
       </c>
       <c r="K94" s="8">
         <f ca="1"/>
-        <v>0.63638631214656705</v>
+        <v>0.43161068755172871</v>
       </c>
       <c r="L94" s="8">
         <f ca="1"/>
-        <v>3.0545743297533722E-3</v>
-      </c>
-    </row>
-    <row r="95" spans="9:12" x14ac:dyDescent="0.3">
+        <v>1.9689748119705731E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I95" s="8">
         <v>9.2000000000000011</v>
       </c>
       <c r="J95" s="8">
         <f ca="1"/>
-        <v>0.44387199209227735</v>
+        <v>0.40066932382155351</v>
       </c>
       <c r="K95" s="8">
         <f ca="1"/>
-        <v>0.63429376518945524</v>
+        <v>0.43127436838074856</v>
       </c>
       <c r="L95" s="8">
         <f ca="1"/>
-        <v>2.9219557572091161E-3</v>
-      </c>
-    </row>
-    <row r="96" spans="9:12" x14ac:dyDescent="0.3">
+        <v>1.8916436349895906E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I96" s="8">
         <v>9.3000000000000007</v>
       </c>
       <c r="J96" s="8">
         <f ca="1"/>
-        <v>0.44387199209227735</v>
+        <v>0.40066932382155351</v>
       </c>
       <c r="K96" s="8">
         <f ca="1"/>
-        <v>0.63224621924217372</v>
+        <v>0.43094528188011205</v>
       </c>
       <c r="L96" s="8">
         <f ca="1"/>
-        <v>2.7950951051328044E-3</v>
-      </c>
-    </row>
-    <row r="97" spans="9:12" x14ac:dyDescent="0.3">
+        <v>1.817349356488851E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I97" s="8">
         <v>9.4</v>
       </c>
       <c r="J97" s="8">
         <f ca="1"/>
-        <v>0.44387199209227735</v>
+        <v>0.40066932382155351</v>
       </c>
       <c r="K97" s="8">
         <f ca="1"/>
-        <v>0.63024223810228119</v>
+        <v>0.4306231972199146</v>
       </c>
       <c r="L97" s="8">
         <f ca="1"/>
-        <v>2.6737424042428556E-3</v>
-      </c>
-    </row>
-    <row r="98" spans="9:12" x14ac:dyDescent="0.3">
+        <v>1.7459731903338691E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I98" s="8">
         <v>9.5</v>
       </c>
       <c r="J98" s="8">
         <f ca="1"/>
-        <v>0.44387199209227735</v>
+        <v>0.40066932382155351</v>
       </c>
       <c r="K98" s="8">
         <f ca="1"/>
-        <v>0.628280446039018</v>
+        <v>0.43030789328940555</v>
       </c>
       <c r="L98" s="8">
         <f ca="1"/>
-        <v>2.5576549621629634E-3</v>
-      </c>
-    </row>
-    <row r="99" spans="9:12" x14ac:dyDescent="0.3">
+        <v>1.6774003103705897E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I99" s="8">
         <v>9.6000000000000014</v>
       </c>
       <c r="J99" s="8">
         <f ca="1"/>
-        <v>0.44387199209227735</v>
+        <v>0.40066932382155351</v>
       </c>
       <c r="K99" s="8">
         <f ca="1"/>
-        <v>0.62635952464373945</v>
+        <v>0.42999915819078205</v>
       </c>
       <c r="L99" s="8">
         <f ca="1"/>
-        <v>2.4466103552522678E-3</v>
-      </c>
-    </row>
-    <row r="100" spans="9:12" x14ac:dyDescent="0.3">
+        <v>1.6115206171304922E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I100" s="8">
         <v>9.7000000000000011</v>
       </c>
       <c r="J100" s="8">
         <f ca="1"/>
-        <v>0.44387199209227735</v>
+        <v>0.40066932382155351</v>
       </c>
       <c r="K100" s="8">
         <f ca="1"/>
-        <v>0.62447820987516767</v>
+        <v>0.42969678876429512</v>
       </c>
       <c r="L100" s="8">
         <f ca="1"/>
-        <v>2.3403868753761477E-3</v>
-      </c>
-    </row>
-    <row r="101" spans="9:12" x14ac:dyDescent="0.3">
+        <v>1.5482283351091823E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I101" s="8">
         <v>9.8000000000000007</v>
       </c>
       <c r="J101" s="8">
         <f ca="1"/>
-        <v>0.44387199209227735</v>
+        <v>0.40066932382155351</v>
       </c>
       <c r="K101" s="8">
         <f ca="1"/>
-        <v>0.62263528928554635</v>
+        <v>0.42940059014243048</v>
       </c>
       <c r="L101" s="8">
         <f ca="1"/>
-        <v>2.2387751965904758E-3</v>
-      </c>
-    </row>
-    <row r="102" spans="9:12" x14ac:dyDescent="0.3">
+        <v>1.4874218429057343E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I102" s="8">
         <v>9.9</v>
       </c>
       <c r="J102" s="8">
         <f ca="1"/>
-        <v>0.44387199209227735</v>
+        <v>0.40066932382155351</v>
       </c>
       <c r="K102" s="8">
         <f ca="1"/>
-        <v>0.62082959941490734</v>
+        <v>0.42911037533110846</v>
       </c>
       <c r="L102" s="8">
         <f ca="1"/>
-        <v>2.1415750790994472E-3</v>
-      </c>
-    </row>
-    <row r="103" spans="9:12" x14ac:dyDescent="0.3">
+        <v>1.4290035100239334E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="9:12" x14ac:dyDescent="0.35">
       <c r="I103" s="8">
         <v>10</v>
       </c>
       <c r="J103" s="8">
         <f ca="1"/>
-        <v>0.44387199209227735</v>
+        <v>0.40066932382155351</v>
       </c>
       <c r="K103" s="8">
         <f ca="1"/>
-        <v>0.61906002334168098</v>
+        <v>0.42882596481601293</v>
       </c>
       <c r="L103" s="8">
         <f ca="1"/>
-        <v>2.0485949742964195E-3</v>
+        <v>1.3728795400756784E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5141,32 +5180,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9FF235-2370-447F-B1BD-46AD74C3D800}">
-  <dimension ref="B2:O15"/>
+  <dimension ref="B2:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="17"/>
-    <col min="3" max="3" width="17.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="17"/>
-    <col min="6" max="6" width="14.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="17"/>
-    <col min="8" max="8" width="15.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="17"/>
-    <col min="10" max="11" width="17.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="17"/>
-    <col min="13" max="13" width="14.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="9.140625" style="17"/>
-    <col min="18" max="18" width="11.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="2" width="9.109375" style="17"/>
+    <col min="3" max="3" width="17.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.109375" style="17"/>
+    <col min="6" max="6" width="9.33203125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="17"/>
+    <col min="8" max="8" width="15.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="17"/>
+    <col min="10" max="11" width="17.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" style="17"/>
+    <col min="13" max="13" width="14.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="9.109375" style="17"/>
+    <col min="18" max="18" width="11.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B2" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="18">
         <f ca="1">TODAY()</f>
@@ -5185,28 +5224,28 @@
         <v>45775</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="11" cm="1">
+        <v>24</v>
+      </c>
+      <c r="K2" s="11" t="e" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">_xll.\AKA.Bond(dated, maturity, coupon, _xll.ENUM(D5), _xll.ENUM(D6))</f>
-        <v>2510157316528</v>
-      </c>
-      <c r="M2" s="18" cm="1">
-        <f t="array" aca="1" ref="M2:M12" ca="1">_xll.AKA.Value.FlowDate(K3)</f>
-        <v>45410</v>
-      </c>
-      <c r="N2" s="17" cm="1">
-        <f t="array" aca="1" ref="N2:N12" ca="1">_xll.AKA.Value.Interest(K3)</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="17" cm="1">
-        <f t="array" aca="1" ref="O2:O12" ca="1">_xll.AKA.Value.Principal(K3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+        <v>#NAME?</v>
+      </c>
+      <c r="M2" s="18" t="e" cm="1">
+        <f t="array" aca="1" ref="M2" ca="1">_xll.AKA.Value.FlowDate(K3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N2" s="17" t="e" cm="1">
+        <f t="array" aca="1" ref="N2" ca="1">_xll.AKA.Value.Interest(K3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O2" s="17" t="e" cm="1">
+        <f t="array" aca="1" ref="O2" ca="1">_xll.AKA.Value.Principal(K3)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="18" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">_xll.TMX.DATE.ADDYEARS(dated,D3)</f>
@@ -5228,28 +5267,16 @@
         <v>46140</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="11" cm="1">
+        <v>25</v>
+      </c>
+      <c r="K3" s="11" t="e" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">_xll.\AKA.Value(K2, pvdate, pvdate)</f>
-        <v>2509338702096</v>
-      </c>
-      <c r="M3" s="18">
-        <f ca="1"/>
-        <v>45775</v>
-      </c>
-      <c r="N3" s="17">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="O3" s="17">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B4" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="19">
         <v>0.05</v>
@@ -5266,71 +5293,47 @@
         <f ca="1"/>
         <v>46505</v>
       </c>
-      <c r="M4" s="18">
-        <f ca="1"/>
-        <v>46140</v>
-      </c>
-      <c r="N4" s="17">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="O4" s="17">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="17">
+        <f ca="1"/>
+        <v>3.5072588759522785</v>
+      </c>
+      <c r="G5" s="17">
+        <f ca="1"/>
+        <v>5.083333333333333</v>
+      </c>
+      <c r="H5" s="18">
+        <f ca="1"/>
+        <v>46871</v>
+      </c>
+      <c r="J5" s="17" t="e" cm="1">
+        <f t="array" aca="1" ref="J5" ca="1">TRANSPOSE(_xll.FREQ_ENUM())</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K5" s="17" t="e" cm="1">
+        <f t="array" aca="1" ref="K5" ca="1">TRANSPOSE(_xll.DC_ENUM())</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B6" s="16" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="17">
-        <f ca="1"/>
-        <v>3.5072588759522785</v>
-      </c>
-      <c r="G5" s="17">
-        <f ca="1"/>
-        <v>5.083333333333333</v>
-      </c>
-      <c r="H5" s="18">
-        <f ca="1"/>
-        <v>46871</v>
-      </c>
-      <c r="J5" s="17" t="str" cm="1">
-        <f t="array" ref="J5:J15">TRANSPOSE(_xll.FREQ_ENUM())</f>
-        <v>FREQ_INT_AT_MATURITY</v>
-      </c>
-      <c r="K5" s="17" t="str" cm="1">
-        <f t="array" ref="K5:K14">TRANSPOSE(_xll.DC_ENUM())</f>
-        <v>DC_30_360</v>
-      </c>
-      <c r="M5" s="18">
-        <f ca="1"/>
-        <v>46505</v>
-      </c>
-      <c r="N5" s="17">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="O5" s="17">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="16" t="s">
-        <v>21</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="17">
         <f ca="1"/>
@@ -5344,28 +5347,10 @@
         <f ca="1"/>
         <v>47236</v>
       </c>
-      <c r="J6" s="17" t="str">
-        <v>FREQ_ANNUAL</v>
-      </c>
-      <c r="K6" s="17" t="str">
-        <v>DC_30E_360</v>
-      </c>
-      <c r="M6" s="18">
-        <f ca="1"/>
-        <v>46871</v>
-      </c>
-      <c r="N6" s="17">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="O6" s="17">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="17">
         <v>100</v>
@@ -5382,32 +5367,14 @@
         <f ca="1"/>
         <v>47601</v>
       </c>
-      <c r="J7" s="17" t="str">
-        <v>FREQ_SEMIANNUAL</v>
-      </c>
-      <c r="K7" s="17" t="str">
-        <v>DC_ACT_360</v>
-      </c>
-      <c r="M7" s="18">
-        <f ca="1"/>
-        <v>47236</v>
-      </c>
-      <c r="N7" s="17">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="O7" s="17">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="11" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xll.\TMX.BOND.BASIC(dated, maturity, coupon, _xll.ENUM(frequency), _xll.ENUM(day_count))</f>
-        <v>2509342831696</v>
+        <v>2273572593760</v>
       </c>
       <c r="F8" s="17">
         <f ca="1"/>
@@ -5421,28 +5388,10 @@
         <f ca="1"/>
         <v>47966</v>
       </c>
-      <c r="J8" s="17" t="str">
-        <v>FREQ_QUARTERLY</v>
-      </c>
-      <c r="K8" s="17" t="str">
-        <v>DC_ACT_365</v>
-      </c>
-      <c r="M8" s="18">
-        <f ca="1"/>
-        <v>47601</v>
-      </c>
-      <c r="N8" s="17">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="O8" s="17">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="18">
         <f ca="1">dated+D9</f>
@@ -5463,32 +5412,14 @@
         <f ca="1"/>
         <v>48332</v>
       </c>
-      <c r="J9" s="17" t="str">
-        <v>FREQ_MONTHLY</v>
-      </c>
-      <c r="K9" s="17" t="str">
-        <v>DC_ACT_ACT</v>
-      </c>
-      <c r="M9" s="18">
-        <f ca="1"/>
-        <v>47966</v>
-      </c>
-      <c r="N9" s="17">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="O9" s="17">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B10" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="11" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">_xll.\TMX.BOND.BASIC.INSTRUMENT(bond_basic,pvdate)</f>
-        <v>2509955577872</v>
+        <v>2273345526544</v>
       </c>
       <c r="F10" s="17">
         <f ca="1"/>
@@ -5502,26 +5433,8 @@
         <f ca="1"/>
         <v>48697</v>
       </c>
-      <c r="J10" s="17" t="str">
-        <v>FREQ_SEMIANNUAL_COMPOUNDED</v>
-      </c>
-      <c r="K10" s="17" t="str">
-        <v>DC_CD_365</v>
-      </c>
-      <c r="M10" s="18">
-        <f ca="1"/>
-        <v>48332</v>
-      </c>
-      <c r="N10" s="17">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="O10" s="17">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="F11" s="17">
         <f ca="1"/>
         <v>9.5060131282640992</v>
@@ -5533,65 +5446,6 @@
       <c r="H11" s="18">
         <f ca="1"/>
         <v>49062</v>
-      </c>
-      <c r="J11" s="17" t="str">
-        <v>FREQ_QUARTERLY_COMPOUNDED</v>
-      </c>
-      <c r="K11" s="17" t="str">
-        <v>DC_30_360_ISDA</v>
-      </c>
-      <c r="M11" s="18">
-        <f ca="1"/>
-        <v>48697</v>
-      </c>
-      <c r="N11" s="17">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="O11" s="17">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="J12" s="17" t="str">
-        <v>FREQ_ANNUAL_BY_WEEKS</v>
-      </c>
-      <c r="K12" s="17" t="str">
-        <v>DC_30E_360_ISDA</v>
-      </c>
-      <c r="M12" s="18">
-        <f ca="1"/>
-        <v>49062</v>
-      </c>
-      <c r="N12" s="17">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="O12" s="17">
-        <f ca="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="J13" s="17" t="str">
-        <v>FREQ_SEMIANNUAL_BY_WEEKS</v>
-      </c>
-      <c r="K13" s="17" t="str">
-        <v>DC_NO_LEAP_365</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="J14" s="17" t="str">
-        <v>FREQ_QUARTERLY_BY_WEEKS</v>
-      </c>
-      <c r="K14" s="17" t="str">
-        <v>DC_BUS_252</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="J15" s="17" t="str">
-        <v>FREQ_MONTHLY_BY_WEEKS</v>
       </c>
     </row>
   </sheetData>
@@ -5624,4 +5478,266 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EAD57E-B813-416C-A1C4-B7528B2439C2}">
+  <dimension ref="B2:H24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="21">
+        <f ca="1">TODAY()</f>
+        <v>45410</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="11" cm="1">
+        <f t="array" aca="1" ref="C3" ca="1">_xll.\TMX.BOND.BASIC(pvdate,10)</f>
+        <v>2273572596336</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="11" cm="1">
+        <f t="array" aca="1" ref="C4" ca="1">_xll.\TMX.BOND.BASIC.INSTRUMENT(bond,pvdate)</f>
+        <v>2273345526368</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C5" cm="1">
+        <f t="array" aca="1" ref="C5:D24" ca="1">_xll.TMX.INSTRUMENT(C4)</f>
+        <v>0.50103698227889693</v>
+      </c>
+      <c r="D5">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="H5" t="e" cm="1">
+        <f t="array" ref="H5">_xll.TMX.CURVE.PWFLAT.FORWARD(G2,C5)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <f ca="1"/>
+        <v>0.99933605755080523</v>
+      </c>
+      <c r="D6">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f ca="1"/>
+        <v>1.5003730398297022</v>
+      </c>
+      <c r="D7">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <f ca="1"/>
+        <v>1.9986721151016105</v>
+      </c>
+      <c r="D8">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <f ca="1"/>
+        <v>2.4997090973805074</v>
+      </c>
+      <c r="D9">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <f ca="1"/>
+        <v>2.9980081726524159</v>
+      </c>
+      <c r="D10">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <f ca="1"/>
+        <v>3.4990451549313129</v>
+      </c>
+      <c r="D11">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <f ca="1"/>
+        <v>4.0000821372102093</v>
+      </c>
+      <c r="D12">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <f ca="1"/>
+        <v>4.5011191194891067</v>
+      </c>
+      <c r="D13">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <f ca="1"/>
+        <v>4.9994181947610148</v>
+      </c>
+      <c r="D14">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <f ca="1"/>
+        <v>5.5004551770399122</v>
+      </c>
+      <c r="D15">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <f ca="1"/>
+        <v>5.9987542523118202</v>
+      </c>
+      <c r="D16">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <f ca="1"/>
+        <v>6.4997912345907167</v>
+      </c>
+      <c r="D17">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <f ca="1"/>
+        <v>6.9980903098626257</v>
+      </c>
+      <c r="D18">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <f ca="1"/>
+        <v>7.4991272921415222</v>
+      </c>
+      <c r="D19">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <f ca="1"/>
+        <v>8.0001642744204187</v>
+      </c>
+      <c r="D20">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f ca="1"/>
+        <v>8.501201256699316</v>
+      </c>
+      <c r="D21">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f ca="1"/>
+        <v>8.999500331971225</v>
+      </c>
+      <c r="D22">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <f ca="1"/>
+        <v>9.5005373142501224</v>
+      </c>
+      <c r="D23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <f ca="1"/>
+        <v>9.9988363895220296</v>
+      </c>
+      <c r="D24">
+        <f ca="1"/>
+        <v>102.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bond -> inastrument_bond excel_clock
</commit_message>
<xml_diff>
--- a/bondxll.xlsx
+++ b/bondxll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\source\repos\tmcrossx\bondxll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF9A12B-AA35-4905-AC66-6124ABD01521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D66D49-59E8-4FA5-936C-D4A7BEDD67F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3585" yWindow="1665" windowWidth="32415" windowHeight="17685" activeTab="4" xr2:uid="{B41655E8-20ED-4B49-A343-A4ADF5D922ED}"/>
   </bookViews>
@@ -428,7 +428,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -492,6 +492,7 @@
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -906,307 +907,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.13576598236086435</c:v>
+                  <c:v>0.64889800400870623</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.13576598236086435</c:v>
+                  <c:v>0.64889800400870623</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.13576598236086435</c:v>
+                  <c:v>0.64889800400870623</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.13576598236086435</c:v>
+                  <c:v>0.64889800400870623</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.13576598236086435</c:v>
+                  <c:v>0.64889800400870623</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.13576598236086435</c:v>
+                  <c:v>0.64889800400870623</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.13576598236086435</c:v>
+                  <c:v>0.64889800400870623</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.13576598236086435</c:v>
+                  <c:v>0.64889800400870623</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.13576598236086435</c:v>
+                  <c:v>0.64889800400870623</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.13576598236086435</c:v>
+                  <c:v>0.64889800400870623</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.98790496237513259</c:v>
+                  <c:v>0.45380318968065492</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.98790496237513259</c:v>
+                  <c:v>0.45380318968065492</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.98790496237513259</c:v>
+                  <c:v>0.45380318968065492</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.98790496237513259</c:v>
+                  <c:v>0.45380318968065492</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.98790496237513259</c:v>
+                  <c:v>0.45380318968065492</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.98790496237513259</c:v>
+                  <c:v>0.45380318968065492</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.98790496237513259</c:v>
+                  <c:v>0.45380318968065492</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.98790496237513259</c:v>
+                  <c:v>0.45380318968065492</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.98790496237513259</c:v>
+                  <c:v>0.45380318968065492</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.98790496237513259</c:v>
+                  <c:v>0.45380318968065492</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.43194729349529037</c:v>
+                  <c:v>0.21048511246585933</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.43194729349529037</c:v>
+                  <c:v>0.21048511246585933</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.43194729349529037</c:v>
+                  <c:v>0.21048511246585933</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.43194729349529037</c:v>
+                  <c:v>0.21048511246585933</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.43194729349529037</c:v>
+                  <c:v>0.21048511246585933</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.43194729349529037</c:v>
+                  <c:v>0.21048511246585933</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.43194729349529037</c:v>
+                  <c:v>0.21048511246585933</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.43194729349529037</c:v>
+                  <c:v>0.21048511246585933</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.43194729349529037</c:v>
+                  <c:v>0.21048511246585933</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.43194729349529037</c:v>
+                  <c:v>0.21048511246585933</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.62138664627289697</c:v>
+                  <c:v>5.8698200570927339E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.62138664627289697</c:v>
+                  <c:v>5.8698200570927339E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.62138664627289697</c:v>
+                  <c:v>5.8698200570927339E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.62138664627289697</c:v>
+                  <c:v>5.8698200570927339E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.62138664627289697</c:v>
+                  <c:v>5.8698200570927339E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.62138664627289697</c:v>
+                  <c:v>5.8698200570927339E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.62138664627289697</c:v>
+                  <c:v>5.8698200570927339E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.62138664627289697</c:v>
+                  <c:v>5.8698200570927339E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.62138664627289697</c:v>
+                  <c:v>5.8698200570927339E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.62138664627289697</c:v>
+                  <c:v>5.8698200570927339E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.27089298674800433</c:v>
+                  <c:v>0.81697990723956559</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.27089298674800433</c:v>
+                  <c:v>0.81697990723956559</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.27089298674800433</c:v>
+                  <c:v>0.81697990723956559</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.27089298674800433</c:v>
+                  <c:v>0.81697990723956559</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.27089298674800433</c:v>
+                  <c:v>0.81697990723956559</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.27089298674800433</c:v>
+                  <c:v>0.81697990723956559</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.27089298674800433</c:v>
+                  <c:v>0.81697990723956559</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.27089298674800433</c:v>
+                  <c:v>0.81697990723956559</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.27089298674800433</c:v>
+                  <c:v>0.81697990723956559</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.27089298674800433</c:v>
+                  <c:v>0.81697990723956559</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.50729570832494009</c:v>
+                  <c:v>0.33923522652932059</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.50729570832494009</c:v>
+                  <c:v>0.33923522652932059</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.50729570832494009</c:v>
+                  <c:v>0.33923522652932059</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.50729570832494009</c:v>
+                  <c:v>0.33923522652932059</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.50729570832494009</c:v>
+                  <c:v>0.33923522652932059</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.50729570832494009</c:v>
+                  <c:v>0.33923522652932059</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.50729570832494009</c:v>
+                  <c:v>0.33923522652932059</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.50729570832494009</c:v>
+                  <c:v>0.33923522652932059</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.50729570832494009</c:v>
+                  <c:v>0.33923522652932059</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.50729570832494009</c:v>
+                  <c:v>0.33923522652932059</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.64016095181935651</c:v>
+                  <c:v>0.62733293516835054</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.64016095181935651</c:v>
+                  <c:v>0.62733293516835054</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.64016095181935651</c:v>
+                  <c:v>0.62733293516835054</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.64016095181935651</c:v>
+                  <c:v>0.62733293516835054</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.64016095181935651</c:v>
+                  <c:v>0.62733293516835054</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.64016095181935651</c:v>
+                  <c:v>0.62733293516835054</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.64016095181935651</c:v>
+                  <c:v>0.62733293516835054</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.64016095181935651</c:v>
+                  <c:v>0.62733293516835054</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.64016095181935651</c:v>
+                  <c:v>0.62733293516835054</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.64016095181935651</c:v>
+                  <c:v>0.62733293516835054</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.29006265836598133</c:v>
+                  <c:v>0.67523521635063011</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.29006265836598133</c:v>
+                  <c:v>0.67523521635063011</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.29006265836598133</c:v>
+                  <c:v>0.67523521635063011</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.29006265836598133</c:v>
+                  <c:v>0.67523521635063011</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.29006265836598133</c:v>
+                  <c:v>0.67523521635063011</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.29006265836598133</c:v>
+                  <c:v>0.67523521635063011</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.29006265836598133</c:v>
+                  <c:v>0.67523521635063011</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.29006265836598133</c:v>
+                  <c:v>0.67523521635063011</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.29006265836598133</c:v>
+                  <c:v>0.67523521635063011</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.29006265836598133</c:v>
+                  <c:v>0.67523521635063011</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.99292478307626375</c:v>
+                  <c:v>0.89987586081846582</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.99292478307626375</c:v>
+                  <c:v>0.89987586081846582</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.99292478307626375</c:v>
+                  <c:v>0.89987586081846582</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.99292478307626375</c:v>
+                  <c:v>0.89987586081846582</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.99292478307626375</c:v>
+                  <c:v>0.89987586081846582</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.99292478307626375</c:v>
+                  <c:v>0.89987586081846582</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.99292478307626375</c:v>
+                  <c:v>0.89987586081846582</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.99292478307626375</c:v>
+                  <c:v>0.89987586081846582</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.99292478307626375</c:v>
+                  <c:v>0.89987586081846582</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.99292478307626375</c:v>
+                  <c:v>0.89987586081846582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1563,307 +1564,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83955157724683815</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83955157724683815</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.83955157724683815</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.83955157724683815</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.83955157724683804</c:v>
+                  <c:v>0.14270304597466366</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.77557106862084046</c:v>
+                  <c:v>0.18872076943230393</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.72225397809917569</c:v>
+                  <c:v>0.22706887231367079</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.67713951688853646</c:v>
+                  <c:v>0.25951726705944272</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.63846997870798838</c:v>
+                  <c:v>0.287330176841533</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.60495637895151344</c:v>
+                  <c:v>0.31143469865267787</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.57563197916459785</c:v>
+                  <c:v>0.33252615523742962</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.54975750876437823</c:v>
+                  <c:v>0.3511362639886812</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.52675797951973857</c:v>
+                  <c:v>0.3676785828786826</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.50617945335348213</c:v>
+                  <c:v>0.38247960504342066</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.48765877980385119</c:v>
+                  <c:v>0.39580052499168494</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.51148002659295988</c:v>
+                  <c:v>0.39856255664354062</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.5331357054921495</c:v>
+                  <c:v>0.40107349450886404</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.55290828187836616</c:v>
+                  <c:v>0.40336608995111584</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.57103314356573154</c:v>
+                  <c:v>0.40546763577317996</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.58770801631810754</c:v>
+                  <c:v>0.40740105792947895</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.60310020655106999</c:v>
+                  <c:v>0.40918575530452417</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.61735223454455379</c:v>
+                  <c:v>0.41083825287401049</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.63058626053850309</c:v>
+                  <c:v>0.41237271490281918</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.64290759508459383</c:v>
+                  <c:v>0.41380135196412393</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.65440750732761166</c:v>
+                  <c:v>0.41513474655467492</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.64723137139753684</c:v>
+                  <c:v>0.40853314545503572</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.64050374396309151</c:v>
+                  <c:v>0.40234414442412392</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.63418385152467327</c:v>
+                  <c:v>0.39653023436478263</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.62823571746498563</c:v>
+                  <c:v>0.39105831901481425</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.6226274767801373</c:v>
+                  <c:v>0.38589908454198696</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.61733080502222482</c:v>
+                  <c:v>0.38102647420653901</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.61232043984582107</c:v>
+                  <c:v>0.37641724821354766</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.60757377809975455</c:v>
+                  <c:v>0.3720506130622927</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.60307053490476836</c:v>
+                  <c:v>0.36790790791879441</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.59879245386953128</c:v>
+                  <c:v>0.36397233803247103</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.59934353173302801</c:v>
+                  <c:v>0.35652662736267726</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.59986836779350106</c:v>
+                  <c:v>0.34943547434382605</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.60036879287441725</c:v>
+                  <c:v>0.34267414239561916</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.60084647136074643</c:v>
+                  <c:v>0.33622014371778525</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.60130291969212746</c:v>
+                  <c:v>0.33005298942563283</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.60173952244388329</c:v>
+                  <c:v>0.32415397227661746</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.60215754635513896</c:v>
+                  <c:v>0.31850597713394324</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.60255815260342549</c:v>
+                  <c:v>0.31309331512221372</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.60294240757627193</c:v>
+                  <c:v>0.30790157809055479</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.60331129235020442</c:v>
+                  <c:v>0.3029175105401623</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.59679328635800433</c:v>
+                  <c:v>0.31299716537740557</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.59052597290396591</c:v>
+                  <c:v>0.32268914118244707</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.58449516184441941</c:v>
+                  <c:v>0.33201538205144937</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.5786877141574488</c:v>
+                  <c:v>0.34099620659196994</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.573091446386368</c:v>
+                  <c:v>0.34965045569465353</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.56769504532139714</c:v>
+                  <c:v>0.35799562447224126</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.56248799166221486</c:v>
+                  <c:v>0.36604798031026448</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.55746049157748712</c:v>
+                  <c:v>0.37382266870559727</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.552603415224445</c:v>
+                  <c:v>0.38133380834176622</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.54790824141650429</c:v>
+                  <c:v>0.38859457665672953</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.5472424621854951</c:v>
+                  <c:v>0.38778540698250968</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.54659815970387315</c:v>
+                  <c:v>0.3870023395558454</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.54597431126928697</c:v>
+                  <c:v>0.38624413141256719</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.54536995809828159</c:v>
+                  <c:v>0.38550961727376643</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.54478420040946096</c:v>
+                  <c:v>0.3847977035700057</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.54421619295363488</c:v>
+                  <c:v>0.38410736300878329</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.54366514094425133</c:v>
+                  <c:v>0.38343762962849276</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.54313029634690857</c:v>
+                  <c:v>0.38278759428879905</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.54261095449151775</c:v>
+                  <c:v>0.38215640055315447</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.54210645097485233</c:v>
+                  <c:v>0.38154324092424252</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.54348750028252135</c:v>
+                  <c:v>0.38500506760373704</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.54483018710942188</c:v>
+                  <c:v>0.38837073243102332</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.54613608799585933</c:v>
+                  <c:v>0.39164418726304145</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.54740669426374444</c:v>
+                  <c:v>0.39482917034284298</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.54864341769781932</c:v>
+                  <c:v>0.39792922054051638</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.54984759577836584</c:v>
+                  <c:v>0.40094769046983003</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.5510204965061708</c:v>
+                  <c:v>0.4038877585827978</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.55216332285633996</c:v>
+                  <c:v>0.40675244033389463</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.55327721689384646</c:v>
+                  <c:v>0.4095445984963561</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.55436326358041532</c:v>
+                  <c:v>0.412266952704756</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.55110029314566922</c:v>
+                  <c:v>0.41551347447816184</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.547916907355673</c:v>
+                  <c:v>0.4186808127936798</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.54481022965700199</c:v>
+                  <c:v>0.42177182970400445</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.54177752047496608</c:v>
+                  <c:v>0.42478925097360715</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.53881616915603681</c:v>
+                  <c:v>0.4277356740956898</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.53592368647243149</c:v>
+                  <c:v>0.43061357574981701</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.5330976976436218</c:v>
+                  <c:v>0.4334253187452286</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.53033593583364858</c:v>
+                  <c:v>0.43617315849074456</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.52763623608682086</c:v>
+                  <c:v>0.4388592490284961</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.52499652966770038</c:v>
+                  <c:v>0.44148564866540868</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.53013859838647581</c:v>
+                  <c:v>0.44652290374401371</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.53516888300266929</c:v>
+                  <c:v>0.45145065327743172</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.54009098945507339</c:v>
+                  <c:v>0.45627242970260407</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.54490837023827765</c:v>
+                  <c:v>0.46099161514000692</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.54962433247867748</c:v>
+                  <c:v>0.46561144930504328</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.55424204550573564</c:v>
+                  <c:v>0.47013503692497483</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.55876454795491637</c:v>
+                  <c:v>0.47456535469707262</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.5631947544357464</c:v>
+                  <c:v>0.47890525782076032</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.56753546179575165</c:v>
+                  <c:v>0.48315748613386844</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.57178935500855677</c:v>
+                  <c:v>0.48732466988071438</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3066,7 +3067,7 @@
       </c>
       <c r="E3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="G3" s="1" t="str" cm="1">
         <f t="array" ref="G3:G6">TRANSPOSE(_xll.ENUM(G2))</f>
@@ -3155,7 +3156,7 @@
       </c>
       <c r="E2" s="11" cm="1">
         <f t="array" aca="1" ref="E2" ca="1">_xll.\TMX.INSTRUMENT(_xlfn.ANCHORARRAY(B3),_xlfn.ANCHORARRAY(C3))</f>
-        <v>2424275870208</v>
+        <v>1762235819808</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
@@ -3165,7 +3166,7 @@
       </c>
       <c r="C3" s="13" cm="1">
         <f t="array" aca="1" ref="C3:C12" ca="1">_xlfn.RANDARRAY(B2,1)</f>
-        <v>0.6132626960585803</v>
+        <v>0.25738384178428064</v>
       </c>
       <c r="E3" s="13" cm="1">
         <f t="array" aca="1" ref="E3:F12" ca="1">_xll.TMX.INSTRUMENT(E2)</f>
@@ -3173,7 +3174,7 @@
       </c>
       <c r="F3" s="13">
         <f ca="1"/>
-        <v>0.6132626960585803</v>
+        <v>0.25738384178428064</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -3182,7 +3183,7 @@
       </c>
       <c r="C4" s="13">
         <f ca="1"/>
-        <v>0.24428501223752686</v>
+        <v>0.92873519737266763</v>
       </c>
       <c r="E4" s="13">
         <f ca="1"/>
@@ -3190,7 +3191,7 @@
       </c>
       <c r="F4" s="13">
         <f ca="1"/>
-        <v>0.24428501223752686</v>
+        <v>0.92873519737266763</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -3199,7 +3200,7 @@
       </c>
       <c r="C5" s="13">
         <f ca="1"/>
-        <v>0.15723591662069514</v>
+        <v>0.33857070081028562</v>
       </c>
       <c r="E5" s="13">
         <f ca="1"/>
@@ -3207,7 +3208,7 @@
       </c>
       <c r="F5" s="13">
         <f ca="1"/>
-        <v>0.15723591662069514</v>
+        <v>0.33857070081028562</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -3216,7 +3217,7 @@
       </c>
       <c r="C6" s="13">
         <f ca="1"/>
-        <v>0.35970348262696916</v>
+        <v>0.93818866730402761</v>
       </c>
       <c r="E6" s="13">
         <f ca="1"/>
@@ -3224,7 +3225,7 @@
       </c>
       <c r="F6" s="13">
         <f ca="1"/>
-        <v>0.35970348262696916</v>
+        <v>0.93818866730402761</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -3233,7 +3234,7 @@
       </c>
       <c r="C7" s="13">
         <f ca="1"/>
-        <v>0.42146289193856235</v>
+        <v>0.43159435295837389</v>
       </c>
       <c r="E7" s="13">
         <f ca="1"/>
@@ -3241,7 +3242,7 @@
       </c>
       <c r="F7" s="13">
         <f ca="1"/>
-        <v>0.42146289193856235</v>
+        <v>0.43159435295837389</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -3250,7 +3251,7 @@
       </c>
       <c r="C8" s="13">
         <f ca="1"/>
-        <v>0.13380963858617623</v>
+        <v>0.31056102145971054</v>
       </c>
       <c r="E8" s="13">
         <f ca="1"/>
@@ -3258,7 +3259,7 @@
       </c>
       <c r="F8" s="13">
         <f ca="1"/>
-        <v>0.13380963858617623</v>
+        <v>0.31056102145971054</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -3267,7 +3268,7 @@
       </c>
       <c r="C9" s="13">
         <f ca="1"/>
-        <v>0.13979392580150751</v>
+        <v>0.94944724384164414</v>
       </c>
       <c r="E9" s="13">
         <f ca="1"/>
@@ -3275,7 +3276,7 @@
       </c>
       <c r="F9" s="13">
         <f ca="1"/>
-        <v>0.13979392580150751</v>
+        <v>0.94944724384164414</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
@@ -3284,7 +3285,7 @@
       </c>
       <c r="C10" s="13">
         <f ca="1"/>
-        <v>0.77970734486749382</v>
+        <v>7.687113598929507E-2</v>
       </c>
       <c r="E10" s="13">
         <f ca="1"/>
@@ -3292,7 +3293,7 @@
       </c>
       <c r="F10" s="13">
         <f ca="1"/>
-        <v>0.77970734486749382</v>
+        <v>7.687113598929507E-2</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
@@ -3301,7 +3302,7 @@
       </c>
       <c r="C11" s="13">
         <f ca="1"/>
-        <v>9.5467293576763979E-2</v>
+        <v>0.25402193878181634</v>
       </c>
       <c r="E11" s="13">
         <f ca="1"/>
@@ -3309,7 +3310,7 @@
       </c>
       <c r="F11" s="13">
         <f ca="1"/>
-        <v>9.5467293576763979E-2</v>
+        <v>0.25402193878181634</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
@@ -3318,7 +3319,7 @@
       </c>
       <c r="C12" s="13">
         <f ca="1"/>
-        <v>0.25970554895019315</v>
+        <v>0.66554898175000443</v>
       </c>
       <c r="E12" s="13">
         <f ca="1"/>
@@ -3326,7 +3327,7 @@
       </c>
       <c r="F12" s="13">
         <f ca="1"/>
-        <v>0.25970554895019315</v>
+        <v>0.66554898175000443</v>
       </c>
     </row>
   </sheetData>
@@ -3365,7 +3366,7 @@
       </c>
       <c r="F2" s="11" cm="1">
         <f t="array" aca="1" ref="F2" ca="1">_xll.\TMX.CURVE.PWFLAT(_xlfn.ANCHORARRAY(B3),_xlfn.ANCHORARRAY(C3))</f>
-        <v>2424279499248</v>
+        <v>1762170651824</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>14</v>
@@ -3381,7 +3382,7 @@
       </c>
       <c r="M2" s="21" cm="1">
         <f t="array" aca="1" ref="M2" ca="1">_xll.\TMX.CURVE.CONSTANT(C3)</f>
-        <v>2424279498528</v>
+        <v>1762170646784</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
@@ -3391,7 +3392,7 @@
       </c>
       <c r="C3" s="8" cm="1">
         <f t="array" aca="1" ref="C3:C12" ca="1">_xlfn.RANDARRAY(ROWS(_xlfn.ANCHORARRAY(B3)))</f>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="F3" s="8" cm="1">
         <f t="array" aca="1" ref="F3:G13" ca="1">TRANSPOSE(_xll.TMX.CURVE.PWFLAT(F2))</f>
@@ -3399,7 +3400,7 @@
       </c>
       <c r="G3" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="I3" s="8" cm="1">
         <f t="array" ref="I3:I103">_xll.ARRAY.SEQUENCE(0,D2,0.1)</f>
@@ -3407,11 +3408,11 @@
       </c>
       <c r="J3" s="8" cm="1">
         <f t="array" aca="1" ref="J3:J103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY($I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.FORWARD(pwflat,_xlpm.t)))</f>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="K3" s="8" cm="1">
         <f t="array" aca="1" ref="K3:K103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY($I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.SPOT(pwflat,_xlpm.t)))</f>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="L3" s="8" cm="1">
         <f t="array" aca="1" ref="L3:L103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY($I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.DISCOUNT(pwflat,_xlpm.t)))</f>
@@ -3419,7 +3420,7 @@
       </c>
       <c r="M3" s="22" cm="1">
         <f t="array" aca="1" ref="M3:M103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.FORWARD(M2,_xlpm.t)))</f>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
@@ -3428,7 +3429,7 @@
       </c>
       <c r="C4" s="8">
         <f ca="1"/>
-        <v>0.13576598236086435</v>
+        <v>0.64889800400870623</v>
       </c>
       <c r="F4" s="8">
         <f ca="1"/>
@@ -3436,26 +3437,26 @@
       </c>
       <c r="G4" s="8">
         <f ca="1"/>
-        <v>0.13576598236086435</v>
+        <v>0.64889800400870623</v>
       </c>
       <c r="I4" s="8">
         <v>0.1</v>
       </c>
       <c r="J4" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="K4" s="8">
         <f ca="1"/>
-        <v>0.83955157724683815</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="L4" s="8">
         <f ca="1"/>
-        <v>0.91947248641484092</v>
+        <v>0.98583103358917079</v>
       </c>
       <c r="M4" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
@@ -3464,7 +3465,7 @@
       </c>
       <c r="C5" s="8">
         <f ca="1"/>
-        <v>0.98790496237513259</v>
+        <v>0.45380318968065492</v>
       </c>
       <c r="F5" s="8">
         <f ca="1"/>
@@ -3472,26 +3473,26 @@
       </c>
       <c r="G5" s="8">
         <f ca="1"/>
-        <v>0.98790496237513259</v>
+        <v>0.45380318968065492</v>
       </c>
       <c r="I5" s="8">
         <v>0.2</v>
       </c>
       <c r="J5" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="K5" s="8">
         <f ca="1"/>
-        <v>0.83955157724683815</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="L5" s="8">
         <f ca="1"/>
-        <v>0.8454296532478911</v>
+        <v>0.97186282677704483</v>
       </c>
       <c r="M5" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
@@ -3500,7 +3501,7 @@
       </c>
       <c r="C6" s="8">
         <f ca="1"/>
-        <v>0.43194729349529037</v>
+        <v>0.21048511246585933</v>
       </c>
       <c r="F6" s="8">
         <f ca="1"/>
@@ -3508,26 +3509,26 @@
       </c>
       <c r="G6" s="8">
         <f ca="1"/>
-        <v>0.43194729349529037</v>
+        <v>0.21048511246585933</v>
       </c>
       <c r="I6" s="8">
         <v>0.30000000000000004</v>
       </c>
       <c r="J6" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="K6" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="L6" s="8">
         <f ca="1"/>
-        <v>0.77734930497927035</v>
+        <v>0.95809253501596436</v>
       </c>
       <c r="M6" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
@@ -3536,7 +3537,7 @@
       </c>
       <c r="C7" s="8">
         <f ca="1"/>
-        <v>0.62138664627289697</v>
+        <v>5.8698200570927339E-2</v>
       </c>
       <c r="F7" s="8">
         <f ca="1"/>
@@ -3544,26 +3545,26 @@
       </c>
       <c r="G7" s="8">
         <f ca="1"/>
-        <v>0.62138664627289697</v>
+        <v>5.8698200570927339E-2</v>
       </c>
       <c r="I7" s="8">
         <v>0.4</v>
       </c>
       <c r="J7" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="K7" s="8">
         <f ca="1"/>
-        <v>0.83955157724683815</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="L7" s="8">
         <f ca="1"/>
-        <v>0.71475129876167642</v>
+        <v>0.94451735402486769</v>
       </c>
       <c r="M7" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
@@ -3572,7 +3573,7 @@
       </c>
       <c r="C8" s="8">
         <f ca="1"/>
-        <v>0.27089298674800433</v>
+        <v>0.81697990723956559</v>
       </c>
       <c r="F8" s="8">
         <f ca="1"/>
@@ -3580,26 +3581,26 @@
       </c>
       <c r="G8" s="8">
         <f ca="1"/>
-        <v>0.27089298674800433</v>
+        <v>0.81697990723956559</v>
       </c>
       <c r="I8" s="8">
         <v>0.5</v>
       </c>
       <c r="J8" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="K8" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="L8" s="8">
         <f ca="1"/>
-        <v>0.65719415365826372</v>
+        <v>0.93113451940542735</v>
       </c>
       <c r="M8" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
@@ -3608,7 +3609,7 @@
       </c>
       <c r="C9" s="8">
         <f ca="1"/>
-        <v>0.50729570832494009</v>
+        <v>0.33923522652932059</v>
       </c>
       <c r="F9" s="8">
         <f ca="1"/>
@@ -3616,26 +3617,26 @@
       </c>
       <c r="G9" s="8">
         <f ca="1"/>
-        <v>0.50729570832494009</v>
+        <v>0.33923522652932059</v>
       </c>
       <c r="I9" s="8">
         <v>0.60000000000000009</v>
       </c>
       <c r="J9" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="K9" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="L9" s="8">
         <f ca="1"/>
-        <v>0.60427194228198278</v>
+        <v>0.91794130567622434</v>
       </c>
       <c r="M9" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
@@ -3644,7 +3645,7 @@
       </c>
       <c r="C10" s="8">
         <f ca="1"/>
-        <v>0.64016095181935651</v>
+        <v>0.62733293516835054</v>
       </c>
       <c r="F10" s="8">
         <f ca="1"/>
@@ -3652,26 +3653,26 @@
       </c>
       <c r="G10" s="8">
         <f ca="1"/>
-        <v>0.64016095181935651</v>
+        <v>0.62733293516835054</v>
       </c>
       <c r="I10" s="8">
         <v>0.70000000000000007</v>
       </c>
       <c r="J10" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="K10" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="L10" s="8">
         <f ca="1"/>
-        <v>0.55561142556104004</v>
+        <v>0.90493502615738897</v>
       </c>
       <c r="M10" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
@@ -3680,7 +3681,7 @@
       </c>
       <c r="C11" s="8">
         <f ca="1"/>
-        <v>0.29006265836598133</v>
+        <v>0.67523521635063011</v>
       </c>
       <c r="F11" s="8">
         <f ca="1"/>
@@ -3688,26 +3689,26 @@
       </c>
       <c r="G11" s="8">
         <f ca="1"/>
-        <v>0.29006265836598133</v>
+        <v>0.67523521635063011</v>
       </c>
       <c r="I11" s="8">
         <v>0.8</v>
       </c>
       <c r="J11" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="K11" s="8">
         <f ca="1"/>
-        <v>0.83955157724683815</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="L11" s="8">
         <f ca="1"/>
-        <v>0.51086941917207185</v>
+        <v>0.89211303219359572</v>
       </c>
       <c r="M11" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
@@ -3716,7 +3717,7 @@
       </c>
       <c r="C12" s="8">
         <f ca="1"/>
-        <v>0.99292478307626375</v>
+        <v>0.89987586081846582</v>
       </c>
       <c r="F12" s="8">
         <f ca="1"/>
@@ -3724,26 +3725,26 @@
       </c>
       <c r="G12" s="8">
         <f ca="1"/>
-        <v>0.99292478307626375</v>
+        <v>0.89987586081846582</v>
       </c>
       <c r="I12" s="8">
         <v>0.9</v>
       </c>
       <c r="J12" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="K12" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="L12" s="8">
         <f ca="1"/>
-        <v>0.4697303747345678</v>
+        <v>0.87947271266521065</v>
       </c>
       <c r="M12" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
@@ -3760,19 +3761,19 @@
       </c>
       <c r="J13" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="K13" s="8">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
       <c r="L13" s="8">
         <f ca="1"/>
-        <v>0.43190415542146815</v>
+        <v>0.86701149345984174</v>
       </c>
       <c r="M13" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
@@ -3781,19 +3782,19 @@
       </c>
       <c r="J14" s="8">
         <f ca="1"/>
-        <v>0.13576598236086435</v>
+        <v>0.64889800400870623</v>
       </c>
       <c r="K14" s="8">
         <f ca="1"/>
-        <v>0.77557106862084046</v>
+        <v>0.18872076943230393</v>
       </c>
       <c r="L14" s="8">
         <f ca="1"/>
-        <v>0.42607999179807854</v>
+        <v>0.81253779699771611</v>
       </c>
       <c r="M14" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
@@ -3802,19 +3803,19 @@
       </c>
       <c r="J15" s="8">
         <f ca="1"/>
-        <v>0.13576598236086435</v>
+        <v>0.64889800400870623</v>
       </c>
       <c r="K15" s="8">
         <f ca="1"/>
-        <v>0.72225397809917569</v>
+        <v>0.22706887231367079</v>
       </c>
       <c r="L15" s="8">
         <f ca="1"/>
-        <v>0.4203343661482466</v>
+        <v>0.76148664333074867</v>
       </c>
       <c r="M15" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
@@ -3823,19 +3824,19 @@
       </c>
       <c r="J16" s="8">
         <f ca="1"/>
-        <v>0.13576598236086435</v>
+        <v>0.64889800400870623</v>
       </c>
       <c r="K16" s="8">
         <f ca="1"/>
-        <v>0.67713951688853646</v>
+        <v>0.25951726705944272</v>
       </c>
       <c r="L16" s="8">
         <f ca="1"/>
-        <v>0.41466621939726506</v>
+        <v>0.71364299623085847</v>
       </c>
       <c r="M16" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="17" spans="9:13" x14ac:dyDescent="0.3">
@@ -3844,19 +3845,19 @@
       </c>
       <c r="J17" s="8">
         <f ca="1"/>
-        <v>0.13576598236086435</v>
+        <v>0.64889800400870623</v>
       </c>
       <c r="K17" s="8">
         <f ca="1"/>
-        <v>0.63846997870798838</v>
+        <v>0.287330176841533</v>
       </c>
       <c r="L17" s="8">
         <f ca="1"/>
-        <v>0.40907450675162549</v>
+        <v>0.66880533008263277</v>
       </c>
       <c r="M17" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="18" spans="9:13" x14ac:dyDescent="0.3">
@@ -3865,19 +3866,19 @@
       </c>
       <c r="J18" s="8">
         <f ca="1"/>
-        <v>0.13576598236086435</v>
+        <v>0.64889800400870623</v>
       </c>
       <c r="K18" s="8">
         <f ca="1"/>
-        <v>0.60495637895151344</v>
+        <v>0.31143469865267787</v>
       </c>
       <c r="L18" s="8">
         <f ca="1"/>
-        <v>0.40355819750640287</v>
+        <v>0.62678478167664142</v>
       </c>
       <c r="M18" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="19" spans="9:13" x14ac:dyDescent="0.3">
@@ -3886,19 +3887,19 @@
       </c>
       <c r="J19" s="8">
         <f ca="1"/>
-        <v>0.13576598236086435</v>
+        <v>0.64889800400870623</v>
       </c>
       <c r="K19" s="8">
         <f ca="1"/>
-        <v>0.57563197916459785</v>
+        <v>0.33252615523742962</v>
       </c>
       <c r="L19" s="8">
         <f ca="1"/>
-        <v>0.39811627485523299</v>
+        <v>0.58740435325197449</v>
       </c>
       <c r="M19" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="20" spans="9:13" x14ac:dyDescent="0.3">
@@ -3907,19 +3908,19 @@
       </c>
       <c r="J20" s="8">
         <f ca="1"/>
-        <v>0.13576598236086435</v>
+        <v>0.64889800400870623</v>
       </c>
       <c r="K20" s="8">
         <f ca="1"/>
-        <v>0.54975750876437823</v>
+        <v>0.3511362639886812</v>
       </c>
       <c r="L20" s="8">
         <f ca="1"/>
-        <v>0.39274773570284971</v>
+        <v>0.55049816914313776</v>
       </c>
       <c r="M20" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="21" spans="9:13" x14ac:dyDescent="0.3">
@@ -3928,19 +3929,19 @@
       </c>
       <c r="J21" s="8">
         <f ca="1"/>
-        <v>0.13576598236086435</v>
+        <v>0.64889800400870623</v>
       </c>
       <c r="K21" s="8">
         <f ca="1"/>
-        <v>0.52675797951973857</v>
+        <v>0.3676785828786826</v>
       </c>
       <c r="L21" s="8">
         <f ca="1"/>
-        <v>0.38745159048014366</v>
+        <v>0.5159107731573439</v>
       </c>
       <c r="M21" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="22" spans="9:13" x14ac:dyDescent="0.3">
@@ -3949,19 +3950,19 @@
       </c>
       <c r="J22" s="8">
         <f ca="1"/>
-        <v>0.13576598236086435</v>
+        <v>0.64889800400870623</v>
       </c>
       <c r="K22" s="8">
         <f ca="1"/>
-        <v>0.50617945335348213</v>
+        <v>0.38247960504342066</v>
       </c>
       <c r="L22" s="8">
         <f ca="1"/>
-        <v>0.38222686426896496</v>
+        <v>0.48349647818160635</v>
       </c>
       <c r="M22" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="23" spans="9:13" x14ac:dyDescent="0.3">
@@ -3970,19 +3971,19 @@
       </c>
       <c r="J23" s="8">
         <f ca="1"/>
-        <v>0.13576598236086435</v>
+        <v>0.64889800400870623</v>
       </c>
       <c r="K23" s="8">
         <f ca="1"/>
-        <v>0.48765877980385119</v>
+        <v>0.39580052499168494</v>
       </c>
       <c r="L23" s="8">
         <f ca="1"/>
-        <v>0.3770725916325845</v>
+        <v>0.45311874833502652</v>
       </c>
       <c r="M23" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="24" spans="9:13" x14ac:dyDescent="0.3">
@@ -3991,19 +3992,19 @@
       </c>
       <c r="J24" s="8">
         <f ca="1"/>
-        <v>0.98790496237513259</v>
+        <v>0.45380318968065492</v>
       </c>
       <c r="K24" s="8">
         <f ca="1"/>
-        <v>0.51148002659295988</v>
+        <v>0.39856255664354062</v>
       </c>
       <c r="L24" s="8">
         <f ca="1"/>
-        <v>0.34160231001906682</v>
+        <v>0.43301566686988746</v>
       </c>
       <c r="M24" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="25" spans="9:13" x14ac:dyDescent="0.3">
@@ -4012,19 +4013,19 @@
       </c>
       <c r="J25" s="8">
         <f ca="1"/>
-        <v>0.98790496237513259</v>
+        <v>0.45380318968065492</v>
       </c>
       <c r="K25" s="8">
         <f ca="1"/>
-        <v>0.5331357054921495</v>
+        <v>0.40107349450886404</v>
       </c>
       <c r="L25" s="8">
         <f ca="1"/>
-        <v>0.30946863023035126</v>
+        <v>0.41380447928480535</v>
       </c>
       <c r="M25" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="26" spans="9:13" x14ac:dyDescent="0.3">
@@ -4033,19 +4034,19 @@
       </c>
       <c r="J26" s="8">
         <f ca="1"/>
-        <v>0.98790496237513259</v>
+        <v>0.45380318968065492</v>
       </c>
       <c r="K26" s="8">
         <f ca="1"/>
-        <v>0.55290828187836616</v>
+        <v>0.40336608995111584</v>
       </c>
       <c r="L26" s="8">
         <f ca="1"/>
-        <v>0.2803576836581691</v>
+        <v>0.39544561572013898</v>
       </c>
       <c r="M26" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="27" spans="9:13" x14ac:dyDescent="0.3">
@@ -4054,19 +4055,19 @@
       </c>
       <c r="J27" s="8">
         <f ca="1"/>
-        <v>0.98790496237513259</v>
+        <v>0.45380318968065492</v>
       </c>
       <c r="K27" s="8">
         <f ca="1"/>
-        <v>0.57103314356573154</v>
+        <v>0.40546763577317996</v>
       </c>
       <c r="L27" s="8">
         <f ca="1"/>
-        <v>0.2539851322899358</v>
+        <v>0.37790126334063417</v>
       </c>
       <c r="M27" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="28" spans="9:13" x14ac:dyDescent="0.3">
@@ -4075,19 +4076,19 @@
       </c>
       <c r="J28" s="8">
         <f ca="1"/>
-        <v>0.98790496237513259</v>
+        <v>0.45380318968065492</v>
       </c>
       <c r="K28" s="8">
         <f ca="1"/>
-        <v>0.58770801631810754</v>
+        <v>0.40740105792947895</v>
       </c>
       <c r="L28" s="8">
         <f ca="1"/>
-        <v>0.2300933829074871</v>
+        <v>0.36113528350506807</v>
       </c>
       <c r="M28" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="29" spans="9:13" x14ac:dyDescent="0.3">
@@ -4096,19 +4097,19 @@
       </c>
       <c r="J29" s="8">
         <f ca="1"/>
-        <v>0.98790496237513259</v>
+        <v>0.45380318968065492</v>
       </c>
       <c r="K29" s="8">
         <f ca="1"/>
-        <v>0.60310020655106999</v>
+        <v>0.40918575530452417</v>
       </c>
       <c r="L29" s="8">
         <f ca="1"/>
-        <v>0.20844907041260058</v>
+        <v>0.34511314374732605</v>
       </c>
       <c r="M29" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="30" spans="9:13" x14ac:dyDescent="0.3">
@@ -4117,19 +4118,19 @@
       </c>
       <c r="J30" s="8">
         <f ca="1"/>
-        <v>0.98790496237513259</v>
+        <v>0.45380318968065492</v>
       </c>
       <c r="K30" s="8">
         <f ca="1"/>
-        <v>0.61735223454455379</v>
+        <v>0.41083825287401049</v>
       </c>
       <c r="L30" s="8">
         <f ca="1"/>
-        <v>0.18884078516862365</v>
+        <v>0.32980184287253234</v>
       </c>
       <c r="M30" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="31" spans="9:13" x14ac:dyDescent="0.3">
@@ -4138,19 +4139,19 @@
       </c>
       <c r="J31" s="8">
         <f ca="1"/>
-        <v>0.98790496237513259</v>
+        <v>0.45380318968065492</v>
       </c>
       <c r="K31" s="8">
         <f ca="1"/>
-        <v>0.63058626053850309</v>
+        <v>0.41237271490281918</v>
       </c>
       <c r="L31" s="8">
         <f ca="1"/>
-        <v>0.17107699994326819</v>
+        <v>0.31516984383832924</v>
       </c>
       <c r="M31" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="32" spans="9:13" x14ac:dyDescent="0.3">
@@ -4159,19 +4160,19 @@
       </c>
       <c r="J32" s="8">
         <f ca="1"/>
-        <v>0.98790496237513259</v>
+        <v>0.45380318968065492</v>
       </c>
       <c r="K32" s="8">
         <f ca="1"/>
-        <v>0.64290759508459383</v>
+        <v>0.41380135196412393</v>
       </c>
       <c r="L32" s="8">
         <f ca="1"/>
-        <v>0.15498421101567458</v>
+        <v>0.30118700708684903</v>
       </c>
       <c r="M32" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="33" spans="9:13" x14ac:dyDescent="0.3">
@@ -4180,19 +4181,19 @@
       </c>
       <c r="J33" s="8">
         <f ca="1"/>
-        <v>0.98790496237513259</v>
+        <v>0.45380318968065492</v>
       </c>
       <c r="K33" s="8">
         <f ca="1"/>
-        <v>0.65440750732761166</v>
+        <v>0.41513474655467492</v>
       </c>
       <c r="L33" s="8">
         <f ca="1"/>
-        <v>0.14040523240294556</v>
+        <v>0.28782453428917748</v>
       </c>
       <c r="M33" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="34" spans="9:13" x14ac:dyDescent="0.3">
@@ -4201,19 +4202,19 @@
       </c>
       <c r="J34" s="8">
         <f ca="1"/>
-        <v>0.43194729349529037</v>
+        <v>0.21048511246585933</v>
       </c>
       <c r="K34" s="8">
         <f ca="1"/>
-        <v>0.64723137139753684</v>
+        <v>0.40853314545503572</v>
       </c>
       <c r="L34" s="8">
         <f ca="1"/>
-        <v>0.13446958373748727</v>
+        <v>0.28182957014408816</v>
       </c>
       <c r="M34" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="35" spans="9:13" x14ac:dyDescent="0.3">
@@ -4222,19 +4223,19 @@
       </c>
       <c r="J35" s="8">
         <f ca="1"/>
-        <v>0.43194729349529037</v>
+        <v>0.21048511246585933</v>
       </c>
       <c r="K35" s="8">
         <f ca="1"/>
-        <v>0.64050374396309151</v>
+        <v>0.40234414442412392</v>
       </c>
       <c r="L35" s="8">
         <f ca="1"/>
-        <v>0.12878486541116502</v>
+        <v>0.27595947231833795</v>
       </c>
       <c r="M35" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="36" spans="9:13" x14ac:dyDescent="0.3">
@@ -4243,19 +4244,19 @@
       </c>
       <c r="J36" s="8">
         <f ca="1"/>
-        <v>0.43194729349529037</v>
+        <v>0.21048511246585933</v>
       </c>
       <c r="K36" s="8">
         <f ca="1"/>
-        <v>0.63418385152467327</v>
+        <v>0.39653023436478263</v>
       </c>
       <c r="L36" s="8">
         <f ca="1"/>
-        <v>0.1233404693306827</v>
+        <v>0.27021164002570558</v>
       </c>
       <c r="M36" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="37" spans="9:13" x14ac:dyDescent="0.3">
@@ -4264,19 +4265,19 @@
       </c>
       <c r="J37" s="8">
         <f ca="1"/>
-        <v>0.43194729349529037</v>
+        <v>0.21048511246585933</v>
       </c>
       <c r="K37" s="8">
         <f ca="1"/>
-        <v>0.62823571746498563</v>
+        <v>0.39105831901481425</v>
       </c>
       <c r="L37" s="8">
         <f ca="1"/>
-        <v>0.11812623586745946</v>
+        <v>0.26458352664987006</v>
       </c>
       <c r="M37" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="38" spans="9:13" x14ac:dyDescent="0.3">
@@ -4285,19 +4286,19 @@
       </c>
       <c r="J38" s="8">
         <f ca="1"/>
-        <v>0.43194729349529037</v>
+        <v>0.21048511246585933</v>
       </c>
       <c r="K38" s="8">
         <f ca="1"/>
-        <v>0.6226274767801373</v>
+        <v>0.38589908454198696</v>
       </c>
       <c r="L38" s="8">
         <f ca="1"/>
-        <v>0.11313243490066485</v>
+        <v>0.25907263861601243</v>
       </c>
       <c r="M38" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="39" spans="9:13" x14ac:dyDescent="0.3">
@@ -4306,19 +4307,19 @@
       </c>
       <c r="J39" s="8">
         <f ca="1"/>
-        <v>0.43194729349529037</v>
+        <v>0.21048511246585933</v>
       </c>
       <c r="K39" s="8">
         <f ca="1"/>
-        <v>0.61733080502222482</v>
+        <v>0.38102647420653901</v>
       </c>
       <c r="L39" s="8">
         <f ca="1"/>
-        <v>0.10834974544973064</v>
+        <v>0.25367653428590237</v>
       </c>
       <c r="M39" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="40" spans="9:13" x14ac:dyDescent="0.3">
@@ -4327,19 +4328,19 @@
       </c>
       <c r="J40" s="8">
         <f ca="1"/>
-        <v>0.43194729349529037</v>
+        <v>0.21048511246585933</v>
       </c>
       <c r="K40" s="8">
         <f ca="1"/>
-        <v>0.61232043984582107</v>
+        <v>0.37641724821354766</v>
       </c>
       <c r="L40" s="8">
         <f ca="1"/>
-        <v>0.1037692462809012</v>
+        <v>0.24839282287597697</v>
       </c>
       <c r="M40" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="41" spans="9:13" x14ac:dyDescent="0.3">
@@ -4348,19 +4349,19 @@
       </c>
       <c r="J41" s="8">
         <f ca="1"/>
-        <v>0.43194729349529037</v>
+        <v>0.21048511246585933</v>
       </c>
       <c r="K41" s="8">
         <f ca="1"/>
-        <v>0.60757377809975455</v>
+        <v>0.3720506130622927</v>
       </c>
       <c r="L41" s="8">
         <f ca="1"/>
-        <v>9.9382388245665088E-2</v>
+        <v>0.24321916339793145</v>
       </c>
       <c r="M41" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="42" spans="9:13" x14ac:dyDescent="0.3">
@@ -4369,19 +4370,19 @@
       </c>
       <c r="J42" s="8">
         <f ca="1"/>
-        <v>0.43194729349529037</v>
+        <v>0.21048511246585933</v>
       </c>
       <c r="K42" s="8">
         <f ca="1"/>
-        <v>0.60307053490476836</v>
+        <v>0.36790790791879441</v>
       </c>
       <c r="L42" s="8">
         <f ca="1"/>
-        <v>9.5180985125905102E-2</v>
+        <v>0.23815326541957219</v>
       </c>
       <c r="M42" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="43" spans="9:13" x14ac:dyDescent="0.3">
@@ -4390,19 +4391,19 @@
       </c>
       <c r="J43" s="8">
         <f ca="1"/>
-        <v>0.43194729349529037</v>
+        <v>0.21048511246585933</v>
       </c>
       <c r="K43" s="8">
         <f ca="1"/>
-        <v>0.59879245386953128</v>
+        <v>0.36397233803247103</v>
       </c>
       <c r="L43" s="8">
         <f ca="1"/>
-        <v>9.1157196772066199E-2</v>
+        <v>0.23319288126280158</v>
       </c>
       <c r="M43" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="44" spans="9:13" x14ac:dyDescent="0.3">
@@ -4411,19 +4412,19 @@
       </c>
       <c r="J44" s="8">
         <f ca="1"/>
-        <v>0.62138664627289697</v>
+        <v>5.8698200570927339E-2</v>
       </c>
       <c r="K44" s="8">
         <f ca="1"/>
-        <v>0.59934353173302801</v>
+        <v>0.35652662736267726</v>
       </c>
       <c r="L44" s="8">
         <f ca="1"/>
-        <v>8.566520909759387E-2</v>
+        <v>0.23182809048128894</v>
       </c>
       <c r="M44" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="45" spans="9:13" x14ac:dyDescent="0.3">
@@ -4432,19 +4433,19 @@
       </c>
       <c r="J45" s="8">
         <f ca="1"/>
-        <v>0.62138664627289697</v>
+        <v>5.8698200570927339E-2</v>
       </c>
       <c r="K45" s="8">
         <f ca="1"/>
-        <v>0.59986836779350106</v>
+        <v>0.34943547434382605</v>
       </c>
       <c r="L45" s="8">
         <f ca="1"/>
-        <v>8.0504101872940201E-2</v>
+        <v>0.23047128731099478</v>
       </c>
       <c r="M45" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="46" spans="9:13" x14ac:dyDescent="0.3">
@@ -4453,19 +4454,19 @@
       </c>
       <c r="J46" s="8">
         <f ca="1"/>
-        <v>0.62138664627289697</v>
+        <v>5.8698200570927339E-2</v>
       </c>
       <c r="K46" s="8">
         <f ca="1"/>
-        <v>0.60036879287441725</v>
+        <v>0.34267414239561916</v>
       </c>
       <c r="L46" s="8">
         <f ca="1"/>
-        <v>7.5653936612829528E-2</v>
+        <v>0.22912242500345673</v>
       </c>
       <c r="M46" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="47" spans="9:13" x14ac:dyDescent="0.3">
@@ -4474,19 +4475,19 @@
       </c>
       <c r="J47" s="8">
         <f ca="1"/>
-        <v>0.62138664627289697</v>
+        <v>5.8698200570927339E-2</v>
       </c>
       <c r="K47" s="8">
         <f ca="1"/>
-        <v>0.60084647136074643</v>
+        <v>0.33622014371778525</v>
       </c>
       <c r="L47" s="8">
         <f ca="1"/>
-        <v>7.1095981465107552E-2</v>
+        <v>0.22778145708381495</v>
       </c>
       <c r="M47" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="48" spans="9:13" x14ac:dyDescent="0.3">
@@ -4495,19 +4496,19 @@
       </c>
       <c r="J48" s="8">
         <f ca="1"/>
-        <v>0.62138664627289697</v>
+        <v>5.8698200570927339E-2</v>
       </c>
       <c r="K48" s="8">
         <f ca="1"/>
-        <v>0.60130291969212746</v>
+        <v>0.33005298942563283</v>
       </c>
       <c r="L48" s="8">
         <f ca="1"/>
-        <v>6.6812631574101139E-2</v>
+        <v>0.22644833734921266</v>
       </c>
       <c r="M48" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="49" spans="9:13" x14ac:dyDescent="0.3">
@@ -4516,19 +4517,19 @@
       </c>
       <c r="J49" s="8">
         <f ca="1"/>
-        <v>0.62138664627289697</v>
+        <v>5.8698200570927339E-2</v>
       </c>
       <c r="K49" s="8">
         <f ca="1"/>
-        <v>0.60173952244388329</v>
+        <v>0.32415397227661746</v>
       </c>
       <c r="L49" s="8">
         <f ca="1"/>
-        <v>6.2787342755811312E-2</v>
+        <v>0.22512301986720257</v>
       </c>
       <c r="M49" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="50" spans="9:13" x14ac:dyDescent="0.3">
@@ -4537,19 +4538,19 @@
       </c>
       <c r="J50" s="8">
         <f ca="1"/>
-        <v>0.62138664627289697</v>
+        <v>5.8698200570927339E-2</v>
       </c>
       <c r="K50" s="8">
         <f ca="1"/>
-        <v>0.60215754635513896</v>
+        <v>0.31850597713394324</v>
       </c>
       <c r="L50" s="8">
         <f ca="1"/>
-        <v>5.9004564448402019E-2</v>
+        <v>0.22380545897416573</v>
       </c>
       <c r="M50" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="51" spans="9:13" x14ac:dyDescent="0.3">
@@ -4558,19 +4559,19 @@
       </c>
       <c r="J51" s="8">
         <f ca="1"/>
-        <v>0.62138664627289697</v>
+        <v>5.8698200570927339E-2</v>
       </c>
       <c r="K51" s="8">
         <f ca="1"/>
-        <v>0.60255815260342549</v>
+        <v>0.31309331512221372</v>
       </c>
       <c r="L51" s="8">
         <f ca="1"/>
-        <v>5.5449690687658398E-2</v>
+        <v>0.2224956092737374</v>
       </c>
       <c r="M51" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="52" spans="9:13" x14ac:dyDescent="0.3">
@@ -4579,19 +4580,19 @@
       </c>
       <c r="J52" s="8">
         <f ca="1"/>
-        <v>0.62138664627289697</v>
+        <v>5.8698200570927339E-2</v>
       </c>
       <c r="K52" s="8">
         <f ca="1"/>
-        <v>0.60294240757627193</v>
+        <v>0.30790157809055479</v>
       </c>
       <c r="L52" s="8">
         <f ca="1"/>
-        <v>5.2108988825595434E-2</v>
+        <v>0.22119342563524344</v>
       </c>
       <c r="M52" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="53" spans="9:13" x14ac:dyDescent="0.3">
@@ -4600,19 +4601,19 @@
       </c>
       <c r="J53" s="8">
         <f ca="1"/>
-        <v>0.62138664627289697</v>
+        <v>5.8698200570927339E-2</v>
       </c>
       <c r="K53" s="8">
         <f ca="1"/>
-        <v>0.60331129235020442</v>
+        <v>0.3029175105401623</v>
       </c>
       <c r="L53" s="8">
         <f ca="1"/>
-        <v>4.8969555499824777E-2</v>
+        <v>0.21989886319214483</v>
       </c>
       <c r="M53" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="54" spans="9:13" x14ac:dyDescent="0.3">
@@ -4621,19 +4622,19 @@
       </c>
       <c r="J54" s="8">
         <f ca="1"/>
-        <v>0.27089298674800433</v>
+        <v>0.81697990723956559</v>
       </c>
       <c r="K54" s="8">
         <f ca="1"/>
-        <v>0.59679328635800433</v>
+        <v>0.31299716537740557</v>
       </c>
       <c r="L54" s="8">
         <f ca="1"/>
-        <v>4.7660810791740137E-2</v>
+        <v>0.20264784914543943</v>
       </c>
       <c r="M54" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="55" spans="9:13" x14ac:dyDescent="0.3">
@@ -4642,19 +4643,19 @@
       </c>
       <c r="J55" s="8">
         <f ca="1"/>
-        <v>0.27089298674800433</v>
+        <v>0.81697990723956559</v>
       </c>
       <c r="K55" s="8">
         <f ca="1"/>
-        <v>0.59052597290396591</v>
+        <v>0.32268914118244707</v>
       </c>
       <c r="L55" s="8">
         <f ca="1"/>
-        <v>4.6387043111727248E-2</v>
+        <v>0.18675017179155193</v>
       </c>
       <c r="M55" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="56" spans="9:13" x14ac:dyDescent="0.3">
@@ -4663,19 +4664,19 @@
       </c>
       <c r="J56" s="8">
         <f ca="1"/>
-        <v>0.27089298674800433</v>
+        <v>0.81697990723956559</v>
       </c>
       <c r="K56" s="8">
         <f ca="1"/>
-        <v>0.58449516184441941</v>
+        <v>0.33201538205144937</v>
       </c>
       <c r="L56" s="8">
         <f ca="1"/>
-        <v>4.514732038804678E-2</v>
+        <v>0.17209966419295855</v>
       </c>
       <c r="M56" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="57" spans="9:13" x14ac:dyDescent="0.3">
@@ -4684,19 +4685,19 @@
       </c>
       <c r="J57" s="8">
         <f ca="1"/>
-        <v>0.27089298674800433</v>
+        <v>0.81697990723956559</v>
       </c>
       <c r="K57" s="8">
         <f ca="1"/>
-        <v>0.5786877141574488</v>
+        <v>0.34099620659196994</v>
       </c>
       <c r="L57" s="8">
         <f ca="1"/>
-        <v>4.3940727879970672E-2</v>
+        <v>0.15859848528796319</v>
       </c>
       <c r="M57" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="58" spans="9:13" x14ac:dyDescent="0.3">
@@ -4705,19 +4706,19 @@
       </c>
       <c r="J58" s="8">
         <f ca="1"/>
-        <v>0.27089298674800433</v>
+        <v>0.81697990723956559</v>
       </c>
       <c r="K58" s="8">
         <f ca="1"/>
-        <v>0.573091446386368</v>
+        <v>0.34965045569465353</v>
       </c>
       <c r="L58" s="8">
         <f ca="1"/>
-        <v>4.2766382385529218E-2</v>
+        <v>0.14615647032515788</v>
       </c>
       <c r="M58" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="59" spans="9:13" x14ac:dyDescent="0.3">
@@ -4726,19 +4727,19 @@
       </c>
       <c r="J59" s="8">
         <f ca="1"/>
-        <v>0.27089298674800433</v>
+        <v>0.81697990723956559</v>
       </c>
       <c r="K59" s="8">
         <f ca="1"/>
-        <v>0.56769504532139714</v>
+        <v>0.35799562447224126</v>
       </c>
       <c r="L59" s="8">
         <f ca="1"/>
-        <v>4.1623422084216509E-2</v>
+        <v>0.13469053106877793</v>
       </c>
       <c r="M59" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="60" spans="9:13" x14ac:dyDescent="0.3">
@@ -4747,19 +4748,19 @@
       </c>
       <c r="J60" s="8">
         <f ca="1"/>
-        <v>0.27089298674800433</v>
+        <v>0.81697990723956559</v>
       </c>
       <c r="K60" s="8">
         <f ca="1"/>
-        <v>0.56248799166221486</v>
+        <v>0.36604798031026448</v>
       </c>
       <c r="L60" s="8">
         <f ca="1"/>
-        <v>4.0511008188707995E-2</v>
+        <v>0.12412409070187677</v>
       </c>
       <c r="M60" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="61" spans="9:13" x14ac:dyDescent="0.3">
@@ -4768,19 +4769,19 @@
       </c>
       <c r="J61" s="8">
         <f ca="1"/>
-        <v>0.27089298674800433</v>
+        <v>0.81697990723956559</v>
       </c>
       <c r="K61" s="8">
         <f ca="1"/>
-        <v>0.55746049157748712</v>
+        <v>0.37382266870559727</v>
       </c>
       <c r="L61" s="8">
         <f ca="1"/>
-        <v>3.9428324329355793E-2</v>
+        <v>0.11438658542810209</v>
       </c>
       <c r="M61" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="62" spans="9:13" x14ac:dyDescent="0.3">
@@ -4789,19 +4790,19 @@
       </c>
       <c r="J62" s="8">
         <f ca="1"/>
-        <v>0.27089298674800433</v>
+        <v>0.81697990723956559</v>
       </c>
       <c r="K62" s="8">
         <f ca="1"/>
-        <v>0.552603415224445</v>
+        <v>0.38133380834176622</v>
       </c>
       <c r="L62" s="8">
         <f ca="1"/>
-        <v>3.8374575955140704E-2</v>
+        <v>0.10541298299864825</v>
       </c>
       <c r="M62" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="63" spans="9:13" x14ac:dyDescent="0.3">
@@ -4810,19 +4811,19 @@
       </c>
       <c r="J63" s="8">
         <f ca="1"/>
-        <v>0.27089298674800433</v>
+        <v>0.81697990723956559</v>
       </c>
       <c r="K63" s="8">
         <f ca="1"/>
-        <v>0.54790824141650429</v>
+        <v>0.38859457665672953</v>
       </c>
       <c r="L63" s="8">
         <f ca="1"/>
-        <v>3.7348989750645746E-2</v>
+        <v>9.7143358789141168E-2</v>
       </c>
       <c r="M63" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="64" spans="9:13" x14ac:dyDescent="0.3">
@@ -4831,19 +4832,19 @@
       </c>
       <c r="J64" s="8">
         <f ca="1"/>
-        <v>0.50729570832494009</v>
+        <v>0.33923522652932059</v>
       </c>
       <c r="K64" s="8">
         <f ca="1"/>
-        <v>0.5472424621854951</v>
+        <v>0.38778540698250968</v>
       </c>
       <c r="L64" s="8">
         <f ca="1"/>
-        <v>3.550154819986779E-2</v>
+        <v>9.3903183472916013E-2</v>
       </c>
       <c r="M64" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="65" spans="9:13" x14ac:dyDescent="0.3">
@@ -4852,19 +4853,19 @@
       </c>
       <c r="J65" s="8">
         <f ca="1"/>
-        <v>0.50729570832494009</v>
+        <v>0.33923522652932059</v>
       </c>
       <c r="K65" s="8">
         <f ca="1"/>
-        <v>0.54659815970387315</v>
+        <v>0.3870023395558454</v>
       </c>
       <c r="L65" s="8">
         <f ca="1"/>
-        <v>3.3745486609613677E-2</v>
+        <v>9.0771082764411884E-2</v>
       </c>
       <c r="M65" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="66" spans="9:13" x14ac:dyDescent="0.3">
@@ -4873,19 +4874,19 @@
       </c>
       <c r="J66" s="8">
         <f ca="1"/>
-        <v>0.50729570832494009</v>
+        <v>0.33923522652932059</v>
       </c>
       <c r="K66" s="8">
         <f ca="1"/>
-        <v>0.54597431126928697</v>
+        <v>0.38624413141256719</v>
       </c>
       <c r="L66" s="8">
         <f ca="1"/>
-        <v>3.2076289189303345E-2</v>
+        <v>8.7743451868022654E-2</v>
       </c>
       <c r="M66" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="67" spans="9:13" x14ac:dyDescent="0.3">
@@ -4894,19 +4895,19 @@
       </c>
       <c r="J67" s="8">
         <f ca="1"/>
-        <v>0.50729570832494009</v>
+        <v>0.33923522652932059</v>
       </c>
       <c r="K67" s="8">
         <f ca="1"/>
-        <v>0.54536995809828159</v>
+        <v>0.38550961727376643</v>
       </c>
       <c r="L67" s="8">
         <f ca="1"/>
-        <v>3.0489657414518343E-2</v>
+        <v>8.481680622140296E-2</v>
       </c>
       <c r="M67" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="68" spans="9:13" x14ac:dyDescent="0.3">
@@ -4915,19 +4916,19 @@
       </c>
       <c r="J68" s="8">
         <f ca="1"/>
-        <v>0.50729570832494009</v>
+        <v>0.33923522652932059</v>
       </c>
       <c r="K68" s="8">
         <f ca="1"/>
-        <v>0.54478420040946096</v>
+        <v>0.3847977035700057</v>
       </c>
       <c r="L68" s="8">
         <f ca="1"/>
-        <v>2.8981507213443093E-2</v>
+        <v>8.1987779776821132E-2</v>
       </c>
       <c r="M68" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="69" spans="9:13" x14ac:dyDescent="0.3">
@@ -4936,19 +4937,19 @@
       </c>
       <c r="J69" s="8">
         <f ca="1"/>
-        <v>0.50729570832494009</v>
+        <v>0.33923522652932059</v>
       </c>
       <c r="K69" s="8">
         <f ca="1"/>
-        <v>0.54421619295363488</v>
+        <v>0.38410736300878329</v>
       </c>
       <c r="L69" s="8">
         <f ca="1"/>
-        <v>2.7547956524032219E-2</v>
+        <v>7.9253112583411223E-2</v>
       </c>
       <c r="M69" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="70" spans="9:13" x14ac:dyDescent="0.3">
@@ -4957,19 +4958,19 @@
       </c>
       <c r="J70" s="8">
         <f ca="1"/>
-        <v>0.50729570832494009</v>
+        <v>0.33923522652932059</v>
       </c>
       <c r="K70" s="8">
         <f ca="1"/>
-        <v>0.54366514094425133</v>
+        <v>0.38343762962849276</v>
       </c>
       <c r="L70" s="8">
         <f ca="1"/>
-        <v>2.6185315299945677E-2</v>
+        <v>7.6609659066592103E-2</v>
       </c>
       <c r="M70" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="71" spans="9:13" x14ac:dyDescent="0.3">
@@ -4978,19 +4979,19 @@
       </c>
       <c r="J71" s="8">
         <f ca="1"/>
-        <v>0.50729570832494009</v>
+        <v>0.33923522652932059</v>
       </c>
       <c r="K71" s="8">
         <f ca="1"/>
-        <v>0.54313029634690857</v>
+        <v>0.38278759428879905</v>
       </c>
       <c r="L71" s="8">
         <f ca="1"/>
-        <v>2.4890078716288306E-2</v>
+        <v>7.4054376839222086E-2</v>
       </c>
       <c r="M71" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="72" spans="9:13" x14ac:dyDescent="0.3">
@@ -4999,19 +5000,19 @@
       </c>
       <c r="J72" s="8">
         <f ca="1"/>
-        <v>0.50729570832494009</v>
+        <v>0.33923522652932059</v>
       </c>
       <c r="K72" s="8">
         <f ca="1"/>
-        <v>0.54261095449151775</v>
+        <v>0.38215640055315447</v>
       </c>
       <c r="L72" s="8">
         <f ca="1"/>
-        <v>2.3658908262105191E-2</v>
+        <v>7.158432499308548E-2</v>
       </c>
       <c r="M72" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="73" spans="9:13" x14ac:dyDescent="0.3">
@@ -5020,19 +5021,19 @@
       </c>
       <c r="J73" s="8">
         <f ca="1"/>
-        <v>0.50729570832494009</v>
+        <v>0.33923522652932059</v>
       </c>
       <c r="K73" s="8">
         <f ca="1"/>
-        <v>0.54210645097485233</v>
+        <v>0.38154324092424252</v>
       </c>
       <c r="L73" s="8">
         <f ca="1"/>
-        <v>2.248863686123535E-2</v>
+        <v>6.9196660714409025E-2</v>
       </c>
       <c r="M73" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="74" spans="9:13" x14ac:dyDescent="0.3">
@@ -5041,19 +5042,19 @@
       </c>
       <c r="J74" s="8">
         <f ca="1"/>
-        <v>0.64016095181935651</v>
+        <v>0.62733293516835054</v>
       </c>
       <c r="K74" s="8">
         <f ca="1"/>
-        <v>0.54348750028252135</v>
+        <v>0.38500506760373704</v>
       </c>
       <c r="L74" s="8">
         <f ca="1"/>
-        <v>2.1094114661236334E-2</v>
+        <v>6.498908424301994E-2</v>
       </c>
       <c r="M74" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="75" spans="9:13" x14ac:dyDescent="0.3">
@@ -5062,19 +5063,19 @@
       </c>
       <c r="J75" s="8">
         <f ca="1"/>
-        <v>0.64016095181935651</v>
+        <v>0.62733293516835054</v>
       </c>
       <c r="K75" s="8">
         <f ca="1"/>
-        <v>0.54483018710942188</v>
+        <v>0.38837073243102332</v>
       </c>
       <c r="L75" s="8">
         <f ca="1"/>
-        <v>1.9786067081596994E-2</v>
+        <v>6.1037351741171621E-2</v>
       </c>
       <c r="M75" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="76" spans="9:13" x14ac:dyDescent="0.3">
@@ -5083,19 +5084,19 @@
       </c>
       <c r="J76" s="8">
         <f ca="1"/>
-        <v>0.64016095181935651</v>
+        <v>0.62733293516835054</v>
       </c>
       <c r="K76" s="8">
         <f ca="1"/>
-        <v>0.54613608799585933</v>
+        <v>0.39164418726304145</v>
       </c>
       <c r="L76" s="8">
         <f ca="1"/>
-        <v>1.8559131889636489E-2</v>
+        <v>5.7325910031369276E-2</v>
       </c>
       <c r="M76" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="77" spans="9:13" x14ac:dyDescent="0.3">
@@ -5104,19 +5105,19 @@
       </c>
       <c r="J77" s="8">
         <f ca="1"/>
-        <v>0.64016095181935651</v>
+        <v>0.62733293516835054</v>
       </c>
       <c r="K77" s="8">
         <f ca="1"/>
-        <v>0.54740669426374444</v>
+        <v>0.39482917034284298</v>
       </c>
       <c r="L77" s="8">
         <f ca="1"/>
-        <v>1.7408275752188996E-2</v>
+        <v>5.38401464097659E-2</v>
       </c>
       <c r="M77" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="78" spans="9:13" x14ac:dyDescent="0.3">
@@ -5125,19 +5126,19 @@
       </c>
       <c r="J78" s="8">
         <f ca="1"/>
-        <v>0.64016095181935651</v>
+        <v>0.62733293516835054</v>
       </c>
       <c r="K78" s="8">
         <f ca="1"/>
-        <v>0.54864341769781932</v>
+        <v>0.39792922054051638</v>
       </c>
       <c r="L78" s="8">
         <f ca="1"/>
-        <v>1.6328786599501818E-2</v>
+        <v>5.0566338231621606E-2</v>
       </c>
       <c r="M78" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="79" spans="9:13" x14ac:dyDescent="0.3">
@@ -5146,19 +5147,19 @@
       </c>
       <c r="J79" s="8">
         <f ca="1"/>
-        <v>0.64016095181935651</v>
+        <v>0.62733293516835054</v>
       </c>
       <c r="K79" s="8">
         <f ca="1"/>
-        <v>0.54984759577836584</v>
+        <v>0.40094769046983003</v>
       </c>
       <c r="L79" s="8">
         <f ca="1"/>
-        <v>1.5316236557551079E-2</v>
+        <v>4.749159725166012E-2</v>
       </c>
       <c r="M79" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="80" spans="9:13" x14ac:dyDescent="0.3">
@@ -5167,19 +5168,19 @@
       </c>
       <c r="J80" s="8">
         <f ca="1"/>
-        <v>0.64016095181935651</v>
+        <v>0.62733293516835054</v>
       </c>
       <c r="K80" s="8">
         <f ca="1"/>
-        <v>0.5510204965061708</v>
+        <v>0.4038877585827978</v>
       </c>
       <c r="L80" s="8">
         <f ca="1"/>
-        <v>1.4366474678231416E-2</v>
+        <v>4.4603821822940405E-2</v>
       </c>
       <c r="M80" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="81" spans="9:13" x14ac:dyDescent="0.3">
@@ -5188,19 +5189,19 @@
       </c>
       <c r="J81" s="8">
         <f ca="1"/>
-        <v>0.64016095181935651</v>
+        <v>0.62733293516835054</v>
       </c>
       <c r="K81" s="8">
         <f ca="1"/>
-        <v>0.55216332285633996</v>
+        <v>0.40675244033389463</v>
       </c>
       <c r="L81" s="8">
         <f ca="1"/>
-        <v>1.3475610070365896E-2</v>
+        <v>4.1891638904704133E-2</v>
       </c>
       <c r="M81" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="82" spans="9:13" x14ac:dyDescent="0.3">
@@ -5209,19 +5210,19 @@
       </c>
       <c r="J82" s="8">
         <f ca="1"/>
-        <v>0.64016095181935651</v>
+        <v>0.62733293516835054</v>
       </c>
       <c r="K82" s="8">
         <f ca="1"/>
-        <v>0.55327721689384646</v>
+        <v>0.4095445984963561</v>
       </c>
       <c r="L82" s="8">
         <f ca="1"/>
-        <v>1.2639986372657425E-2</v>
+        <v>3.9344373279409102E-2</v>
       </c>
       <c r="M82" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="83" spans="9:13" x14ac:dyDescent="0.3">
@@ -5230,19 +5231,19 @@
       </c>
       <c r="J83" s="8">
         <f ca="1"/>
-        <v>0.64016095181935651</v>
+        <v>0.62733293516835054</v>
       </c>
       <c r="K83" s="8">
         <f ca="1"/>
-        <v>0.55436326358041532</v>
+        <v>0.412266952704756</v>
       </c>
       <c r="L83" s="8">
         <f ca="1"/>
-        <v>1.1856179866048951E-2</v>
+        <v>3.6951997022613765E-2</v>
       </c>
       <c r="M83" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="84" spans="9:13" x14ac:dyDescent="0.3">
@@ -5251,19 +5252,19 @@
       </c>
       <c r="J84" s="8">
         <f ca="1"/>
-        <v>0.29006265836598133</v>
+        <v>0.67523521635063011</v>
       </c>
       <c r="K84" s="8">
         <f ca="1"/>
-        <v>0.55110029314566922</v>
+        <v>0.41551347447816184</v>
       </c>
       <c r="L84" s="8">
         <f ca="1"/>
-        <v>1.1517216329579872E-2</v>
+        <v>3.4539244289941692E-2</v>
       </c>
       <c r="M84" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="85" spans="9:13" x14ac:dyDescent="0.3">
@@ -5272,19 +5273,19 @@
       </c>
       <c r="J85" s="8">
         <f ca="1"/>
-        <v>0.29006265836598133</v>
+        <v>0.67523521635063011</v>
       </c>
       <c r="K85" s="8">
         <f ca="1"/>
-        <v>0.547916907355673</v>
+        <v>0.4186808127936798</v>
       </c>
       <c r="L85" s="8">
         <f ca="1"/>
-        <v>1.1187943660798587E-2</v>
+        <v>3.228402737669113E-2</v>
       </c>
       <c r="M85" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="86" spans="9:13" x14ac:dyDescent="0.3">
@@ -5293,19 +5294,19 @@
       </c>
       <c r="J86" s="8">
         <f ca="1"/>
-        <v>0.29006265836598133</v>
+        <v>0.67523521635063011</v>
       </c>
       <c r="K86" s="8">
         <f ca="1"/>
-        <v>0.54481022965700199</v>
+        <v>0.42177182970400445</v>
       </c>
       <c r="L86" s="8">
         <f ca="1"/>
-        <v>1.0868084805989137E-2</v>
+        <v>3.017606524199383E-2</v>
       </c>
       <c r="M86" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="87" spans="9:13" x14ac:dyDescent="0.3">
@@ -5314,19 +5315,19 @@
       </c>
       <c r="J87" s="8">
         <f ca="1"/>
-        <v>0.29006265836598133</v>
+        <v>0.67523521635063011</v>
       </c>
       <c r="K87" s="8">
         <f ca="1"/>
-        <v>0.54177752047496608</v>
+        <v>0.42478925097360715</v>
       </c>
       <c r="L87" s="8">
         <f ca="1"/>
-        <v>1.0557370632992266E-2</v>
+        <v>2.8205740806079727E-2</v>
       </c>
       <c r="M87" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="88" spans="9:13" x14ac:dyDescent="0.3">
@@ -5335,19 +5336,19 @@
       </c>
       <c r="J88" s="8">
         <f ca="1"/>
-        <v>0.29006265836598133</v>
+        <v>0.67523521635063011</v>
       </c>
       <c r="K88" s="8">
         <f ca="1"/>
-        <v>0.53881616915603681</v>
+        <v>0.4277356740956898</v>
       </c>
       <c r="L88" s="8">
         <f ca="1"/>
-        <v>1.0255539704825263E-2</v>
+        <v>2.6364067051268869E-2</v>
       </c>
       <c r="M88" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="89" spans="9:13" x14ac:dyDescent="0.3">
@@ -5356,19 +5357,19 @@
       </c>
       <c r="J89" s="8">
         <f ca="1"/>
-        <v>0.29006265836598133</v>
+        <v>0.67523521635063011</v>
       </c>
       <c r="K89" s="8">
         <f ca="1"/>
-        <v>0.53592368647243149</v>
+        <v>0.43061357574981701</v>
       </c>
       <c r="L89" s="8">
         <f ca="1"/>
-        <v>9.9623380597966497E-3</v>
+        <v>2.4642646604068986E-2</v>
       </c>
       <c r="M89" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="90" spans="9:13" x14ac:dyDescent="0.3">
@@ -5377,19 +5378,19 @@
       </c>
       <c r="J90" s="8">
         <f ca="1"/>
-        <v>0.29006265836598133</v>
+        <v>0.67523521635063011</v>
       </c>
       <c r="K90" s="8">
         <f ca="1"/>
-        <v>0.5330976976436218</v>
+        <v>0.4334253187452286</v>
       </c>
       <c r="L90" s="8">
         <f ca="1"/>
-        <v>9.677516063605519E-3</v>
+        <v>2.3033623326211002E-2</v>
       </c>
       <c r="M90" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="91" spans="9:13" x14ac:dyDescent="0.3">
@@ -5398,19 +5399,19 @@
       </c>
       <c r="J91" s="8">
         <f ca="1"/>
-        <v>0.29006265836598133</v>
+        <v>0.67523521635063011</v>
       </c>
       <c r="K91" s="8">
         <f ca="1"/>
-        <v>0.53033593583364858</v>
+        <v>0.43617315849074456</v>
       </c>
       <c r="L91" s="8">
         <f ca="1"/>
-        <v>9.4008394441970362E-3</v>
+        <v>2.1529660152768058E-2</v>
       </c>
       <c r="M91" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="92" spans="9:13" x14ac:dyDescent="0.3">
@@ -5419,19 +5420,19 @@
       </c>
       <c r="J92" s="8">
         <f ca="1"/>
-        <v>0.29006265836598133</v>
+        <v>0.67523521635063011</v>
       </c>
       <c r="K92" s="8">
         <f ca="1"/>
-        <v>0.52763623608682086</v>
+        <v>0.4388592490284961</v>
       </c>
       <c r="L92" s="8">
         <f ca="1"/>
-        <v>9.1320728895504383E-3</v>
+        <v>2.0123897311640888E-2</v>
       </c>
       <c r="M92" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="93" spans="9:13" x14ac:dyDescent="0.3">
@@ -5440,19 +5441,19 @@
       </c>
       <c r="J93" s="8">
         <f ca="1"/>
-        <v>0.29006265836598133</v>
+        <v>0.67523521635063011</v>
       </c>
       <c r="K93" s="8">
         <f ca="1"/>
-        <v>0.52499652966770038</v>
+        <v>0.44148564866540868</v>
       </c>
       <c r="L93" s="8">
         <f ca="1"/>
-        <v>8.8709902514644227E-3</v>
+        <v>1.8809922955658757E-2</v>
       </c>
       <c r="M93" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="94" spans="9:13" x14ac:dyDescent="0.3">
@@ -5461,19 +5462,19 @@
       </c>
       <c r="J94" s="8">
         <f ca="1"/>
-        <v>0.99292478307626375</v>
+        <v>0.89987586081846582</v>
       </c>
       <c r="K94" s="8">
         <f ca="1"/>
-        <v>0.53013859838647581</v>
+        <v>0.44652290374401371</v>
       </c>
       <c r="L94" s="8">
         <f ca="1"/>
-        <v>8.0324844800293595E-3</v>
+        <v>1.7191186192908329E-2</v>
       </c>
       <c r="M94" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="95" spans="9:13" x14ac:dyDescent="0.3">
@@ -5482,19 +5483,19 @@
       </c>
       <c r="J95" s="8">
         <f ca="1"/>
-        <v>0.99292478307626375</v>
+        <v>0.89987586081846582</v>
       </c>
       <c r="K95" s="8">
         <f ca="1"/>
-        <v>0.53516888300266929</v>
+        <v>0.45145065327743172</v>
       </c>
       <c r="L95" s="8">
         <f ca="1"/>
-        <v>7.273235696978542E-3</v>
+        <v>1.5711755777546892E-2</v>
       </c>
       <c r="M95" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="96" spans="9:13" x14ac:dyDescent="0.3">
@@ -5503,19 +5504,19 @@
       </c>
       <c r="J96" s="8">
         <f ca="1"/>
-        <v>0.99292478307626375</v>
+        <v>0.89987586081846582</v>
       </c>
       <c r="K96" s="8">
         <f ca="1"/>
-        <v>0.54009098945507339</v>
+        <v>0.45627242970260407</v>
       </c>
       <c r="L96" s="8">
         <f ca="1"/>
-        <v>6.5857562740880542E-3</v>
+        <v>1.4359641116220994E-2</v>
       </c>
       <c r="M96" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="97" spans="9:13" x14ac:dyDescent="0.3">
@@ -5524,19 +5525,19 @@
       </c>
       <c r="J97" s="8">
         <f ca="1"/>
-        <v>0.99292478307626375</v>
+        <v>0.89987586081846582</v>
       </c>
       <c r="K97" s="8">
         <f ca="1"/>
-        <v>0.54490837023827765</v>
+        <v>0.46099161514000692</v>
       </c>
       <c r="L97" s="8">
         <f ca="1"/>
-        <v>5.963256859078875E-3</v>
+        <v>1.312388866439208E-2</v>
       </c>
       <c r="M97" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="98" spans="9:13" x14ac:dyDescent="0.3">
@@ -5545,19 +5546,19 @@
       </c>
       <c r="J98" s="8">
         <f ca="1"/>
-        <v>0.99292478307626375</v>
+        <v>0.89987586081846582</v>
       </c>
       <c r="K98" s="8">
         <f ca="1"/>
-        <v>0.54962433247867748</v>
+        <v>0.46561144930504328</v>
       </c>
       <c r="L98" s="8">
         <f ca="1"/>
-        <v>5.3995977726969437E-3</v>
+        <v>1.1994480366130007E-2</v>
       </c>
       <c r="M98" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="99" spans="9:13" x14ac:dyDescent="0.3">
@@ -5566,19 +5567,19 @@
       </c>
       <c r="J99" s="8">
         <f ca="1"/>
-        <v>0.99292478307626375</v>
+        <v>0.89987586081846582</v>
       </c>
       <c r="K99" s="8">
         <f ca="1"/>
-        <v>0.55424204550573564</v>
+        <v>0.47013503692497483</v>
       </c>
       <c r="L99" s="8">
         <f ca="1"/>
-        <v>4.8892138408584323E-3</v>
+        <v>1.0962266305335007E-2</v>
       </c>
       <c r="M99" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="100" spans="9:13" x14ac:dyDescent="0.3">
@@ -5587,19 +5588,19 @@
       </c>
       <c r="J100" s="8">
         <f ca="1"/>
-        <v>0.99292478307626375</v>
+        <v>0.89987586081846582</v>
       </c>
       <c r="K100" s="8">
         <f ca="1"/>
-        <v>0.55876454795491637</v>
+        <v>0.47456535469707262</v>
       </c>
       <c r="L100" s="8">
         <f ca="1"/>
-        <v>4.4270743199903021E-3</v>
+        <v>1.001888231988377E-2</v>
       </c>
       <c r="M100" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="101" spans="9:13" x14ac:dyDescent="0.3">
@@ -5608,19 +5609,19 @@
       </c>
       <c r="J101" s="8">
         <f ca="1"/>
-        <v>0.99292478307626375</v>
+        <v>0.89987586081846582</v>
       </c>
       <c r="K101" s="8">
         <f ca="1"/>
-        <v>0.5631947544357464</v>
+        <v>0.47890525782076032</v>
       </c>
       <c r="L101" s="8">
         <f ca="1"/>
-        <v>4.0086169377122876E-3</v>
+        <v>9.1566801697240408E-3</v>
       </c>
       <c r="M101" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="102" spans="9:13" x14ac:dyDescent="0.3">
@@ -5629,19 +5630,19 @@
       </c>
       <c r="J102" s="8">
         <f ca="1"/>
-        <v>0.99292478307626375</v>
+        <v>0.89987586081846582</v>
       </c>
       <c r="K102" s="8">
         <f ca="1"/>
-        <v>0.56753546179575165</v>
+        <v>0.48315748613386844</v>
       </c>
       <c r="L102" s="8">
         <f ca="1"/>
-        <v>3.6297157921888362E-3</v>
+        <v>8.3686790115340831E-3</v>
       </c>
       <c r="M102" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
     <row r="103" spans="9:13" x14ac:dyDescent="0.3">
@@ -5650,19 +5651,19 @@
       </c>
       <c r="J103" s="8">
         <f ca="1"/>
-        <v>0.99292478307626375</v>
+        <v>0.89987586081846582</v>
       </c>
       <c r="K103" s="8">
         <f ca="1"/>
-        <v>0.57178935500855677</v>
+        <v>0.48732466988071438</v>
       </c>
       <c r="L103" s="8">
         <f ca="1"/>
-        <v>3.2866275957767017E-3</v>
+        <v>7.648490976825865E-3</v>
       </c>
       <c r="M103" s="22">
         <f ca="1"/>
-        <v>0.83955157724683804</v>
+        <v>0.14270304597466366</v>
       </c>
     </row>
   </sheetData>
@@ -5702,7 +5703,7 @@
       </c>
       <c r="C2" s="18">
         <f ca="1">TODAY()</f>
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="F2" s="17" cm="1">
         <f t="array" aca="1" ref="F2:G11" ca="1">_xll.TMX.INSTRUMENT(C10)</f>
@@ -5714,7 +5715,7 @@
       </c>
       <c r="H2" s="18" cm="1">
         <f t="array" aca="1" ref="H2:H11" ca="1">_xlfn.MAP(_xlfn.TAKE(_xlfn.ANCHORARRAY(F2),,1),_xlfn.LAMBDA(_xlpm.d,_xll.TMX.DATE.ADDYEARS(pvdate, _xlpm.d)))</f>
-        <v>45776</v>
+        <v>45777</v>
       </c>
       <c r="J2" s="20" t="s">
         <v>24</v>
@@ -5742,7 +5743,7 @@
       </c>
       <c r="C3" s="18" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">_xll.TMX.DATE.ADDYEARS(dated,D3)</f>
-        <v>49063.425000000003</v>
+        <v>49064.425000000003</v>
       </c>
       <c r="D3" s="17">
         <v>10</v>
@@ -5757,7 +5758,7 @@
       </c>
       <c r="H3" s="18">
         <f ca="1"/>
-        <v>46141</v>
+        <v>46142</v>
       </c>
       <c r="J3" s="20" t="s">
         <v>25</v>
@@ -5784,7 +5785,7 @@
       </c>
       <c r="H4" s="18">
         <f ca="1"/>
-        <v>46506</v>
+        <v>46507</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
@@ -5807,7 +5808,7 @@
       </c>
       <c r="H5" s="18">
         <f ca="1"/>
-        <v>46872</v>
+        <v>46873</v>
       </c>
       <c r="J5" s="17" t="e" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">TRANSPOSE(_xll.FREQ_ENUM())</f>
@@ -5838,7 +5839,7 @@
       </c>
       <c r="H6" s="18">
         <f ca="1"/>
-        <v>47237</v>
+        <v>47238</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
@@ -5858,7 +5859,7 @@
       </c>
       <c r="H7" s="18">
         <f ca="1"/>
-        <v>47602</v>
+        <v>47603</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
@@ -5867,7 +5868,7 @@
       </c>
       <c r="C8" s="11" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xll.\TMX.BOND.BASIC(dated, maturity, coupon, _xll.ENUM(frequency), _xll.ENUM(day_count))</f>
-        <v>2424279468304</v>
+        <v>1762236499008</v>
       </c>
       <c r="F8" s="17">
         <f ca="1"/>
@@ -5879,7 +5880,7 @@
       </c>
       <c r="H8" s="18">
         <f ca="1"/>
-        <v>47967</v>
+        <v>47968</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
@@ -5888,7 +5889,7 @@
       </c>
       <c r="C9" s="18">
         <f ca="1">dated+D9</f>
-        <v>45591</v>
+        <v>45592</v>
       </c>
       <c r="D9" s="17">
         <v>180</v>
@@ -5903,7 +5904,7 @@
       </c>
       <c r="H9" s="18">
         <f ca="1"/>
-        <v>48333</v>
+        <v>48334</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
@@ -5912,7 +5913,7 @@
       </c>
       <c r="C10" s="11" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">_xll.\TMX.BOND.BASIC.INSTRUMENT(bond_basic,pvdate)</f>
-        <v>2424275869856</v>
+        <v>1762235819456</v>
       </c>
       <c r="F10" s="17">
         <f ca="1"/>
@@ -5924,7 +5925,7 @@
       </c>
       <c r="H10" s="18">
         <f ca="1"/>
-        <v>48698</v>
+        <v>48699</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
@@ -5938,7 +5939,7 @@
       </c>
       <c r="H11" s="18">
         <f ca="1"/>
-        <v>49063</v>
+        <v>49064</v>
       </c>
     </row>
   </sheetData>
@@ -5975,10 +5976,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EAD57E-B813-416C-A1C4-B7528B2439C2}">
-  <dimension ref="B2:H25"/>
+  <dimension ref="B2:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -5989,16 +5990,18 @@
     <col min="5" max="6" width="9.140625" style="23"/>
     <col min="7" max="7" width="9.140625" style="23" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="23"/>
+    <col min="9" max="9" width="9.140625" style="23"/>
+    <col min="10" max="10" width="13" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="29">
         <f ca="1">TODAY()</f>
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>32</v>
@@ -6010,13 +6013,13 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="26" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="25" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">_xll.\TMX.BOND.BASIC(pvdate,10)</f>
-        <v>2424279465392</v>
+        <v>1762236503712</v>
       </c>
       <c r="D3" s="3">
         <v>10</v>
@@ -6031,14 +6034,18 @@
       <c r="H3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="J3" s="31" cm="1">
+        <f t="array" aca="1" ref="J3:J7" ca="1">_xll.TMX.BOND.BASIC(bond)</f>
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="26" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="25" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">_xll.\TMX.BOND.BASIC.INSTRUMENT(bond,pvdate)</f>
-        <v>2424275871792</v>
+        <v>1762235819280</v>
       </c>
       <c r="F4" s="28" t="s">
         <v>35</v>
@@ -6047,8 +6054,12 @@
         <f t="array" aca="1" ref="G4" ca="1">_xll.TMX.VALUE.YIELD(C4, G3)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="J4" s="31">
+        <f ca="1"/>
+        <v>49064</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C5" s="27" t="s">
         <v>8</v>
       </c>
@@ -6062,8 +6073,12 @@
         <f t="array" aca="1" ref="G5" ca="1">_xll.TMX.VALUE.DURATION(C4, G2)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="J5" s="23">
+        <f ca="1"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C6" s="30" cm="1">
         <f t="array" aca="1" ref="C6:C25" ca="1">_xll.TMX.INSTRUMENT.TIME(C4)</f>
         <v>0.50377488928588543</v>
@@ -6078,62 +6093,70 @@
         <f t="array" aca="1" ref="G6" ca="1">_xll.TMX.VALUE.CONVEXITY(C4,G2)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="J6" s="23">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C7" s="23">
         <f ca="1"/>
         <v>0.99933605755080523</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="J7" s="23">
+        <f ca="1"/>
+        <v>1762236503736</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C8" s="23">
         <f ca="1"/>
         <v>1.5031109468366908</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C9" s="23">
         <f ca="1"/>
         <v>1.9986721151016105</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C10" s="23">
         <f ca="1"/>
         <v>2.5024470043874958</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C11" s="23">
         <f ca="1"/>
         <v>2.9980081726524159</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C12" s="23">
         <f ca="1"/>
         <v>3.5017830619383012</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C13" s="23">
         <f ca="1"/>
         <v>4.0000821372102093</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C14" s="23">
         <f ca="1"/>
         <v>4.5038570264960951</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C15" s="23">
         <f ca="1"/>
         <v>4.9994181947610148</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C16" s="23">
         <f ca="1"/>
         <v>5.5031930840469006</v>

</xml_diff>

<commit_message>
curve::plus root1d newton bounds
</commit_message>
<xml_diff>
--- a/bondxll.xlsx
+++ b/bondxll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\source\repos\tmcrossx\bondxll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6313CEB9-1E64-420E-AC13-9F335A7F0AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76D6DB4-9BCF-4A08-B891-7E121B9C6B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3585" yWindow="1665" windowWidth="32415" windowHeight="17685" activeTab="4" xr2:uid="{B41655E8-20ED-4B49-A343-A4ADF5D922ED}"/>
   </bookViews>
@@ -20,25 +20,35 @@
     <sheet name="VALUATION" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="bond">VALUATION!$C$3</definedName>
+    <definedName name="bond">VALUATION!$C$8</definedName>
     <definedName name="bond_basic">BOND!$C$8</definedName>
+    <definedName name="coupon" localSheetId="4">VALUATION!$C$4</definedName>
     <definedName name="coupon">BOND!$C$4</definedName>
+    <definedName name="curve">VALUATION!$G$3</definedName>
     <definedName name="date">ENUM!$E$3</definedName>
+    <definedName name="dated" localSheetId="4">VALUATION!$C$2</definedName>
     <definedName name="dated">BOND!$C$2</definedName>
     <definedName name="day_count" localSheetId="3">BOND!$C$6</definedName>
+    <definedName name="day_count" localSheetId="4">VALUATION!$C$6</definedName>
     <definedName name="DAY_COUNT">ENUM!$E$2</definedName>
     <definedName name="days">ENUM!$E$4</definedName>
     <definedName name="dcf">ENUM!$E$5</definedName>
+    <definedName name="face" localSheetId="4">VALUATION!$C$7</definedName>
     <definedName name="face">BOND!$C$7</definedName>
+    <definedName name="frequency" localSheetId="4">VALUATION!$C$5</definedName>
     <definedName name="frequency">BOND!$C$5</definedName>
+    <definedName name="instrument">VALUATION!$C$9</definedName>
+    <definedName name="maturity" localSheetId="4">VALUATION!$C$3</definedName>
     <definedName name="maturity">BOND!$C$3</definedName>
-    <definedName name="pvdate" localSheetId="4">VALUATION!$C$2</definedName>
+    <definedName name="present">VALUATION!$G$4</definedName>
+    <definedName name="pvdate" localSheetId="4">VALUATION!$G$2</definedName>
     <definedName name="pvdate">BOND!$C$9</definedName>
     <definedName name="pwflat">PWFLAT!$F$2</definedName>
     <definedName name="rate">PWFLAT!$C$3:$C$12</definedName>
     <definedName name="time">PWFLAT!$B$3:$B$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -81,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>TMX_DAY_COUNT_ENUM</t>
   </si>
@@ -197,21 +207,24 @@
     <t>convexity</t>
   </si>
   <si>
-    <t>=TMX.INSTRUMENT.cash(C4)</t>
+    <t>TMX_DAY_COUNT_30_360</t>
   </si>
   <si>
-    <t>=\TMX.CURVE.CONSTANT(H2)</t>
+    <t>oas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="&quot;0x&quot;#"/>
     <numFmt numFmtId="165" formatCode="m/d/yy"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +375,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -455,7 +475,7 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -521,6 +541,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="4" xfId="3"/>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="14" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -936,307 +967,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.10371428101934899</c:v>
+                  <c:v>0.79453585160743101</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.10371428101934899</c:v>
+                  <c:v>0.79453585160743101</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.10371428101934899</c:v>
+                  <c:v>0.79453585160743101</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.10371428101934899</c:v>
+                  <c:v>0.79453585160743101</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.10371428101934899</c:v>
+                  <c:v>0.79453585160743101</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.10371428101934899</c:v>
+                  <c:v>0.79453585160743101</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.10371428101934899</c:v>
+                  <c:v>0.79453585160743101</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.10371428101934899</c:v>
+                  <c:v>0.79453585160743101</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.10371428101934899</c:v>
+                  <c:v>0.79453585160743101</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.10371428101934899</c:v>
+                  <c:v>0.79453585160743101</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.32786045310224088</c:v>
+                  <c:v>0.242849658381314</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.32786045310224088</c:v>
+                  <c:v>0.242849658381314</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.32786045310224088</c:v>
+                  <c:v>0.242849658381314</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.32786045310224088</c:v>
+                  <c:v>0.242849658381314</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.32786045310224088</c:v>
+                  <c:v>0.242849658381314</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.32786045310224088</c:v>
+                  <c:v>0.242849658381314</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.32786045310224088</c:v>
+                  <c:v>0.242849658381314</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.32786045310224088</c:v>
+                  <c:v>0.242849658381314</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.32786045310224088</c:v>
+                  <c:v>0.242849658381314</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.32786045310224088</c:v>
+                  <c:v>0.242849658381314</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.54577121542853657</c:v>
+                  <c:v>0.74945515068588553</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.54577121542853657</c:v>
+                  <c:v>0.74945515068588553</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.54577121542853657</c:v>
+                  <c:v>0.74945515068588553</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.54577121542853657</c:v>
+                  <c:v>0.74945515068588553</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.54577121542853657</c:v>
+                  <c:v>0.74945515068588553</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.54577121542853657</c:v>
+                  <c:v>0.74945515068588553</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.54577121542853657</c:v>
+                  <c:v>0.74945515068588553</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.54577121542853657</c:v>
+                  <c:v>0.74945515068588553</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.54577121542853657</c:v>
+                  <c:v>0.74945515068588553</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.54577121542853657</c:v>
+                  <c:v>0.74945515068588553</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.11805033961160771</c:v>
+                  <c:v>1.2016145554805346E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.11805033961160771</c:v>
+                  <c:v>1.2016145554805346E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.11805033961160771</c:v>
+                  <c:v>1.2016145554805346E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.11805033961160771</c:v>
+                  <c:v>1.2016145554805346E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.11805033961160771</c:v>
+                  <c:v>1.2016145554805346E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.11805033961160771</c:v>
+                  <c:v>1.2016145554805346E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.11805033961160771</c:v>
+                  <c:v>1.2016145554805346E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.11805033961160771</c:v>
+                  <c:v>1.2016145554805346E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.11805033961160771</c:v>
+                  <c:v>1.2016145554805346E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.11805033961160771</c:v>
+                  <c:v>1.2016145554805346E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.79340484028740965</c:v>
+                  <c:v>0.85140762941610237</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.79340484028740965</c:v>
+                  <c:v>0.85140762941610237</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.79340484028740965</c:v>
+                  <c:v>0.85140762941610237</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.79340484028740965</c:v>
+                  <c:v>0.85140762941610237</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.79340484028740965</c:v>
+                  <c:v>0.85140762941610237</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.79340484028740965</c:v>
+                  <c:v>0.85140762941610237</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.79340484028740965</c:v>
+                  <c:v>0.85140762941610237</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.79340484028740965</c:v>
+                  <c:v>0.85140762941610237</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.79340484028740965</c:v>
+                  <c:v>0.85140762941610237</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.79340484028740965</c:v>
+                  <c:v>0.85140762941610237</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.54345481613037738</c:v>
+                  <c:v>0.11763237961991213</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.54345481613037738</c:v>
+                  <c:v>0.11763237961991213</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.54345481613037738</c:v>
+                  <c:v>0.11763237961991213</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.54345481613037738</c:v>
+                  <c:v>0.11763237961991213</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.54345481613037738</c:v>
+                  <c:v>0.11763237961991213</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.54345481613037738</c:v>
+                  <c:v>0.11763237961991213</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.54345481613037738</c:v>
+                  <c:v>0.11763237961991213</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.54345481613037738</c:v>
+                  <c:v>0.11763237961991213</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.54345481613037738</c:v>
+                  <c:v>0.11763237961991213</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.54345481613037738</c:v>
+                  <c:v>0.11763237961991213</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.57740717064861236</c:v>
+                  <c:v>0.47263522532870339</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.57740717064861236</c:v>
+                  <c:v>0.47263522532870339</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.57740717064861236</c:v>
+                  <c:v>0.47263522532870339</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.57740717064861236</c:v>
+                  <c:v>0.47263522532870339</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.57740717064861236</c:v>
+                  <c:v>0.47263522532870339</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.57740717064861236</c:v>
+                  <c:v>0.47263522532870339</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.57740717064861236</c:v>
+                  <c:v>0.47263522532870339</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.57740717064861236</c:v>
+                  <c:v>0.47263522532870339</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.57740717064861236</c:v>
+                  <c:v>0.47263522532870339</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.57740717064861236</c:v>
+                  <c:v>0.47263522532870339</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.70384581205313657</c:v>
+                  <c:v>0.91905236752737207</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.70384581205313657</c:v>
+                  <c:v>0.91905236752737207</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.70384581205313657</c:v>
+                  <c:v>0.91905236752737207</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.70384581205313657</c:v>
+                  <c:v>0.91905236752737207</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.70384581205313657</c:v>
+                  <c:v>0.91905236752737207</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.70384581205313657</c:v>
+                  <c:v>0.91905236752737207</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.70384581205313657</c:v>
+                  <c:v>0.91905236752737207</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.70384581205313657</c:v>
+                  <c:v>0.91905236752737207</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.70384581205313657</c:v>
+                  <c:v>0.91905236752737207</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.70384581205313657</c:v>
+                  <c:v>0.91905236752737207</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.3680418096501068</c:v>
+                  <c:v>0.76489947289387872</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.3680418096501068</c:v>
+                  <c:v>0.76489947289387872</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.3680418096501068</c:v>
+                  <c:v>0.76489947289387872</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.3680418096501068</c:v>
+                  <c:v>0.76489947289387872</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.3680418096501068</c:v>
+                  <c:v>0.76489947289387872</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.3680418096501068</c:v>
+                  <c:v>0.76489947289387872</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.3680418096501068</c:v>
+                  <c:v>0.76489947289387872</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.3680418096501068</c:v>
+                  <c:v>0.76489947289387872</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.3680418096501068</c:v>
+                  <c:v>0.76489947289387872</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.3680418096501068</c:v>
+                  <c:v>0.76489947289387872</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1593,307 +1624,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956178</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956178</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45158686362248929</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956178</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45158686362248929</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956178</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.45158686362248934</c:v>
+                  <c:v>0.32283416468956183</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.41996208338584018</c:v>
+                  <c:v>0.36571613622755</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.39360809985529926</c:v>
+                  <c:v>0.40145111250920679</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.37130857532945694</c:v>
+                  <c:v>0.43168840013214704</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.35219469716444923</c:v>
+                  <c:v>0.4576060752375245</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.33562933608810924</c:v>
+                  <c:v>0.48006806032885158</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.32113464514631168</c:v>
+                  <c:v>0.49972229728376283</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.30834521196237274</c:v>
+                  <c:v>0.51706427106750796</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.29697682690998251</c:v>
+                  <c:v>0.53247935887528153</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.28680511396837022</c:v>
+                  <c:v>0.54627180586118407</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.27765057232091916</c:v>
+                  <c:v>0.55868500814849642</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.28004151902479163</c:v>
+                  <c:v>0.54364522958815442</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.28221510693740293</c:v>
+                  <c:v>0.52997270362420712</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.28419968720543937</c:v>
+                  <c:v>0.51748909296147261</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.28601888578447277</c:v>
+                  <c:v>0.50604578318729931</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.28769254847718351</c:v>
+                  <c:v>0.49551793819505996</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.28923746788583954</c:v>
+                  <c:v>0.48579992743299277</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.29066794881978036</c:v>
+                  <c:v>0.47680176931996765</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.29199625254415396</c:v>
+                  <c:v>0.46844633678644432</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.29323294911512243</c:v>
+                  <c:v>0.46066714097937084</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.29438719924802642</c:v>
+                  <c:v>0.45340655822610226</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.30249636106030092</c:v>
+                  <c:v>0.46295651282157918</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.3100987002593083</c:v>
+                  <c:v>0.47190959525483872</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.31724029162807282</c:v>
+                  <c:v>0.48032006663153715</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.32396178938691</c:v>
+                  <c:v>0.48823580439784148</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.33029920155952786</c:v>
+                  <c:v>0.49569921429178559</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.33628453527811142</c:v>
+                  <c:v>0.50274799030273287</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.34194633744433917</c:v>
+                  <c:v>0.50941575139416939</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.34731015002287069</c:v>
+                  <c:v>0.51573257769131986</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.3523988952896826</c:v>
+                  <c:v>0.52172546417835997</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.35723320329315394</c:v>
+                  <c:v>0.52741870634104804</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.35139947491067719</c:v>
+                  <c:v>0.51484791217552994</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.34584354311784216</c:v>
+                  <c:v>0.50287572725598884</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.34054602675723211</c:v>
+                  <c:v>0.49146038814665904</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.33548930659483156</c:v>
+                  <c:v>0.48056392808775317</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.33065732955075994</c:v>
+                  <c:v>0.47015175514257668</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.32603543846512617</c:v>
+                  <c:v>0.46019228536892937</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.32161022359590236</c:v>
+                  <c:v>0.45065662281969276</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.31736939267956288</c:v>
+                  <c:v>0.44151827954334083</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.31330165690266581</c:v>
+                  <c:v>0.4327529298701055</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.30939663055684469</c:v>
+                  <c:v>0.42433819418379953</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.3188869876103852</c:v>
+                  <c:v>0.43271210467855065</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.32801233093109722</c:v>
+                  <c:v>0.44076394169273431</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.33679332167366915</c:v>
+                  <c:v>0.44851193580072241</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.34524909053688657</c:v>
+                  <c:v>0.45597296716397018</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.35339737689598699</c:v>
+                  <c:v>0.46316268829582707</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.36125465302797671</c:v>
+                  <c:v>0.47009563367297491</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.36883623526059828</c:v>
+                  <c:v>0.47678531780881922</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.37615638362312959</c:v>
+                  <c:v>0.48324432318135863</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.38322839136320208</c:v>
+                  <c:v>0.4894843792192356</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.39006466551193886</c:v>
+                  <c:v>0.49551643338918333</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.39257925814502803</c:v>
+                  <c:v>0.48932161283558867</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.39501273488672717</c:v>
+                  <c:v>0.48332662520307779</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.39736895839853115</c:v>
+                  <c:v>0.47752195463826563</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.39965154992559127</c:v>
+                  <c:v>0.47189868002860386</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.40186390786720333</c:v>
+                  <c:v>0.46644842925308555</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.40400922465906963</c:v>
+                  <c:v>0.46116333759197681</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.406090502143716</c:v>
+                  <c:v>0.45603600986105047</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.40811056558469638</c:v>
+                  <c:v>0.45105948588691613</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.41007207646216992</c:v>
+                  <c:v>0.4462272089844958</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.41197754417171584</c:v>
+                  <c:v>0.44153299713643029</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.41430753891082706</c:v>
+                  <c:v>0.44197105668843417</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.41657281157385184</c:v>
+                  <c:v>0.44239694791954898</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.4187760219721362</c:v>
+                  <c:v>0.44281117089775662</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.42091968614343994</c:v>
+                  <c:v>0.44321419866033696</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.42300618593684225</c:v>
+                  <c:v>0.44360647901591516</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.42503777784094454</c:v>
+                  <c:v>0.44398843620424133</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.42701660112416095</c:v>
+                  <c:v>0.44436047242663695</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.4289446853488334</c:v>
+                  <c:v>0.44472296925871468</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.43082395731465339</c:v>
+                  <c:v>0.4450762889558032</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.43265624748132792</c:v>
+                  <c:v>0.44542077566046445</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.43600426679702925</c:v>
+                  <c:v>0.45126807926375961</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.43927062710503062</c:v>
+                  <c:v>0.45697276570599887</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.44245827993573067</c:v>
+                  <c:v>0.46253998982432859</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.44557003627046171</c:v>
+                  <c:v>0.4679746609874601</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.4486085748090814</c:v>
+                  <c:v>0.47328145753498846</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.45157644966075638</c:v>
+                  <c:v>0.4784648402093184</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.45447609750434703</c:v>
+                  <c:v>0.48352906466125017</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.4573098442605833</c:v>
+                  <c:v>0.48847819310291068</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.46007991131443216</c:v>
+                  <c:v>0.49331610517509561</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.46278842132263992</c:v>
+                  <c:v>0.49804650809012085</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.4617472497657989</c:v>
+                  <c:v>0.50097895825279948</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.46072871237323709</c:v>
+                  <c:v>0.5038476594988982</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.45973207901062274</c:v>
+                  <c:v>0.50665466824508076</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.4587566506131705</c:v>
+                  <c:v>0.50940195340091898</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.45780175755040137</c:v>
+                  <c:v>0.5120914009745291</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.45686675809310656</c:v>
+                  <c:v>0.51472481839035567</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.45595103697513756</c:v>
+                  <c:v>0.51730393853987655</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.45505400404324947</c:v>
+                  <c:v>0.5198304235843052</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.45417509298877334</c:v>
+                  <c:v>0.52230586852682603</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.4533137601553866</c:v>
+                  <c:v>0.52473180457049662</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3044,7 +3075,7 @@
   <dimension ref="B2:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3185,7 +3216,7 @@
       </c>
       <c r="E2" s="11" cm="1">
         <f t="array" aca="1" ref="E2" ca="1">_xll.\TMX.INSTRUMENT(_xlfn.ANCHORARRAY(B3),_xlfn.ANCHORARRAY(C3))</f>
-        <v>2369228324736</v>
+        <v>1521044377504</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
@@ -3195,7 +3226,7 @@
       </c>
       <c r="C3" s="13" cm="1">
         <f t="array" aca="1" ref="C3:C12" ca="1">_xlfn.RANDARRAY(B2,1)</f>
-        <v>2.0068364801222982E-2</v>
+        <v>8.5139449099762343E-2</v>
       </c>
       <c r="E3" s="13" cm="1">
         <f t="array" aca="1" ref="E3:F12" ca="1">_xll.TMX.INSTRUMENT(E2)</f>
@@ -3203,7 +3234,7 @@
       </c>
       <c r="F3" s="13">
         <f ca="1"/>
-        <v>2.0068364801222982E-2</v>
+        <v>8.5139449099762343E-2</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -3212,7 +3243,7 @@
       </c>
       <c r="C4" s="13">
         <f ca="1"/>
-        <v>0.88391639921788756</v>
+        <v>0.4269311202523145</v>
       </c>
       <c r="E4" s="13">
         <f ca="1"/>
@@ -3220,7 +3251,7 @@
       </c>
       <c r="F4" s="13">
         <f ca="1"/>
-        <v>0.88391639921788756</v>
+        <v>0.4269311202523145</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -3229,7 +3260,7 @@
       </c>
       <c r="C5" s="13">
         <f ca="1"/>
-        <v>0.69681207321570282</v>
+        <v>0.26579143885957057</v>
       </c>
       <c r="E5" s="13">
         <f ca="1"/>
@@ -3237,7 +3268,7 @@
       </c>
       <c r="F5" s="13">
         <f ca="1"/>
-        <v>0.69681207321570282</v>
+        <v>0.26579143885957057</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -3246,7 +3277,7 @@
       </c>
       <c r="C6" s="13">
         <f ca="1"/>
-        <v>0.5259301480321954</v>
+        <v>0.50639962796242388</v>
       </c>
       <c r="E6" s="13">
         <f ca="1"/>
@@ -3254,7 +3285,7 @@
       </c>
       <c r="F6" s="13">
         <f ca="1"/>
-        <v>0.5259301480321954</v>
+        <v>0.50639962796242388</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -3263,7 +3294,7 @@
       </c>
       <c r="C7" s="13">
         <f ca="1"/>
-        <v>0.60818471010780817</v>
+        <v>0.4226585336927593</v>
       </c>
       <c r="E7" s="13">
         <f ca="1"/>
@@ -3271,7 +3302,7 @@
       </c>
       <c r="F7" s="13">
         <f ca="1"/>
-        <v>0.60818471010780817</v>
+        <v>0.4226585336927593</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -3280,7 +3311,7 @@
       </c>
       <c r="C8" s="13">
         <f ca="1"/>
-        <v>0.39294805145532119</v>
+        <v>0.39055904915126072</v>
       </c>
       <c r="E8" s="13">
         <f ca="1"/>
@@ -3288,7 +3319,7 @@
       </c>
       <c r="F8" s="13">
         <f ca="1"/>
-        <v>0.39294805145532119</v>
+        <v>0.39055904915126072</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -3297,7 +3328,7 @@
       </c>
       <c r="C9" s="13">
         <f ca="1"/>
-        <v>0.63638207086617493</v>
+        <v>0.9144784094379006</v>
       </c>
       <c r="E9" s="13">
         <f ca="1"/>
@@ -3305,7 +3336,7 @@
       </c>
       <c r="F9" s="13">
         <f ca="1"/>
-        <v>0.63638207086617493</v>
+        <v>0.9144784094379006</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
@@ -3314,7 +3345,7 @@
       </c>
       <c r="C10" s="13">
         <f ca="1"/>
-        <v>0.48146602157327378</v>
+        <v>0.6514604791187546</v>
       </c>
       <c r="E10" s="13">
         <f ca="1"/>
@@ -3322,7 +3353,7 @@
       </c>
       <c r="F10" s="13">
         <f ca="1"/>
-        <v>0.48146602157327378</v>
+        <v>0.6514604791187546</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
@@ -3331,7 +3362,7 @@
       </c>
       <c r="C11" s="13">
         <f ca="1"/>
-        <v>0.75821217263766649</v>
+        <v>0.40009338252089188</v>
       </c>
       <c r="E11" s="13">
         <f ca="1"/>
@@ -3339,7 +3370,7 @@
       </c>
       <c r="F11" s="13">
         <f ca="1"/>
-        <v>0.75821217263766649</v>
+        <v>0.40009338252089188</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
@@ -3348,7 +3379,7 @@
       </c>
       <c r="C12" s="13">
         <f ca="1"/>
-        <v>0.26799948659394413</v>
+        <v>0.85222715656285697</v>
       </c>
       <c r="E12" s="13">
         <f ca="1"/>
@@ -3356,7 +3387,7 @@
       </c>
       <c r="F12" s="13">
         <f ca="1"/>
-        <v>0.26799948659394413</v>
+        <v>0.85222715656285697</v>
       </c>
     </row>
   </sheetData>
@@ -3395,7 +3426,7 @@
       </c>
       <c r="F2" s="11" cm="1">
         <f t="array" aca="1" ref="F2" ca="1">_xll.\TMX.CURVE.PWFLAT(_xlfn.ANCHORARRAY(B3),_xlfn.ANCHORARRAY(C3))</f>
-        <v>2369230323376</v>
+        <v>1521042482912</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>14</v>
@@ -3411,7 +3442,7 @@
       </c>
       <c r="M2" s="21" cm="1">
         <f t="array" aca="1" ref="M2" ca="1">_xll.\TMX.CURVE.CONSTANT(C3)</f>
-        <v>2369230318192</v>
+        <v>1521042510848</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
@@ -3421,7 +3452,7 @@
       </c>
       <c r="C3" s="8" cm="1">
         <f t="array" aca="1" ref="C3:C12" ca="1">_xlfn.RANDARRAY(ROWS(_xlfn.ANCHORARRAY(B3)))</f>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="F3" s="8" cm="1">
         <f t="array" aca="1" ref="F3:G13" ca="1">TRANSPOSE(_xll.TMX.CURVE.PWFLAT(F2))</f>
@@ -3429,7 +3460,7 @@
       </c>
       <c r="G3" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="I3" s="8" cm="1">
         <f t="array" ref="I3:I103">_xll.ARRAY.SEQUENCE(0,D2,0.1)</f>
@@ -3437,11 +3468,11 @@
       </c>
       <c r="J3" s="8" cm="1">
         <f t="array" aca="1" ref="J3:J103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY($I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.FORWARD(pwflat,_xlpm.t)))</f>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="K3" s="8" cm="1">
         <f t="array" aca="1" ref="K3:K103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY($I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.SPOT(pwflat,_xlpm.t)))</f>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="L3" s="8" cm="1">
         <f t="array" aca="1" ref="L3:L103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY($I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.DISCOUNT(pwflat,_xlpm.t)))</f>
@@ -3449,7 +3480,7 @@
       </c>
       <c r="M3" s="22" cm="1">
         <f t="array" aca="1" ref="M3:M103" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(I3),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.CURVE.FORWARD(M2,_xlpm.t)))</f>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
@@ -3458,7 +3489,7 @@
       </c>
       <c r="C4" s="8">
         <f ca="1"/>
-        <v>0.10371428101934899</v>
+        <v>0.79453585160743101</v>
       </c>
       <c r="F4" s="8">
         <f ca="1"/>
@@ -3466,26 +3497,26 @@
       </c>
       <c r="G4" s="8">
         <f ca="1"/>
-        <v>0.10371428101934899</v>
+        <v>0.79453585160743101</v>
       </c>
       <c r="I4" s="8">
         <v>0.1</v>
       </c>
       <c r="J4" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="K4" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956178</v>
       </c>
       <c r="L4" s="8">
         <f ca="1"/>
-        <v>0.95584579009470738</v>
+        <v>0.96823213025589894</v>
       </c>
       <c r="M4" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
@@ -3494,7 +3525,7 @@
       </c>
       <c r="C5" s="8">
         <f ca="1"/>
-        <v>0.32786045310224088</v>
+        <v>0.242849658381314</v>
       </c>
       <c r="F5" s="8">
         <f ca="1"/>
@@ -3502,26 +3533,26 @@
       </c>
       <c r="G5" s="8">
         <f ca="1"/>
-        <v>0.32786045310224088</v>
+        <v>0.242849658381314</v>
       </c>
       <c r="I5" s="8">
         <v>0.2</v>
       </c>
       <c r="J5" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="K5" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956178</v>
       </c>
       <c r="L5" s="8">
         <f ca="1"/>
-        <v>0.91364117447376736</v>
+        <v>0.93747345796319836</v>
       </c>
       <c r="M5" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
@@ -3530,7 +3561,7 @@
       </c>
       <c r="C6" s="8">
         <f ca="1"/>
-        <v>0.54577121542853657</v>
+        <v>0.74945515068588553</v>
       </c>
       <c r="F6" s="8">
         <f ca="1"/>
@@ -3538,26 +3569,26 @@
       </c>
       <c r="G6" s="8">
         <f ca="1"/>
-        <v>0.54577121542853657</v>
+        <v>0.74945515068588553</v>
       </c>
       <c r="I6" s="8">
         <v>0.30000000000000004</v>
       </c>
       <c r="J6" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="K6" s="8">
         <f ca="1"/>
-        <v>0.45158686362248929</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="L6" s="8">
         <f ca="1"/>
-        <v>0.87330007044285274</v>
+        <v>0.90769192337574878</v>
       </c>
       <c r="M6" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
@@ -3566,7 +3597,7 @@
       </c>
       <c r="C7" s="8">
         <f ca="1"/>
-        <v>0.11805033961160771</v>
+        <v>1.2016145554805346E-2</v>
       </c>
       <c r="F7" s="8">
         <f ca="1"/>
@@ -3574,26 +3605,26 @@
       </c>
       <c r="G7" s="8">
         <f ca="1"/>
-        <v>0.11805033961160771</v>
+        <v>1.2016145554805346E-2</v>
       </c>
       <c r="I7" s="8">
         <v>0.4</v>
       </c>
       <c r="J7" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="K7" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956178</v>
       </c>
       <c r="L7" s="8">
         <f ca="1"/>
-        <v>0.83474019564867263</v>
+        <v>0.8788564846893423</v>
       </c>
       <c r="M7" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
@@ -3602,7 +3633,7 @@
       </c>
       <c r="C8" s="8">
         <f ca="1"/>
-        <v>0.79340484028740965</v>
+        <v>0.85140762941610237</v>
       </c>
       <c r="F8" s="8">
         <f ca="1"/>
@@ -3610,26 +3641,26 @@
       </c>
       <c r="G8" s="8">
         <f ca="1"/>
-        <v>0.79340484028740965</v>
+        <v>0.85140762941610237</v>
       </c>
       <c r="I8" s="8">
         <v>0.5</v>
       </c>
       <c r="J8" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="K8" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="L8" s="8">
         <f ca="1"/>
-        <v>0.79788290170627751</v>
+        <v>0.85093708623691611</v>
       </c>
       <c r="M8" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
@@ -3638,7 +3669,7 @@
       </c>
       <c r="C9" s="8">
         <f ca="1"/>
-        <v>0.54345481613037738</v>
+        <v>0.11763237961991213</v>
       </c>
       <c r="F9" s="8">
         <f ca="1"/>
@@ -3646,26 +3677,26 @@
       </c>
       <c r="G9" s="8">
         <f ca="1"/>
-        <v>0.54345481613037738</v>
+        <v>0.11763237961991213</v>
       </c>
       <c r="I9" s="8">
         <v>0.60000000000000009</v>
       </c>
       <c r="J9" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="K9" s="8">
         <f ca="1"/>
-        <v>0.45158686362248929</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="L9" s="8">
         <f ca="1"/>
-        <v>0.7626530127711818</v>
+        <v>0.82390462768500827</v>
       </c>
       <c r="M9" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
@@ -3674,7 +3705,7 @@
       </c>
       <c r="C10" s="8">
         <f ca="1"/>
-        <v>0.57740717064861236</v>
+        <v>0.47263522532870339</v>
       </c>
       <c r="F10" s="8">
         <f ca="1"/>
@@ -3682,26 +3713,26 @@
       </c>
       <c r="G10" s="8">
         <f ca="1"/>
-        <v>0.57740717064861236</v>
+        <v>0.47263522532870339</v>
       </c>
       <c r="I10" s="8">
         <v>0.70000000000000007</v>
       </c>
       <c r="J10" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="K10" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="L10" s="8">
         <f ca="1"/>
-        <v>0.72897867163330599</v>
+        <v>0.79773093267447071</v>
       </c>
       <c r="M10" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
@@ -3710,7 +3741,7 @@
       </c>
       <c r="C11" s="8">
         <f ca="1"/>
-        <v>0.70384581205313657</v>
+        <v>0.91905236752737207</v>
       </c>
       <c r="F11" s="8">
         <f ca="1"/>
@@ -3718,26 +3749,26 @@
       </c>
       <c r="G11" s="8">
         <f ca="1"/>
-        <v>0.70384581205313657</v>
+        <v>0.91905236752737207</v>
       </c>
       <c r="I11" s="8">
         <v>0.8</v>
       </c>
       <c r="J11" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="K11" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956178</v>
       </c>
       <c r="L11" s="8">
         <f ca="1"/>
-        <v>0.69679119455636829</v>
+        <v>0.77238872048873375</v>
       </c>
       <c r="M11" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
@@ -3746,7 +3777,7 @@
       </c>
       <c r="C12" s="8">
         <f ca="1"/>
-        <v>0.3680418096501068</v>
+        <v>0.76489947289387872</v>
       </c>
       <c r="F12" s="8">
         <f ca="1"/>
@@ -3754,26 +3785,26 @@
       </c>
       <c r="G12" s="8">
         <f ca="1"/>
-        <v>0.3680418096501068</v>
+        <v>0.76489947289387872</v>
       </c>
       <c r="I12" s="8">
         <v>0.9</v>
       </c>
       <c r="J12" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="K12" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="L12" s="8">
         <f ca="1"/>
-        <v>0.66602492960077453</v>
+        <v>0.74785157625186238</v>
       </c>
       <c r="M12" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
@@ -3790,19 +3821,19 @@
       </c>
       <c r="J13" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="K13" s="8">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
       <c r="L13" s="8">
         <f ca="1"/>
-        <v>0.63661712500270429</v>
+        <v>0.72409392485415824</v>
       </c>
       <c r="M13" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
@@ -3811,19 +3842,19 @@
       </c>
       <c r="J14" s="8">
         <f ca="1"/>
-        <v>0.10371428101934899</v>
+        <v>0.79453585160743101</v>
       </c>
       <c r="K14" s="8">
         <f ca="1"/>
-        <v>0.41996208338584018</v>
+        <v>0.36571613622755</v>
       </c>
       <c r="L14" s="8">
         <f ca="1"/>
-        <v>0.63004861751823893</v>
+        <v>0.66878827424454668</v>
       </c>
       <c r="M14" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
@@ -3832,19 +3863,19 @@
       </c>
       <c r="J15" s="8">
         <f ca="1"/>
-        <v>0.10371428101934899</v>
+        <v>0.79453585160743101</v>
       </c>
       <c r="K15" s="8">
         <f ca="1"/>
-        <v>0.39360809985529926</v>
+        <v>0.40145111250920679</v>
       </c>
       <c r="L15" s="8">
         <f ca="1"/>
-        <v>0.62354788277378315</v>
+        <v>0.61770682005195499</v>
       </c>
       <c r="M15" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
@@ -3853,19 +3884,19 @@
       </c>
       <c r="J16" s="8">
         <f ca="1"/>
-        <v>0.10371428101934899</v>
+        <v>0.79453585160743101</v>
       </c>
       <c r="K16" s="8">
         <f ca="1"/>
-        <v>0.37130857532945694</v>
+        <v>0.43168840013214704</v>
       </c>
       <c r="L16" s="8">
         <f ca="1"/>
-        <v>0.61711422150063466</v>
+        <v>0.570526922291264</v>
       </c>
       <c r="M16" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="17" spans="9:13" x14ac:dyDescent="0.3">
@@ -3874,19 +3905,19 @@
       </c>
       <c r="J17" s="8">
         <f ca="1"/>
-        <v>0.10371428101934899</v>
+        <v>0.79453585160743101</v>
       </c>
       <c r="K17" s="8">
         <f ca="1"/>
-        <v>0.35219469716444923</v>
+        <v>0.4576060752375245</v>
       </c>
       <c r="L17" s="8">
         <f ca="1"/>
-        <v>0.61074694164484944</v>
+        <v>0.52695058312653187</v>
       </c>
       <c r="M17" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="18" spans="9:13" x14ac:dyDescent="0.3">
@@ -3895,19 +3926,19 @@
       </c>
       <c r="J18" s="8">
         <f ca="1"/>
-        <v>0.10371428101934899</v>
+        <v>0.79453585160743101</v>
       </c>
       <c r="K18" s="8">
         <f ca="1"/>
-        <v>0.33562933608810924</v>
+        <v>0.48006806032885158</v>
       </c>
       <c r="L18" s="8">
         <f ca="1"/>
-        <v>0.60444535829277535</v>
+        <v>0.48670256635646286</v>
       </c>
       <c r="M18" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="19" spans="9:13" x14ac:dyDescent="0.3">
@@ -3916,19 +3947,19 @@
       </c>
       <c r="J19" s="8">
         <f ca="1"/>
-        <v>0.10371428101934899</v>
+        <v>0.79453585160743101</v>
       </c>
       <c r="K19" s="8">
         <f ca="1"/>
-        <v>0.32113464514631168</v>
+        <v>0.49972229728376283</v>
       </c>
       <c r="L19" s="8">
         <f ca="1"/>
-        <v>0.59820879359735324</v>
+        <v>0.44952865614187038</v>
       </c>
       <c r="M19" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="20" spans="9:13" x14ac:dyDescent="0.3">
@@ -3937,19 +3968,19 @@
       </c>
       <c r="J20" s="8">
         <f ca="1"/>
-        <v>0.10371428101934899</v>
+        <v>0.79453585160743101</v>
       </c>
       <c r="K20" s="8">
         <f ca="1"/>
-        <v>0.30834521196237274</v>
+        <v>0.51706427106750796</v>
       </c>
       <c r="L20" s="8">
         <f ca="1"/>
-        <v>0.59203657670517373</v>
+        <v>0.41519405658485792</v>
       </c>
       <c r="M20" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="21" spans="9:13" x14ac:dyDescent="0.3">
@@ -3958,19 +3989,19 @@
       </c>
       <c r="J21" s="8">
         <f ca="1"/>
-        <v>0.10371428101934899</v>
+        <v>0.79453585160743101</v>
       </c>
       <c r="K21" s="8">
         <f ca="1"/>
-        <v>0.29697682690998251</v>
+        <v>0.53247935887528153</v>
       </c>
       <c r="L21" s="8">
         <f ca="1"/>
-        <v>0.58592804368428497</v>
+        <v>0.38348190399196003</v>
       </c>
       <c r="M21" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="22" spans="9:13" x14ac:dyDescent="0.3">
@@ -3979,19 +4010,19 @@
       </c>
       <c r="J22" s="8">
         <f ca="1"/>
-        <v>0.10371428101934899</v>
+        <v>0.79453585160743101</v>
       </c>
       <c r="K22" s="8">
         <f ca="1"/>
-        <v>0.28680511396837022</v>
+        <v>0.54627180586118407</v>
       </c>
       <c r="L22" s="8">
         <f ca="1"/>
-        <v>0.57988253745273866</v>
+        <v>0.35419189712363663</v>
       </c>
       <c r="M22" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="23" spans="9:13" x14ac:dyDescent="0.3">
@@ -4000,19 +4031,19 @@
       </c>
       <c r="J23" s="8">
         <f ca="1"/>
-        <v>0.10371428101934899</v>
+        <v>0.79453585160743101</v>
       </c>
       <c r="K23" s="8">
         <f ca="1"/>
-        <v>0.27765057232091916</v>
+        <v>0.55868500814849642</v>
       </c>
       <c r="L23" s="8">
         <f ca="1"/>
-        <v>0.57389940770787395</v>
+        <v>0.32713903519294757</v>
       </c>
       <c r="M23" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="24" spans="9:13" x14ac:dyDescent="0.3">
@@ -4021,19 +4052,19 @@
       </c>
       <c r="J24" s="8">
         <f ca="1"/>
-        <v>0.32786045310224088</v>
+        <v>0.242849658381314</v>
       </c>
       <c r="K24" s="8">
         <f ca="1"/>
-        <v>0.28004151902479163</v>
+        <v>0.54364522958815442</v>
       </c>
       <c r="L24" s="8">
         <f ca="1"/>
-        <v>0.55538862234902608</v>
+        <v>0.31929016562462759</v>
       </c>
       <c r="M24" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="25" spans="9:13" x14ac:dyDescent="0.3">
@@ -4042,19 +4073,19 @@
       </c>
       <c r="J25" s="8">
         <f ca="1"/>
-        <v>0.32786045310224088</v>
+        <v>0.242849658381314</v>
       </c>
       <c r="K25" s="8">
         <f ca="1"/>
-        <v>0.28221510693740293</v>
+        <v>0.52997270362420712</v>
       </c>
       <c r="L25" s="8">
         <f ca="1"/>
-        <v>0.53747489071081622</v>
+        <v>0.31162960979809373</v>
       </c>
       <c r="M25" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="26" spans="9:13" x14ac:dyDescent="0.3">
@@ -4063,19 +4094,19 @@
       </c>
       <c r="J26" s="8">
         <f ca="1"/>
-        <v>0.32786045310224088</v>
+        <v>0.242849658381314</v>
       </c>
       <c r="K26" s="8">
         <f ca="1"/>
-        <v>0.28419968720543937</v>
+        <v>0.51748909296147261</v>
       </c>
       <c r="L26" s="8">
         <f ca="1"/>
-        <v>0.52013895593760018</v>
+        <v>0.30415284807518017</v>
       </c>
       <c r="M26" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="27" spans="9:13" x14ac:dyDescent="0.3">
@@ -4084,19 +4115,19 @@
       </c>
       <c r="J27" s="8">
         <f ca="1"/>
-        <v>0.32786045310224088</v>
+        <v>0.242849658381314</v>
       </c>
       <c r="K27" s="8">
         <f ca="1"/>
-        <v>0.28601888578447277</v>
+        <v>0.50604578318729931</v>
       </c>
       <c r="L27" s="8">
         <f ca="1"/>
-        <v>0.5033621815569127</v>
+        <v>0.29685547339244911</v>
       </c>
       <c r="M27" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="28" spans="9:13" x14ac:dyDescent="0.3">
@@ -4105,19 +4136,19 @@
       </c>
       <c r="J28" s="8">
         <f ca="1"/>
-        <v>0.32786045310224088</v>
+        <v>0.242849658381314</v>
       </c>
       <c r="K28" s="8">
         <f ca="1"/>
-        <v>0.28769254847718351</v>
+        <v>0.49551793819505996</v>
       </c>
       <c r="L28" s="8">
         <f ca="1"/>
-        <v>0.48712653221640462</v>
+        <v>0.28973318065768738</v>
       </c>
       <c r="M28" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="29" spans="9:13" x14ac:dyDescent="0.3">
@@ -4126,19 +4157,19 @@
       </c>
       <c r="J29" s="8">
         <f ca="1"/>
-        <v>0.32786045310224088</v>
+        <v>0.242849658381314</v>
       </c>
       <c r="K29" s="8">
         <f ca="1"/>
-        <v>0.28923746788583954</v>
+        <v>0.48579992743299277</v>
       </c>
       <c r="L29" s="8">
         <f ca="1"/>
-        <v>0.47141455321001702</v>
+        <v>0.28278176922111914</v>
       </c>
       <c r="M29" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="30" spans="9:13" x14ac:dyDescent="0.3">
@@ -4147,19 +4178,19 @@
       </c>
       <c r="J30" s="8">
         <f ca="1"/>
-        <v>0.32786045310224088</v>
+        <v>0.242849658381314</v>
       </c>
       <c r="K30" s="8">
         <f ca="1"/>
-        <v>0.29066794881978036</v>
+        <v>0.47680176931996765</v>
       </c>
       <c r="L30" s="8">
         <f ca="1"/>
-        <v>0.45620935542714453</v>
+        <v>0.27599713921607372</v>
       </c>
       <c r="M30" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="31" spans="9:13" x14ac:dyDescent="0.3">
@@ -4168,19 +4199,19 @@
       </c>
       <c r="J31" s="8">
         <f ca="1"/>
-        <v>0.32786045310224088</v>
+        <v>0.242849658381314</v>
       </c>
       <c r="K31" s="8">
         <f ca="1"/>
-        <v>0.29199625254415396</v>
+        <v>0.46844633678644432</v>
       </c>
       <c r="L31" s="8">
         <f ca="1"/>
-        <v>0.44149459228403304</v>
+        <v>0.2693752891407778</v>
       </c>
       <c r="M31" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="32" spans="9:13" x14ac:dyDescent="0.3">
@@ -4189,19 +4220,19 @@
       </c>
       <c r="J32" s="8">
         <f ca="1"/>
-        <v>0.32786045310224088</v>
+        <v>0.242849658381314</v>
       </c>
       <c r="K32" s="8">
         <f ca="1"/>
-        <v>0.29323294911512243</v>
+        <v>0.46066714097937084</v>
       </c>
       <c r="L32" s="8">
         <f ca="1"/>
-        <v>0.42725444508808941</v>
+        <v>0.26291231349813321</v>
       </c>
       <c r="M32" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="33" spans="9:13" x14ac:dyDescent="0.3">
@@ -4210,19 +4241,19 @@
       </c>
       <c r="J33" s="8">
         <f ca="1"/>
-        <v>0.32786045310224088</v>
+        <v>0.242849658381314</v>
       </c>
       <c r="K33" s="8">
         <f ca="1"/>
-        <v>0.29438719924802642</v>
+        <v>0.45340655822610226</v>
       </c>
       <c r="L33" s="8">
         <f ca="1"/>
-        <v>0.4134736053635803</v>
+        <v>0.25660440049208433</v>
       </c>
       <c r="M33" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="34" spans="9:13" x14ac:dyDescent="0.3">
@@ -4231,19 +4262,19 @@
       </c>
       <c r="J34" s="8">
         <f ca="1"/>
-        <v>0.54577121542853657</v>
+        <v>0.74945515068588553</v>
       </c>
       <c r="K34" s="8">
         <f ca="1"/>
-        <v>0.30249636106030092</v>
+        <v>0.46295651282157918</v>
       </c>
       <c r="L34" s="8">
         <f ca="1"/>
-        <v>0.39151215311812443</v>
+        <v>0.23807603320492313</v>
       </c>
       <c r="M34" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="35" spans="9:13" x14ac:dyDescent="0.3">
@@ -4252,19 +4283,19 @@
       </c>
       <c r="J35" s="8">
         <f ca="1"/>
-        <v>0.54577121542853657</v>
+        <v>0.74945515068588553</v>
       </c>
       <c r="K35" s="8">
         <f ca="1"/>
-        <v>0.3100987002593083</v>
+        <v>0.47190959525483872</v>
       </c>
       <c r="L35" s="8">
         <f ca="1"/>
-        <v>0.37071717432142454</v>
+        <v>0.22088552385294191</v>
       </c>
       <c r="M35" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="36" spans="9:13" x14ac:dyDescent="0.3">
@@ -4273,19 +4304,19 @@
       </c>
       <c r="J36" s="8">
         <f ca="1"/>
-        <v>0.54577121542853657</v>
+        <v>0.74945515068588553</v>
       </c>
       <c r="K36" s="8">
         <f ca="1"/>
-        <v>0.31724029162807282</v>
+        <v>0.48032006663153715</v>
       </c>
       <c r="L36" s="8">
         <f ca="1"/>
-        <v>0.35102670998062613</v>
+        <v>0.20493627199603032</v>
       </c>
       <c r="M36" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="37" spans="9:13" x14ac:dyDescent="0.3">
@@ -4294,19 +4325,19 @@
       </c>
       <c r="J37" s="8">
         <f ca="1"/>
-        <v>0.54577121542853657</v>
+        <v>0.74945515068588553</v>
       </c>
       <c r="K37" s="8">
         <f ca="1"/>
-        <v>0.32396178938691</v>
+        <v>0.48823580439784148</v>
       </c>
       <c r="L37" s="8">
         <f ca="1"/>
-        <v>0.3323820953102104</v>
+        <v>0.19013865160652069</v>
       </c>
       <c r="M37" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="38" spans="9:13" x14ac:dyDescent="0.3">
@@ -4315,19 +4346,19 @@
       </c>
       <c r="J38" s="8">
         <f ca="1"/>
-        <v>0.54577121542853657</v>
+        <v>0.74945515068588553</v>
       </c>
       <c r="K38" s="8">
         <f ca="1"/>
-        <v>0.33029920155952786</v>
+        <v>0.49569921429178559</v>
       </c>
       <c r="L38" s="8">
         <f ca="1"/>
-        <v>0.31472778059974754</v>
+        <v>0.17640950534647309</v>
       </c>
       <c r="M38" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="39" spans="9:13" x14ac:dyDescent="0.3">
@@ -4336,19 +4367,19 @@
       </c>
       <c r="J39" s="8">
         <f ca="1"/>
-        <v>0.54577121542853657</v>
+        <v>0.74945515068588553</v>
       </c>
       <c r="K39" s="8">
         <f ca="1"/>
-        <v>0.33628453527811142</v>
+        <v>0.50274799030273287</v>
       </c>
       <c r="L39" s="8">
         <f ca="1"/>
-        <v>0.29801116476673595</v>
+        <v>0.16367168660800263</v>
       </c>
       <c r="M39" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="40" spans="9:13" x14ac:dyDescent="0.3">
@@ -4357,19 +4388,19 @@
       </c>
       <c r="J40" s="8">
         <f ca="1"/>
-        <v>0.54577121542853657</v>
+        <v>0.74945515068588553</v>
       </c>
       <c r="K40" s="8">
         <f ca="1"/>
-        <v>0.34194633744433917</v>
+        <v>0.50941575139416939</v>
       </c>
       <c r="L40" s="8">
         <f ca="1"/>
-        <v>0.282182444886937</v>
+        <v>0.15185361409531142</v>
       </c>
       <c r="M40" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="41" spans="9:13" x14ac:dyDescent="0.3">
@@ -4378,19 +4409,19 @@
       </c>
       <c r="J41" s="8">
         <f ca="1"/>
-        <v>0.54577121542853657</v>
+        <v>0.74945515068588553</v>
       </c>
       <c r="K41" s="8">
         <f ca="1"/>
-        <v>0.34731015002287069</v>
+        <v>0.51573257769131986</v>
       </c>
       <c r="L41" s="8">
         <f ca="1"/>
-        <v>0.26719445974938616</v>
+        <v>0.14088887871153832</v>
       </c>
       <c r="M41" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="42" spans="9:13" x14ac:dyDescent="0.3">
@@ -4399,19 +4430,19 @@
       </c>
       <c r="J42" s="8">
         <f ca="1"/>
-        <v>0.54577121542853657</v>
+        <v>0.74945515068588553</v>
       </c>
       <c r="K42" s="8">
         <f ca="1"/>
-        <v>0.3523988952896826</v>
+        <v>0.52172546417835997</v>
       </c>
       <c r="L42" s="8">
         <f ca="1"/>
-        <v>0.25300255406401595</v>
+        <v>0.13071586159670365</v>
       </c>
       <c r="M42" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="43" spans="9:13" x14ac:dyDescent="0.3">
@@ -4420,19 +4451,19 @@
       </c>
       <c r="J43" s="8">
         <f ca="1"/>
-        <v>0.54577121542853657</v>
+        <v>0.74945515068588553</v>
       </c>
       <c r="K43" s="8">
         <f ca="1"/>
-        <v>0.35723320329315394</v>
+        <v>0.52741870634104804</v>
       </c>
       <c r="L43" s="8">
         <f ca="1"/>
-        <v>0.23956444604310673</v>
+        <v>0.12127739717239043</v>
       </c>
       <c r="M43" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="44" spans="9:13" x14ac:dyDescent="0.3">
@@ -4441,19 +4472,19 @@
       </c>
       <c r="J44" s="8">
         <f ca="1"/>
-        <v>0.11805033961160771</v>
+        <v>1.2016145554805346E-2</v>
       </c>
       <c r="K44" s="8">
         <f ca="1"/>
-        <v>0.35139947491067719</v>
+        <v>0.51484791217552994</v>
       </c>
       <c r="L44" s="8">
         <f ca="1"/>
-        <v>0.23675300686026765</v>
+        <v>0.12113175601537184</v>
       </c>
       <c r="M44" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="45" spans="9:13" x14ac:dyDescent="0.3">
@@ -4462,19 +4493,19 @@
       </c>
       <c r="J45" s="8">
         <f ca="1"/>
-        <v>0.11805033961160771</v>
+        <v>1.2016145554805346E-2</v>
       </c>
       <c r="K45" s="8">
         <f ca="1"/>
-        <v>0.34584354311784216</v>
+        <v>0.50287572725598884</v>
       </c>
       <c r="L45" s="8">
         <f ca="1"/>
-        <v>0.2339745616841919</v>
+        <v>0.12098628975786654</v>
       </c>
       <c r="M45" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="46" spans="9:13" x14ac:dyDescent="0.3">
@@ -4483,19 +4514,19 @@
       </c>
       <c r="J46" s="8">
         <f ca="1"/>
-        <v>0.11805033961160771</v>
+        <v>1.2016145554805346E-2</v>
       </c>
       <c r="K46" s="8">
         <f ca="1"/>
-        <v>0.34054602675723211</v>
+        <v>0.49146038814665904</v>
       </c>
       <c r="L46" s="8">
         <f ca="1"/>
-        <v>0.23122872330977937</v>
+        <v>0.12084099818983977</v>
       </c>
       <c r="M46" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="47" spans="9:13" x14ac:dyDescent="0.3">
@@ -4504,19 +4535,19 @@
       </c>
       <c r="J47" s="8">
         <f ca="1"/>
-        <v>0.11805033961160771</v>
+        <v>1.2016145554805346E-2</v>
       </c>
       <c r="K47" s="8">
         <f ca="1"/>
-        <v>0.33548930659483156</v>
+        <v>0.48056392808775317</v>
       </c>
       <c r="L47" s="8">
         <f ca="1"/>
-        <v>0.2285151090760541</v>
+        <v>0.12069588110150918</v>
       </c>
       <c r="M47" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="48" spans="9:13" x14ac:dyDescent="0.3">
@@ -4525,19 +4556,19 @@
       </c>
       <c r="J48" s="8">
         <f ca="1"/>
-        <v>0.11805033961160771</v>
+        <v>1.2016145554805346E-2</v>
       </c>
       <c r="K48" s="8">
         <f ca="1"/>
-        <v>0.33065732955075994</v>
+        <v>0.47015175514257668</v>
       </c>
       <c r="L48" s="8">
         <f ca="1"/>
-        <v>0.22583334081283973</v>
+        <v>0.12055093828334357</v>
       </c>
       <c r="M48" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="49" spans="9:13" x14ac:dyDescent="0.3">
@@ -4546,19 +4577,19 @@
       </c>
       <c r="J49" s="8">
         <f ca="1"/>
-        <v>0.11805033961160771</v>
+        <v>1.2016145554805346E-2</v>
       </c>
       <c r="K49" s="8">
         <f ca="1"/>
-        <v>0.32603543846512617</v>
+        <v>0.46019228536892937</v>
       </c>
       <c r="L49" s="8">
         <f ca="1"/>
-        <v>0.22318304478805881</v>
+        <v>0.1204061695260641</v>
       </c>
       <c r="M49" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="50" spans="9:13" x14ac:dyDescent="0.3">
@@ -4567,19 +4598,19 @@
       </c>
       <c r="J50" s="8">
         <f ca="1"/>
-        <v>0.11805033961160771</v>
+        <v>1.2016145554805346E-2</v>
       </c>
       <c r="K50" s="8">
         <f ca="1"/>
-        <v>0.32161022359590236</v>
+        <v>0.45065662281969276</v>
       </c>
       <c r="L50" s="8">
         <f ca="1"/>
-        <v>0.22056385165565348</v>
+        <v>0.12026157462064305</v>
       </c>
       <c r="M50" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="51" spans="9:13" x14ac:dyDescent="0.3">
@@ -4588,19 +4619,19 @@
       </c>
       <c r="J51" s="8">
         <f ca="1"/>
-        <v>0.11805033961160771</v>
+        <v>1.2016145554805346E-2</v>
       </c>
       <c r="K51" s="8">
         <f ca="1"/>
-        <v>0.31736939267956288</v>
+        <v>0.44151827954334083</v>
       </c>
       <c r="L51" s="8">
         <f ca="1"/>
-        <v>0.2179753964041149</v>
+        <v>0.12011715335830372</v>
       </c>
       <c r="M51" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="52" spans="9:13" x14ac:dyDescent="0.3">
@@ -4609,19 +4640,19 @@
       </c>
       <c r="J52" s="8">
         <f ca="1"/>
-        <v>0.11805033961160771</v>
+        <v>1.2016145554805346E-2</v>
       </c>
       <c r="K52" s="8">
         <f ca="1"/>
-        <v>0.31330165690266581</v>
+        <v>0.4327529298701055</v>
       </c>
       <c r="L52" s="8">
         <f ca="1"/>
-        <v>0.21541731830561989</v>
+        <v>0.11997290553051994</v>
       </c>
       <c r="M52" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="53" spans="9:13" x14ac:dyDescent="0.3">
@@ -4630,19 +4661,19 @@
       </c>
       <c r="J53" s="8">
         <f ca="1"/>
-        <v>0.11805033961160771</v>
+        <v>1.2016145554805346E-2</v>
       </c>
       <c r="K53" s="8">
         <f ca="1"/>
-        <v>0.30939663055684469</v>
+        <v>0.42433819418379953</v>
       </c>
       <c r="L53" s="8">
         <f ca="1"/>
-        <v>0.21288926086576171</v>
+        <v>0.11982883092901617</v>
       </c>
       <c r="M53" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="54" spans="9:13" x14ac:dyDescent="0.3">
@@ -4651,19 +4682,19 @@
       </c>
       <c r="J54" s="8">
         <f ca="1"/>
-        <v>0.79340484028740965</v>
+        <v>0.85140762941610237</v>
       </c>
       <c r="K54" s="8">
         <f ca="1"/>
-        <v>0.3188869876103852</v>
+        <v>0.43271210467855065</v>
       </c>
       <c r="L54" s="8">
         <f ca="1"/>
-        <v>0.19665120910369796</v>
+        <v>0.11004876031468627</v>
       </c>
       <c r="M54" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="55" spans="9:13" x14ac:dyDescent="0.3">
@@ -4672,19 +4703,19 @@
       </c>
       <c r="J55" s="8">
         <f ca="1"/>
-        <v>0.79340484028740965</v>
+        <v>0.85140762941610237</v>
       </c>
       <c r="K55" s="8">
         <f ca="1"/>
-        <v>0.32801233093109722</v>
+        <v>0.44076394169273431</v>
       </c>
       <c r="L55" s="8">
         <f ca="1"/>
-        <v>0.18165170719951809</v>
+        <v>0.10106691052882588</v>
       </c>
       <c r="M55" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="56" spans="9:13" x14ac:dyDescent="0.3">
@@ -4693,19 +4724,19 @@
       </c>
       <c r="J56" s="8">
         <f ca="1"/>
-        <v>0.79340484028740965</v>
+        <v>0.85140762941610237</v>
       </c>
       <c r="K56" s="8">
         <f ca="1"/>
-        <v>0.33679332167366915</v>
+        <v>0.44851193580072241</v>
       </c>
       <c r="L56" s="8">
         <f ca="1"/>
-        <v>0.16779628785901271</v>
+        <v>9.2818132169083495E-2</v>
       </c>
       <c r="M56" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="57" spans="9:13" x14ac:dyDescent="0.3">
@@ -4714,19 +4745,19 @@
       </c>
       <c r="J57" s="8">
         <f ca="1"/>
-        <v>0.79340484028740965</v>
+        <v>0.85140762941610237</v>
       </c>
       <c r="K57" s="8">
         <f ca="1"/>
-        <v>0.34524909053688657</v>
+        <v>0.45597296716397018</v>
       </c>
       <c r="L57" s="8">
         <f ca="1"/>
-        <v>0.15499768544064438</v>
+        <v>8.5242593988821835E-2</v>
       </c>
       <c r="M57" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="58" spans="9:13" x14ac:dyDescent="0.3">
@@ -4735,19 +4766,19 @@
       </c>
       <c r="J58" s="8">
         <f ca="1"/>
-        <v>0.79340484028740965</v>
+        <v>0.85140762941610237</v>
       </c>
       <c r="K58" s="8">
         <f ca="1"/>
-        <v>0.35339737689598699</v>
+        <v>0.46316268829582707</v>
       </c>
       <c r="L58" s="8">
         <f ca="1"/>
-        <v>0.14317529339494325</v>
+        <v>7.8285351064404235E-2</v>
       </c>
       <c r="M58" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="59" spans="9:13" x14ac:dyDescent="0.3">
@@ -4756,19 +4787,19 @@
       </c>
       <c r="J59" s="8">
         <f ca="1"/>
-        <v>0.79340484028740965</v>
+        <v>0.85140762941610237</v>
       </c>
       <c r="K59" s="8">
         <f ca="1"/>
-        <v>0.36125465302797671</v>
+        <v>0.47009563367297491</v>
       </c>
       <c r="L59" s="8">
         <f ca="1"/>
-        <v>0.13225464924163727</v>
+        <v>7.1895936002493735E-2</v>
       </c>
       <c r="M59" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="60" spans="9:13" x14ac:dyDescent="0.3">
@@ -4777,19 +4808,19 @@
       </c>
       <c r="J60" s="8">
         <f ca="1"/>
-        <v>0.79340484028740965</v>
+        <v>0.85140762941610237</v>
       </c>
       <c r="K60" s="8">
         <f ca="1"/>
-        <v>0.36883623526059828</v>
+        <v>0.47678531780881922</v>
       </c>
       <c r="L60" s="8">
         <f ca="1"/>
-        <v>0.1221669735063096</v>
+        <v>6.6028006104521808E-2</v>
       </c>
       <c r="M60" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="61" spans="9:13" x14ac:dyDescent="0.3">
@@ -4798,19 +4829,19 @@
       </c>
       <c r="J61" s="8">
         <f ca="1"/>
-        <v>0.79340484028740965</v>
+        <v>0.85140762941610237</v>
       </c>
       <c r="K61" s="8">
         <f ca="1"/>
-        <v>0.37615638362312959</v>
+        <v>0.48324432318135863</v>
       </c>
       <c r="L61" s="8">
         <f ca="1"/>
-        <v>0.1128487319646348</v>
+        <v>6.0638996892104349E-2</v>
       </c>
       <c r="M61" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="62" spans="9:13" x14ac:dyDescent="0.3">
@@ -4819,19 +4850,19 @@
       </c>
       <c r="J62" s="8">
         <f ca="1"/>
-        <v>0.79340484028740965</v>
+        <v>0.85140762941610237</v>
       </c>
       <c r="K62" s="8">
         <f ca="1"/>
-        <v>0.38322839136320208</v>
+        <v>0.4894843792192356</v>
       </c>
       <c r="L62" s="8">
         <f ca="1"/>
-        <v>0.10424123357619276</v>
+        <v>5.5689823653834583E-2</v>
       </c>
       <c r="M62" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="63" spans="9:13" x14ac:dyDescent="0.3">
@@ -4840,19 +4871,19 @@
       </c>
       <c r="J63" s="8">
         <f ca="1"/>
-        <v>0.79340484028740965</v>
+        <v>0.85140762941610237</v>
       </c>
       <c r="K63" s="8">
         <f ca="1"/>
-        <v>0.39006466551193886</v>
+        <v>0.49551643338918333</v>
       </c>
       <c r="L63" s="8">
         <f ca="1"/>
-        <v>9.629027040705733E-2</v>
+        <v>5.1144586865274379E-2</v>
       </c>
       <c r="M63" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="64" spans="9:13" x14ac:dyDescent="0.3">
@@ -4861,19 +4892,19 @@
       </c>
       <c r="J64" s="8">
         <f ca="1"/>
-        <v>0.54345481613037738</v>
+        <v>0.11763237961991213</v>
       </c>
       <c r="K64" s="8">
         <f ca="1"/>
-        <v>0.39257925814502803</v>
+        <v>0.48932161283558867</v>
       </c>
       <c r="L64" s="8">
         <f ca="1"/>
-        <v>9.1196981058199109E-2</v>
+        <v>5.0546485522135261E-2</v>
       </c>
       <c r="M64" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="65" spans="9:13" x14ac:dyDescent="0.3">
@@ -4882,19 +4913,19 @@
       </c>
       <c r="J65" s="8">
         <f ca="1"/>
-        <v>0.54345481613037738</v>
+        <v>0.11763237961991213</v>
       </c>
       <c r="K65" s="8">
         <f ca="1"/>
-        <v>0.39501273488672717</v>
+        <v>0.48332662520307779</v>
       </c>
       <c r="L65" s="8">
         <f ca="1"/>
-        <v>8.637310188815539E-2</v>
+        <v>4.9955378560831577E-2</v>
       </c>
       <c r="M65" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="66" spans="9:13" x14ac:dyDescent="0.3">
@@ -4903,19 +4934,19 @@
       </c>
       <c r="J66" s="8">
         <f ca="1"/>
-        <v>0.54345481613037738</v>
+        <v>0.11763237961991213</v>
       </c>
       <c r="K66" s="8">
         <f ca="1"/>
-        <v>0.39736895839853115</v>
+        <v>0.47752195463826563</v>
       </c>
       <c r="L66" s="8">
         <f ca="1"/>
-        <v>8.1804384662577612E-2</v>
+        <v>4.9371184186253442E-2</v>
       </c>
       <c r="M66" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="67" spans="9:13" x14ac:dyDescent="0.3">
@@ -4924,19 +4955,19 @@
       </c>
       <c r="J67" s="8">
         <f ca="1"/>
-        <v>0.54345481613037738</v>
+        <v>0.11763237961991213</v>
       </c>
       <c r="K67" s="8">
         <f ca="1"/>
-        <v>0.39965154992559127</v>
+        <v>0.47189868002860386</v>
       </c>
       <c r="L67" s="8">
         <f ca="1"/>
-        <v>7.7477329015913518E-2</v>
+        <v>4.8793821559793851E-2</v>
       </c>
       <c r="M67" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="68" spans="9:13" x14ac:dyDescent="0.3">
@@ -4945,19 +4976,19 @@
       </c>
       <c r="J68" s="8">
         <f ca="1"/>
-        <v>0.54345481613037738</v>
+        <v>0.11763237961991213</v>
       </c>
       <c r="K68" s="8">
         <f ca="1"/>
-        <v>0.40186390786720333</v>
+        <v>0.46644842925308555</v>
       </c>
       <c r="L68" s="8">
         <f ca="1"/>
-        <v>7.3379153728672736E-2</v>
+        <v>4.8223210788156445E-2</v>
       </c>
       <c r="M68" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="69" spans="9:13" x14ac:dyDescent="0.3">
@@ -4966,19 +4997,19 @@
       </c>
       <c r="J69" s="8">
         <f ca="1"/>
-        <v>0.54345481613037738</v>
+        <v>0.11763237961991213</v>
       </c>
       <c r="K69" s="8">
         <f ca="1"/>
-        <v>0.40400922465906963</v>
+        <v>0.46116333759197681</v>
       </c>
       <c r="L69" s="8">
         <f ca="1"/>
-        <v>6.9497752168345181E-2</v>
+        <v>4.7659272912297226E-2</v>
       </c>
       <c r="M69" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="70" spans="9:13" x14ac:dyDescent="0.3">
@@ -4987,19 +5018,19 @@
       </c>
       <c r="J70" s="8">
         <f ca="1"/>
-        <v>0.54345481613037738</v>
+        <v>0.11763237961991213</v>
       </c>
       <c r="K70" s="8">
         <f ca="1"/>
-        <v>0.406090502143716</v>
+        <v>0.45603600986105047</v>
       </c>
       <c r="L70" s="8">
         <f ca="1"/>
-        <v>6.5821658096522503E-2</v>
+        <v>4.7101929896501402E-2</v>
       </c>
       <c r="M70" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="71" spans="9:13" x14ac:dyDescent="0.3">
@@ -5008,19 +5039,19 @@
       </c>
       <c r="J71" s="8">
         <f ca="1"/>
-        <v>0.54345481613037738</v>
+        <v>0.11763237961991213</v>
       </c>
       <c r="K71" s="8">
         <f ca="1"/>
-        <v>0.40811056558469638</v>
+        <v>0.45105948588691613</v>
       </c>
       <c r="L71" s="8">
         <f ca="1"/>
-        <v>6.2340011799436039E-2</v>
+        <v>4.6551104617577152E-2</v>
       </c>
       <c r="M71" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="72" spans="9:13" x14ac:dyDescent="0.3">
@@ -5029,19 +5060,19 @@
       </c>
       <c r="J72" s="8">
         <f ca="1"/>
-        <v>0.54345481613037738</v>
+        <v>0.11763237961991213</v>
       </c>
       <c r="K72" s="8">
         <f ca="1"/>
-        <v>0.41007207646216992</v>
+        <v>0.4462272089844958</v>
       </c>
       <c r="L72" s="8">
         <f ca="1"/>
-        <v>5.9042524868168411E-2</v>
+        <v>4.6006723263969547E-2</v>
       </c>
       <c r="M72" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="73" spans="9:13" x14ac:dyDescent="0.3">
@@ -5050,19 +5081,19 @@
       </c>
       <c r="J73" s="8">
         <f ca="1"/>
-        <v>0.54345481613037738</v>
+        <v>0.11763237961991213</v>
       </c>
       <c r="K73" s="8">
         <f ca="1"/>
-        <v>0.41197754417171584</v>
+        <v>0.44153299713643029</v>
       </c>
       <c r="L73" s="8">
         <f ca="1"/>
-        <v>5.5919461025051465E-2</v>
+        <v>4.5468705877041458E-2</v>
       </c>
       <c r="M73" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="74" spans="9:13" x14ac:dyDescent="0.3">
@@ -5071,19 +5102,19 @@
       </c>
       <c r="J74" s="8">
         <f ca="1"/>
-        <v>0.57740717064861236</v>
+        <v>0.47263522532870339</v>
       </c>
       <c r="K74" s="8">
         <f ca="1"/>
-        <v>0.41430753891082706</v>
+        <v>0.44197105668843417</v>
       </c>
       <c r="L74" s="8">
         <f ca="1"/>
-        <v>5.2782079867438436E-2</v>
+        <v>4.3369689006246964E-2</v>
       </c>
       <c r="M74" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="75" spans="9:13" x14ac:dyDescent="0.3">
@@ -5092,19 +5123,19 @@
       </c>
       <c r="J75" s="8">
         <f ca="1"/>
-        <v>0.57740717064861236</v>
+        <v>0.47263522532870339</v>
       </c>
       <c r="K75" s="8">
         <f ca="1"/>
-        <v>0.41657281157385184</v>
+        <v>0.44239694791954898</v>
       </c>
       <c r="L75" s="8">
         <f ca="1"/>
-        <v>4.9820722433902634E-2</v>
+        <v>4.136757118455376E-2</v>
       </c>
       <c r="M75" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="76" spans="9:13" x14ac:dyDescent="0.3">
@@ -5113,19 +5144,19 @@
       </c>
       <c r="J76" s="8">
         <f ca="1"/>
-        <v>0.57740717064861236</v>
+        <v>0.47263522532870339</v>
       </c>
       <c r="K76" s="8">
         <f ca="1"/>
-        <v>0.4187760219721362</v>
+        <v>0.44281117089775662</v>
       </c>
       <c r="L76" s="8">
         <f ca="1"/>
-        <v>4.702551279382753E-2</v>
+        <v>3.9457879181157049E-2</v>
       </c>
       <c r="M76" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="77" spans="9:13" x14ac:dyDescent="0.3">
@@ -5134,19 +5165,19 @@
       </c>
       <c r="J77" s="8">
         <f ca="1"/>
-        <v>0.57740717064861236</v>
+        <v>0.47263522532870339</v>
       </c>
       <c r="K77" s="8">
         <f ca="1"/>
-        <v>0.42091968614343994</v>
+        <v>0.44321419866033696</v>
       </c>
       <c r="L77" s="8">
         <f ca="1"/>
-        <v>4.4387132123971933E-2</v>
+        <v>3.7636346272403504E-2</v>
       </c>
       <c r="M77" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="78" spans="9:13" x14ac:dyDescent="0.3">
@@ -5155,19 +5186,19 @@
       </c>
       <c r="J78" s="8">
         <f ca="1"/>
-        <v>0.57740717064861236</v>
+        <v>0.47263522532870339</v>
       </c>
       <c r="K78" s="8">
         <f ca="1"/>
-        <v>0.42300618593684225</v>
+        <v>0.44360647901591516</v>
       </c>
       <c r="L78" s="8">
         <f ca="1"/>
-        <v>4.1896776813082175E-2</v>
+        <v>3.5898902710000499E-2</v>
       </c>
       <c r="M78" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="79" spans="9:13" x14ac:dyDescent="0.3">
@@ -5176,19 +5207,19 @@
       </c>
       <c r="J79" s="8">
         <f ca="1"/>
-        <v>0.57740717064861236</v>
+        <v>0.47263522532870339</v>
       </c>
       <c r="K79" s="8">
         <f ca="1"/>
-        <v>0.42503777784094454</v>
+        <v>0.44398843620424133</v>
       </c>
       <c r="L79" s="8">
         <f ca="1"/>
-        <v>3.9546143845394649E-2</v>
+        <v>3.424166421112658E-2</v>
       </c>
       <c r="M79" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="80" spans="9:13" x14ac:dyDescent="0.3">
@@ -5197,19 +5228,19 @@
       </c>
       <c r="J80" s="8">
         <f ca="1"/>
-        <v>0.57740717064861236</v>
+        <v>0.47263522532870339</v>
       </c>
       <c r="K80" s="8">
         <f ca="1"/>
-        <v>0.42701660112416095</v>
+        <v>0.44436047242663695</v>
       </c>
       <c r="L80" s="8">
         <f ca="1"/>
-        <v>3.7327394087119381E-2</v>
+        <v>3.266093214074714E-2</v>
       </c>
       <c r="M80" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="81" spans="9:13" x14ac:dyDescent="0.3">
@@ -5218,19 +5249,19 @@
       </c>
       <c r="J81" s="8">
         <f ca="1"/>
-        <v>0.57740717064861236</v>
+        <v>0.47263522532870339</v>
       </c>
       <c r="K81" s="8">
         <f ca="1"/>
-        <v>0.4289446853488334</v>
+        <v>0.44472296925871468</v>
       </c>
       <c r="L81" s="8">
         <f ca="1"/>
-        <v>3.5233128235808417E-2</v>
+        <v>3.1153172930619505E-2</v>
       </c>
       <c r="M81" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="82" spans="9:13" x14ac:dyDescent="0.3">
@@ -5239,19 +5270,19 @@
       </c>
       <c r="J82" s="8">
         <f ca="1"/>
-        <v>0.57740717064861236</v>
+        <v>0.47263522532870339</v>
       </c>
       <c r="K82" s="8">
         <f ca="1"/>
-        <v>0.43082395731465339</v>
+        <v>0.4450762889558032</v>
       </c>
       <c r="L82" s="8">
         <f ca="1"/>
-        <v>3.3256359250222925E-2</v>
+        <v>2.971501784836449E-2</v>
       </c>
       <c r="M82" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="83" spans="9:13" x14ac:dyDescent="0.3">
@@ -5260,19 +5291,19 @@
       </c>
       <c r="J83" s="8">
         <f ca="1"/>
-        <v>0.57740717064861236</v>
+        <v>0.47263522532870339</v>
       </c>
       <c r="K83" s="8">
         <f ca="1"/>
-        <v>0.43265624748132792</v>
+        <v>0.44542077566046445</v>
       </c>
       <c r="L83" s="8">
         <f ca="1"/>
-        <v>3.139049942877143E-2</v>
+        <v>2.834325367167604E-2</v>
       </c>
       <c r="M83" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="84" spans="9:13" x14ac:dyDescent="0.3">
@@ -5281,19 +5312,19 @@
       </c>
       <c r="J84" s="8">
         <f ca="1"/>
-        <v>0.70384581205313657</v>
+        <v>0.91905236752737207</v>
       </c>
       <c r="K84" s="8">
         <f ca="1"/>
-        <v>0.43600426679702925</v>
+        <v>0.45126807926375961</v>
       </c>
       <c r="L84" s="8">
         <f ca="1"/>
-        <v>2.9257053444121207E-2</v>
+        <v>2.5854476680211631E-2</v>
       </c>
       <c r="M84" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="85" spans="9:13" x14ac:dyDescent="0.3">
@@ -5302,19 +5333,19 @@
       </c>
       <c r="J85" s="8">
         <f ca="1"/>
-        <v>0.70384581205313657</v>
+        <v>0.91905236752737207</v>
       </c>
       <c r="K85" s="8">
         <f ca="1"/>
-        <v>0.43927062710503062</v>
+        <v>0.45697276570599887</v>
       </c>
       <c r="L85" s="8">
         <f ca="1"/>
-        <v>2.7268606277527044E-2</v>
+        <v>2.3584238350689221E-2</v>
       </c>
       <c r="M85" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="86" spans="9:13" x14ac:dyDescent="0.3">
@@ -5323,19 +5354,19 @@
       </c>
       <c r="J86" s="8">
         <f ca="1"/>
-        <v>0.70384581205313657</v>
+        <v>0.91905236752737207</v>
       </c>
       <c r="K86" s="8">
         <f ca="1"/>
-        <v>0.44245827993573067</v>
+        <v>0.46253998982432859</v>
       </c>
       <c r="L86" s="8">
         <f ca="1"/>
-        <v>2.5415303041103999E-2</v>
+        <v>2.151334425937439E-2</v>
       </c>
       <c r="M86" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="87" spans="9:13" x14ac:dyDescent="0.3">
@@ -5344,19 +5375,19 @@
       </c>
       <c r="J87" s="8">
         <f ca="1"/>
-        <v>0.70384581205313657</v>
+        <v>0.91905236752737207</v>
       </c>
       <c r="K87" s="8">
         <f ca="1"/>
-        <v>0.44557003627046171</v>
+        <v>0.4679746609874601</v>
       </c>
       <c r="L87" s="8">
         <f ca="1"/>
-        <v>2.3687962218833052E-2</v>
+        <v>1.9624292390652033E-2</v>
       </c>
       <c r="M87" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="88" spans="9:13" x14ac:dyDescent="0.3">
@@ -5365,19 +5396,19 @@
       </c>
       <c r="J88" s="8">
         <f ca="1"/>
-        <v>0.70384581205313657</v>
+        <v>0.91905236752737207</v>
       </c>
       <c r="K88" s="8">
         <f ca="1"/>
-        <v>0.4486085748090814</v>
+        <v>0.47328145753498846</v>
       </c>
       <c r="L88" s="8">
         <f ca="1"/>
-        <v>2.2078017461257749E-2</v>
+        <v>1.7901112556672826E-2</v>
       </c>
       <c r="M88" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="89" spans="9:13" x14ac:dyDescent="0.3">
@@ -5386,19 +5417,19 @@
       </c>
       <c r="J89" s="8">
         <f ca="1"/>
-        <v>0.70384581205313657</v>
+        <v>0.91905236752737207</v>
       </c>
       <c r="K89" s="8">
         <f ca="1"/>
-        <v>0.45157644966075638</v>
+        <v>0.4784648402093184</v>
       </c>
       <c r="L89" s="8">
         <f ca="1"/>
-        <v>2.057749225669973E-2</v>
+        <v>1.6329243925291833E-2</v>
       </c>
       <c r="M89" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="90" spans="9:13" x14ac:dyDescent="0.3">
@@ -5407,19 +5438,19 @@
       </c>
       <c r="J90" s="8">
         <f ca="1"/>
-        <v>0.70384581205313657</v>
+        <v>0.91905236752737207</v>
       </c>
       <c r="K90" s="8">
         <f ca="1"/>
-        <v>0.45447609750434703</v>
+        <v>0.48352906466125017</v>
       </c>
       <c r="L90" s="8">
         <f ca="1"/>
-        <v>1.9178950010426618E-2</v>
+        <v>1.4895398341965682E-2</v>
       </c>
       <c r="M90" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="91" spans="9:13" x14ac:dyDescent="0.3">
@@ -5428,19 +5459,19 @@
       </c>
       <c r="J91" s="8">
         <f ca="1"/>
-        <v>0.70384581205313657</v>
+        <v>0.91905236752737207</v>
       </c>
       <c r="K91" s="8">
         <f ca="1"/>
-        <v>0.4573098442605833</v>
+        <v>0.48847819310291068</v>
       </c>
       <c r="L91" s="8">
         <f ca="1"/>
-        <v>1.7875456455457652E-2</v>
+        <v>1.3587456071638113E-2</v>
       </c>
       <c r="M91" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="92" spans="9:13" x14ac:dyDescent="0.3">
@@ -5449,19 +5480,19 @@
       </c>
       <c r="J92" s="8">
         <f ca="1"/>
-        <v>0.70384581205313657</v>
+        <v>0.91905236752737207</v>
       </c>
       <c r="K92" s="8">
         <f ca="1"/>
-        <v>0.46007991131443216</v>
+        <v>0.49331610517509561</v>
       </c>
       <c r="L92" s="8">
         <f ca="1"/>
-        <v>1.6660556295816403E-2</v>
+        <v>1.2394365749572481E-2</v>
       </c>
       <c r="M92" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="93" spans="9:13" x14ac:dyDescent="0.3">
@@ -5470,19 +5501,19 @@
       </c>
       <c r="J93" s="8">
         <f ca="1"/>
-        <v>0.70384581205313657</v>
+        <v>0.91905236752737207</v>
       </c>
       <c r="K93" s="8">
         <f ca="1"/>
-        <v>0.46278842132263992</v>
+        <v>0.49804650809012085</v>
       </c>
       <c r="L93" s="8">
         <f ca="1"/>
-        <v>1.5528226324692153E-2</v>
+        <v>1.1306036656360359E-2</v>
       </c>
       <c r="M93" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="94" spans="9:13" x14ac:dyDescent="0.3">
@@ -5491,19 +5522,19 @@
       </c>
       <c r="J94" s="8">
         <f ca="1"/>
-        <v>0.3680418096501068</v>
+        <v>0.76489947289387872</v>
       </c>
       <c r="K94" s="8">
         <f ca="1"/>
-        <v>0.4617472497657989</v>
+        <v>0.50097895825279948</v>
       </c>
       <c r="L94" s="8">
         <f ca="1"/>
-        <v>1.4967111415251802E-2</v>
+        <v>1.047348592771659E-2</v>
       </c>
       <c r="M94" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="95" spans="9:13" x14ac:dyDescent="0.3">
@@ -5512,19 +5543,19 @@
       </c>
       <c r="J95" s="8">
         <f ca="1"/>
-        <v>0.3680418096501068</v>
+        <v>0.76489947289387872</v>
       </c>
       <c r="K95" s="8">
         <f ca="1"/>
-        <v>0.46072871237323709</v>
+        <v>0.5038476594988982</v>
       </c>
       <c r="L95" s="8">
         <f ca="1"/>
-        <v>1.4426272409929665E-2</v>
+        <v>9.7022398016162574E-3</v>
       </c>
       <c r="M95" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="96" spans="9:13" x14ac:dyDescent="0.3">
@@ -5533,19 +5564,19 @@
       </c>
       <c r="J96" s="8">
         <f ca="1"/>
-        <v>0.3680418096501068</v>
+        <v>0.76489947289387872</v>
       </c>
       <c r="K96" s="8">
         <f ca="1"/>
-        <v>0.45973207901062274</v>
+        <v>0.50665466824508076</v>
       </c>
       <c r="L96" s="8">
         <f ca="1"/>
-        <v>1.3904976623039432E-2</v>
+        <v>8.987788202374768E-3</v>
       </c>
       <c r="M96" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="97" spans="9:13" x14ac:dyDescent="0.3">
@@ -5554,19 +5585,19 @@
       </c>
       <c r="J97" s="8">
         <f ca="1"/>
-        <v>0.3680418096501068</v>
+        <v>0.76489947289387872</v>
       </c>
       <c r="K97" s="8">
         <f ca="1"/>
-        <v>0.4587566506131705</v>
+        <v>0.50940195340091898</v>
       </c>
       <c r="L97" s="8">
         <f ca="1"/>
-        <v>1.3402520598368743E-2</v>
+        <v>8.3259470959000919E-3</v>
       </c>
       <c r="M97" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="98" spans="9:13" x14ac:dyDescent="0.3">
@@ -5575,19 +5606,19 @@
       </c>
       <c r="J98" s="8">
         <f ca="1"/>
-        <v>0.3680418096501068</v>
+        <v>0.76489947289387872</v>
       </c>
       <c r="K98" s="8">
         <f ca="1"/>
-        <v>0.45780175755040137</v>
+        <v>0.5120914009745291</v>
       </c>
       <c r="L98" s="8">
         <f ca="1"/>
-        <v>1.291821875019343E-2</v>
+        <v>7.7128423004067361E-3</v>
       </c>
       <c r="M98" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="99" spans="9:13" x14ac:dyDescent="0.3">
@@ -5596,19 +5627,19 @@
       </c>
       <c r="J99" s="8">
         <f ca="1"/>
-        <v>0.3680418096501068</v>
+        <v>0.76489947289387872</v>
       </c>
       <c r="K99" s="8">
         <f ca="1"/>
-        <v>0.45686675809310656</v>
+        <v>0.51472481839035567</v>
       </c>
       <c r="L99" s="8">
         <f ca="1"/>
-        <v>1.2451417242019468E-2</v>
+        <v>7.1448848926201529E-3</v>
       </c>
       <c r="M99" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="100" spans="9:13" x14ac:dyDescent="0.3">
@@ -5617,19 +5648,19 @@
       </c>
       <c r="J100" s="8">
         <f ca="1"/>
-        <v>0.3680418096501068</v>
+        <v>0.76489947289387872</v>
       </c>
       <c r="K100" s="8">
         <f ca="1"/>
-        <v>0.45595103697513756</v>
+        <v>0.51730393853987655</v>
       </c>
       <c r="L100" s="8">
         <f ca="1"/>
-        <v>1.2001483701937274E-2</v>
+        <v>6.6187542440837212E-3</v>
       </c>
       <c r="M100" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="101" spans="9:13" x14ac:dyDescent="0.3">
@@ -5638,19 +5669,19 @@
       </c>
       <c r="J101" s="8">
         <f ca="1"/>
-        <v>0.3680418096501068</v>
+        <v>0.76489947289387872</v>
       </c>
       <c r="K101" s="8">
         <f ca="1"/>
-        <v>0.45505400404324947</v>
+        <v>0.5198304235843052</v>
       </c>
       <c r="L101" s="8">
         <f ca="1"/>
-        <v>1.1567808609953241E-2</v>
+        <v>6.1313642862995121E-3</v>
       </c>
       <c r="M101" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="102" spans="9:13" x14ac:dyDescent="0.3">
@@ -5659,19 +5690,19 @@
       </c>
       <c r="J102" s="8">
         <f ca="1"/>
-        <v>0.3680418096501068</v>
+        <v>0.76489947289387872</v>
       </c>
       <c r="K102" s="8">
         <f ca="1"/>
-        <v>0.45417509298877334</v>
+        <v>0.52230586852682603</v>
       </c>
       <c r="L102" s="8">
         <f ca="1"/>
-        <v>1.1149804472459725E-2</v>
+        <v>5.6798648147911067E-3</v>
       </c>
       <c r="M102" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
     <row r="103" spans="9:13" x14ac:dyDescent="0.3">
@@ -5680,19 +5711,19 @@
       </c>
       <c r="J103" s="8">
         <f ca="1"/>
-        <v>0.3680418096501068</v>
+        <v>0.76489947289387872</v>
       </c>
       <c r="K103" s="8">
         <f ca="1"/>
-        <v>0.4533137601553866</v>
+        <v>0.52473180457049662</v>
       </c>
       <c r="L103" s="8">
         <f ca="1"/>
-        <v>1.0746905026538231E-2</v>
+        <v>5.2616130130143822E-3</v>
       </c>
       <c r="M103" s="22">
         <f ca="1"/>
-        <v>0.45158686362248934</v>
+        <v>0.32283416468956183</v>
       </c>
     </row>
   </sheetData>
@@ -5897,7 +5928,7 @@
       </c>
       <c r="C8" s="11" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xll.\TMX.BOND.BASIC(dated, maturity, coupon, _xll.ENUM(frequency), _xll.ENUM(day_count))</f>
-        <v>2369229520592</v>
+        <v>1520972156752</v>
       </c>
       <c r="F8" s="17">
         <f ca="1"/>
@@ -5942,7 +5973,7 @@
       </c>
       <c r="C10" s="11" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">_xll.\TMX.BOND.BASIC.INSTRUMENT(bond_basic,pvdate)</f>
-        <v>2369228324208</v>
+        <v>1521044381200</v>
       </c>
       <c r="F10" s="17">
         <f ca="1"/>
@@ -6005,19 +6036,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EAD57E-B813-416C-A1C4-B7528B2439C2}">
-  <dimension ref="B2:L25"/>
+  <dimension ref="B2:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="23"/>
-    <col min="3" max="3" width="10.7109375" style="23" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="23" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="23"/>
+    <col min="3" max="3" width="19.140625" style="23" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="23"/>
-    <col min="7" max="7" width="9.140625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="23" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" style="23" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="23"/>
     <col min="10" max="11" width="13" style="23" bestFit="1" customWidth="1"/>
@@ -6026,53 +6059,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="29">
+      <c r="B2" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="31">
         <f ca="1">TODAY()</f>
         <v>45412</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.01</v>
+        <v>22</v>
+      </c>
+      <c r="G2" s="36">
+        <f ca="1">TODAY()</f>
+        <v>45412</v>
       </c>
       <c r="K2" s="25" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">_xll.\TMX.BOND.BASIC(J3,J4,J5,_xll.ENUM(J6),_xll.ENUM(J7),J8)</f>
-        <v>2369229518016</v>
+        <v>1520972158096</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="25" cm="1">
-        <f t="array" aca="1" ref="C3" ca="1">_xll.\TMX.BOND.BASIC(pvdate,10)</f>
-        <v>2369229539856</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="B3" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3">
         <v>10</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="23" t="e" cm="1">
-        <f t="array" aca="1" ref="G3" ca="1">_xll.TMX.VALUE.PRESENT(C4, G2, H3)</f>
-        <v>#VALUE!</v>
+        <v>32</v>
+      </c>
+      <c r="G3" s="24" cm="1">
+        <f t="array" aca="1" ref="G3" ca="1">_xll.\TMX.CURVE.CONSTANT(H3+0*RAND())</f>
+        <v>1520986619520</v>
       </c>
       <c r="H3" s="3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="31" cm="1">
+        <v>0.05</v>
+      </c>
+      <c r="J3" s="33" cm="1">
         <f t="array" aca="1" ref="J3:J8" ca="1">_xll.TMX.BOND.BASIC(bond)</f>
         <v>45412</v>
       </c>
-      <c r="K3" s="31" cm="1">
+      <c r="K3" s="33" cm="1">
         <f t="array" aca="1" ref="K3:K8" ca="1">_xll.TMX.BOND.BASIC(K2)</f>
         <v>45412</v>
       </c>
@@ -6082,25 +6109,27 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="25" cm="1">
-        <f t="array" aca="1" ref="C4" ca="1">_xll.\TMX.BOND.BASIC.INSTRUMENT(bond,pvdate)</f>
-        <v>2369228326144</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="23" t="e" cm="1">
-        <f t="array" aca="1" ref="G4" ca="1">_xll.TMX.VALUE.YIELD(C4, G3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J4" s="31">
+      <c r="B4" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="39" cm="1">
+        <f t="array" aca="1" ref="G4" ca="1">_xll.TMX.VALUE.PRESENT(instrument, curve, H4)</f>
+        <v>99.511699960922385</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="33">
         <f ca="1"/>
         <v>49064</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="33">
         <f ca="1"/>
         <v>49064</v>
       </c>
@@ -6110,24 +6139,24 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>33</v>
+      <c r="B5" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>30</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="23" t="e" cm="1">
-        <f t="array" aca="1" ref="G5" ca="1">_xll.TMX.VALUE.DURATION(C4, G2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J5" s="23">
+        <v>35</v>
+      </c>
+      <c r="G5" s="23" cm="1">
+        <f t="array" aca="1" ref="G5" ca="1">_xll.TMX.VALUE.YIELD(instrument, present)</f>
+        <v>4.9999999999861489E-2</v>
+      </c>
+      <c r="J5" s="34">
         <f ca="1"/>
         <v>0.05</v>
       </c>
-      <c r="K5" s="23">
+      <c r="K5" s="34">
         <f ca="1"/>
         <v>0.05</v>
       </c>
@@ -6137,25 +6166,27 @@
       </c>
     </row>
     <row r="6" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="30" cm="1">
-        <f t="array" aca="1" ref="C6:C25" ca="1">_xll.TMX.INSTRUMENT.TIME(C4)</f>
-        <v>0.50377488928588543</v>
-      </c>
-      <c r="D6" s="30" t="s">
+      <c r="B6" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="23" t="e" cm="1">
-        <f t="array" aca="1" ref="G6" ca="1">_xll.TMX.VALUE.CONVEXITY(C4,G2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J6" s="23" t="str">
+      <c r="F6" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="41" cm="1">
+        <f t="array" aca="1" ref="G6" ca="1">_xll.TMX.VALUE.OAS(instrument, curve, H6)</f>
+        <v>1.2681947238615968E-2</v>
+      </c>
+      <c r="H6" s="23">
+        <v>90</v>
+      </c>
+      <c r="J6" s="34" t="str">
         <f ca="1"/>
         <v>TMX_FREQUENCY_SEMIANNUALLY</v>
       </c>
-      <c r="K6" s="23" t="str">
+      <c r="K6" s="34" t="str">
         <f ca="1"/>
         <v>TMX_FREQUENCY_SEMIANNUALLY</v>
       </c>
@@ -6165,15 +6196,24 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="38" t="s">
+        <v>26</v>
+      </c>
       <c r="C7" s="23">
-        <f ca="1"/>
-        <v>0.99933605755080523</v>
-      </c>
-      <c r="J7" s="23" t="str">
+        <v>100</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="40" cm="1">
+        <f t="array" aca="1" ref="G7" ca="1">_xll.TMX.VALUE.DURATION(instrument, curve)</f>
+        <v>-794.44420411936369</v>
+      </c>
+      <c r="J7" s="34" t="str">
         <f ca="1"/>
         <v>TMX_DAY_COUNT_30_360</v>
       </c>
-      <c r="K7" s="23" t="str">
+      <c r="K7" s="34" t="str">
         <f ca="1"/>
         <v>TMX_DAY_COUNT_30_360</v>
       </c>
@@ -6183,15 +6223,26 @@
       </c>
     </row>
     <row r="8" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="23">
-        <f ca="1"/>
-        <v>1.5031109468366908</v>
-      </c>
-      <c r="J8" s="23">
+      <c r="B8" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="25" cm="1">
+        <f t="array" aca="1" ref="C8" ca="1">_xll.\TMX.BOND.BASIC(dated,maturity,coupon,_xll.ENUM(frequency),_xll.ENUM(day_count))</f>
+        <v>1520972156528</v>
+      </c>
+      <c r="D8"/>
+      <c r="F8" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="40" cm="1">
+        <f t="array" aca="1" ref="G8" ca="1">_xll.TMX.VALUE.CONVEXITY(instrument,curve)</f>
+        <v>7292.3297608333796</v>
+      </c>
+      <c r="J8" s="34">
         <f ca="1"/>
         <v>100</v>
       </c>
-      <c r="K8" s="23">
+      <c r="K8" s="34">
         <f ca="1"/>
         <v>100</v>
       </c>
@@ -6201,109 +6252,323 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="23">
-        <f ca="1"/>
-        <v>1.9986721151016105</v>
+      <c r="B9" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="25" cm="1">
+        <f t="array" aca="1" ref="C9" ca="1">_xll.\TMX.BOND.BASIC.INSTRUMENT(bond,pvdate)</f>
+        <v>1521044373984</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C10" s="23">
-        <f ca="1"/>
-        <v>2.5024470043874958</v>
+      <c r="C10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C11" s="23">
-        <f ca="1"/>
-        <v>2.9980081726524159</v>
+      <c r="C11" s="30" cm="1">
+        <f t="array" aca="1" ref="C11:D30" ca="1">_xll.TMX.INSTRUMENT(C9)</f>
+        <v>0.50377488928588543</v>
+      </c>
+      <c r="D11" s="30">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E11" s="29" cm="1">
+        <f t="array" aca="1" ref="E11:E30" ca="1">_xlfn.MAP(_xlfn.TAKE(_xlfn.ANCHORARRAY(C11),,1),_xlfn.LAMBDA(_xlpm.u,_xll.TMX.DATE.ADDYEARS(pvdate,_xlpm.u)))</f>
+        <v>45596</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C12" s="23">
         <f ca="1"/>
-        <v>3.5017830619383012</v>
+        <v>0.99933605755080523</v>
+      </c>
+      <c r="D12" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E12" s="29">
+        <f ca="1"/>
+        <v>45777</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C13" s="23">
         <f ca="1"/>
-        <v>4.0000821372102093</v>
-      </c>
+        <v>1.5031109468366908</v>
+      </c>
+      <c r="D13" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E13" s="29">
+        <f ca="1"/>
+        <v>45961</v>
+      </c>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C14" s="23">
         <f ca="1"/>
-        <v>4.5038570264960951</v>
+        <v>1.9986721151016105</v>
+      </c>
+      <c r="D14" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E14" s="29">
+        <f ca="1"/>
+        <v>46142</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C15" s="23">
         <f ca="1"/>
-        <v>4.9994181947610148</v>
+        <v>2.5024470043874958</v>
+      </c>
+      <c r="D15" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E15" s="29">
+        <f ca="1"/>
+        <v>46326</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C16" s="23">
         <f ca="1"/>
+        <v>2.9980081726524159</v>
+      </c>
+      <c r="D16" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E16" s="29">
+        <f ca="1"/>
+        <v>46507</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="23">
+        <f ca="1"/>
+        <v>3.5017830619383012</v>
+      </c>
+      <c r="D17" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E17" s="29">
+        <f ca="1"/>
+        <v>46691</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="23">
+        <f ca="1"/>
+        <v>4.0000821372102093</v>
+      </c>
+      <c r="D18" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E18" s="29">
+        <f ca="1"/>
+        <v>46873</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="23">
+        <f ca="1"/>
+        <v>4.5038570264960951</v>
+      </c>
+      <c r="D19" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E19" s="29">
+        <f ca="1"/>
+        <v>47057</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="23">
+        <f ca="1"/>
+        <v>4.9994181947610148</v>
+      </c>
+      <c r="D20" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E20" s="29">
+        <f ca="1"/>
+        <v>47238</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="23">
+        <f ca="1"/>
         <v>5.5031930840469006</v>
       </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" s="23">
+      <c r="D21" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E21" s="29">
+        <f ca="1"/>
+        <v>47422</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C22" s="23">
         <f ca="1"/>
         <v>5.9987542523118202</v>
       </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" s="23">
+      <c r="D22" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E22" s="29">
+        <f ca="1"/>
+        <v>47603</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C23" s="23">
         <f ca="1"/>
         <v>6.502529141597706</v>
       </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19" s="23">
+      <c r="D23" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E23" s="29">
+        <f ca="1"/>
+        <v>47787</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C24" s="23">
         <f ca="1"/>
         <v>6.9980903098626257</v>
       </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C20" s="23">
+      <c r="D24" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E24" s="29">
+        <f ca="1"/>
+        <v>47968</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="23">
         <f ca="1"/>
         <v>7.5018651991485106</v>
       </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C21" s="23">
+      <c r="D25" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E25" s="29">
+        <f ca="1"/>
+        <v>48152</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="23">
         <f ca="1"/>
         <v>8.0001642744204187</v>
       </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C22" s="23">
+      <c r="D26" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E26" s="29">
+        <f ca="1"/>
+        <v>48334</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C27" s="23">
         <f ca="1"/>
         <v>8.5039391637063044</v>
       </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C23" s="23">
+      <c r="D27" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E27" s="29">
+        <f ca="1"/>
+        <v>48518</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="23">
         <f ca="1"/>
         <v>8.999500331971225</v>
       </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C24" s="23">
+      <c r="D28" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E28" s="29">
+        <f ca="1"/>
+        <v>48699</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="23">
         <f ca="1"/>
         <v>9.5032752212571108</v>
       </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C25" s="23">
+      <c r="D29" s="23">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E29" s="29">
+        <f ca="1"/>
+        <v>48883</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C30" s="23">
         <f ca="1"/>
         <v>9.9988363895220296</v>
+      </c>
+      <c r="D30" s="23">
+        <f ca="1"/>
+        <v>102.5</v>
+      </c>
+      <c r="E30" s="29">
+        <f ca="1"/>
+        <v>49064</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7007CDED-52BA-4236-9AB4-270D2D758A2D}">
+          <x14:formula1>
+            <xm:f>_xlfn.ANCHORARRAY(ENUM!$G$3)</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4F940A22-B041-4372-AF7C-03B1471C3CC9}">
+          <x14:formula1>
+            <xm:f>_xlfn.ANCHORARRAY(ENUM!$B$3)</xm:f>
+          </x14:formula1>
+          <xm:sqref>C6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>